<commit_message>
added 2015_TM152_NGF_04 to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,30 +5,40 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D093A96B-B646-479D-BA46-242E085FAA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E58E2B0-D4B0-42DB-AB93-A3B14578875E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="2660" windowWidth="22080" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$8</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>No Project</t>
   </si>
@@ -115,6 +125,12 @@
   </si>
   <si>
     <t>https://app.asana.com/0/search?q=2035_TM152_NGF_NoProject_01&amp;child=1201295328698176</t>
+  </si>
+  <si>
+    <t>2015_TM152_NGF_04</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/13098083395690/1202541200237173</t>
   </si>
 </sst>
 </file>
@@ -583,11 +599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -709,86 +725,113 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="16">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="13">
         <v>2015</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="17" t="s">
+      <c r="D5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="H5" s="14"/>
       <c r="I5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2035</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2015</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="16">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
         <v>2035</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="17" t="s">
+      <c r="D8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I8" s="18" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added sensitivity tests to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natchison\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E58E2B0-D4B0-42DB-AB93-A3B14578875E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D69418F-2537-4948-9A37-7851B578E006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="2660" windowWidth="22080" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="795" yWindow="870" windowWidth="25365" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
   <si>
     <t>No Project</t>
   </si>
@@ -131,18 +131,77 @@
   </si>
   <si>
     <t>https://app.asana.com/0/13098083395690/1202541200237173</t>
+  </si>
+  <si>
+    <t>"Final Blueprint runs\Final Blueprint (s24)\BAUS v2.25 - FINAL VERSION"</t>
+  </si>
+  <si>
+    <t>run182</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202512897941570/f</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_SensDiscount_01</t>
+  </si>
+  <si>
+    <t>Sensitivity Test</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_SensDiscount_02</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_SensDiscount_03</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_SensDiscount_04</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_SensDiscount_05</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202512897941573/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202554938897468/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202554938897469/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202554938897470/f</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_Blueprint_00</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202521542566668/f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -171,6 +230,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -198,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -215,45 +280,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{564E6A42-6173-40A4-9CC8-4130B69477E9}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{CC352229-7B38-4835-9297-CE7CE23BF08B}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{A24BC63F-329C-495C-A760-474376839248}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -599,23 +702,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.296875" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.8984375" customWidth="1"/>
+    <col min="6" max="6" width="70.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -644,7 +747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -670,7 +773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -697,7 +800,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -724,7 +827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -751,7 +854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -780,7 +883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -806,7 +909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
@@ -835,8 +938,182 @@
         <v>28</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
correct urbansim_path for  2035_TM152_NGF_NoProject_01 in the model log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natchison\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D69418F-2537-4948-9A37-7851B578E006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42229171-B69D-43AF-B8CE-98664B35B371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="870" windowWidth="25365" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -706,19 +706,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.85546875" customWidth="1"/>
+    <col min="6" max="6" width="70.8984375" customWidth="1"/>
     <col min="7" max="7" width="15" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -747,7 +747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -773,7 +773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -800,7 +800,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -827,7 +827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -854,7 +854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -883,7 +883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -909,7 +909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
@@ -926,10 +926,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>9</v>
@@ -938,7 +938,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>26</v>
       </c>
@@ -967,7 +967,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>26</v>
       </c>
@@ -996,7 +996,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>26</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>26</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
adding a network number column
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42229171-B69D-43AF-B8CE-98664B35B371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A6532E-1D83-4311-B9C4-C962A0B746F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
   <si>
     <t>No Project</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>https://app.asana.com/0/0/1202521542566668/f</t>
+  </si>
+  <si>
+    <t>network number</t>
+  </si>
+  <si>
+    <t>NGF_Networks_Blueprint_01</t>
   </si>
 </sst>
 </file>
@@ -296,7 +302,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -351,6 +357,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,11 +709,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -716,9 +723,10 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="70.8984375" customWidth="1"/>
     <col min="7" max="7" width="15" style="5" customWidth="1"/>
+    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -743,11 +751,14 @@
       <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -772,8 +783,9 @@
       <c r="H2" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -796,11 +808,12 @@
         <v>18</v>
       </c>
       <c r="H3" s="14"/>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -823,11 +836,12 @@
         <v>18</v>
       </c>
       <c r="H4" s="14"/>
-      <c r="I4" t="s">
+      <c r="I4" s="14"/>
+      <c r="J4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -850,11 +864,12 @@
         <v>18</v>
       </c>
       <c r="H5" s="14"/>
-      <c r="I5" t="s">
+      <c r="I5" s="14"/>
+      <c r="J5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -879,11 +894,12 @@
       <c r="H6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -908,8 +924,9 @@
       <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
@@ -934,11 +951,12 @@
       <c r="H8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="14"/>
+      <c r="J8" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>26</v>
       </c>
@@ -963,11 +981,12 @@
       <c r="H9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="28"/>
+      <c r="J9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>26</v>
       </c>
@@ -992,11 +1011,12 @@
       <c r="H10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="28"/>
+      <c r="J10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
@@ -1021,11 +1041,12 @@
       <c r="H11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="28"/>
+      <c r="J11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>26</v>
       </c>
@@ -1050,11 +1071,12 @@
       <c r="H12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="28"/>
+      <c r="J12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>26</v>
       </c>
@@ -1079,11 +1101,12 @@
       <c r="H13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="28"/>
+      <c r="J13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>26</v>
       </c>
@@ -1108,7 +1131,10 @@
       <c r="H14" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating the model run log to reflect the updated naming convention
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A6532E-1D83-4311-B9C4-C962A0B746F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E284001-6480-47D8-8952-DE2FCCC05723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2170" yWindow="5450" windowWidth="19190" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t>No Project</t>
   </si>
@@ -172,9 +172,6 @@
     <t>https://app.asana.com/0/0/1202554938897470/f</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_Blueprint_00</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/0/1202521542566668/f</t>
   </si>
   <si>
@@ -182,13 +179,19 @@
   </si>
   <si>
     <t>NGF_Networks_Blueprint_01</t>
+  </si>
+  <si>
+    <t>Blueprint</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -239,6 +242,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -296,13 +306,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -358,8 +369,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{564E6A42-6173-40A4-9CC8-4130B69477E9}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{CC352229-7B38-4835-9297-CE7CE23BF08B}"/>
@@ -711,9 +724,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -752,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>19</v>
@@ -1114,13 +1127,13 @@
         <v>2035</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>31</v>
@@ -1132,15 +1145,18 @@
         <v>9</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J14" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set up cross-run union comparison for NextGenFwys
1. update ModelRuns.xlsx and ModelRuns.csv
2. update `summarizeAcrossScenariosUnion.bat`
3. add a Readme to the NextGenFwys folder under TM1
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E284001-6480-47D8-8952-DE2FCCC05723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6426C33-2C3F-4385-AB7A-90B1B3098FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2170" yWindow="5450" windowWidth="19190" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7040" yWindow="1460" windowWidth="19430" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
   <si>
     <t>No Project</t>
   </si>
@@ -121,9 +119,6 @@
     <t>NGF</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_NoProject_01</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/search?q=2035_TM152_NGF_NoProject_01&amp;child=1201295328698176</t>
   </si>
   <si>
@@ -142,24 +137,9 @@
     <t>https://app.asana.com/0/0/1202512897941570/f</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_SensDiscount_01</t>
-  </si>
-  <si>
     <t>Sensitivity Test</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_SensDiscount_02</t>
-  </si>
-  <si>
-    <t>2035_TM152_NGF_SensDiscount_03</t>
-  </si>
-  <si>
-    <t>2035_TM152_NGF_SensDiscount_04</t>
-  </si>
-  <si>
-    <t>2035_TM152_NGF_SensDiscount_05</t>
-  </si>
-  <si>
     <t>https://app.asana.com/0/0/1202512897941573/f</t>
   </si>
   <si>
@@ -185,6 +165,39 @@
   </si>
   <si>
     <t>2035_TM152_NGF_NP02_Blueprint_00</t>
+  </si>
+  <si>
+    <t>NextGenFwys</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_BlueprintSegmentedTest</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_SensDiscount_01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_SensDiscount_02</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_SensDiscount_03</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_SensDiscount_04</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_SensDiscount_05</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_SensExtent_01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_TollLevel_01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_Blueprint_00_TollLevel_02</t>
   </si>
 </sst>
 </file>
@@ -722,16 +735,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.3984375" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="70.8984375" customWidth="1"/>
@@ -765,7 +778,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>19</v>
@@ -800,7 +813,7 @@
     </row>
     <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B3" s="13">
         <v>2015</v>
@@ -828,7 +841,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B4" s="13">
         <v>2015</v>
@@ -856,7 +869,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B5" s="13">
         <v>2015</v>
@@ -884,13 +897,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B6" s="13">
         <v>2015</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>26</v>
@@ -909,7 +922,7 @@
       </c>
       <c r="I6" s="14"/>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -941,13 +954,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B8" s="16">
         <v>2035</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>26</v>
@@ -956,205 +969,314 @@
         <v>0</v>
       </c>
       <c r="F8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>32</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B9" s="24">
         <v>2035</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>31</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>32</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B10" s="20">
         <v>2035</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="H10" s="28" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="28"/>
       <c r="J10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B11" s="20">
         <v>2035</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="28"/>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B12" s="20">
         <v>2035</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>9</v>
       </c>
       <c r="I12" s="28"/>
       <c r="J12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B13" s="22">
         <v>2035</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="22" t="s">
         <v>31</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>32</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="28"/>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="16">
+      <c r="A14" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="22">
         <v>2035</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" s="31" t="s">
-        <v>44</v>
-      </c>
+      <c r="H14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="28"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="28"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J14" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="J17" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
Update network and asana task information
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natchison\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6426C33-2C3F-4385-AB7A-90B1B3098FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3103EB4-1420-4A20-B58F-82A3E828052A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="1460" windowWidth="19430" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="1215" windowWidth="26430" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
   <si>
     <t>No Project</t>
   </si>
@@ -198,6 +198,33 @@
   </si>
   <si>
     <t>2035_TM152_NGF_NP02_Blueprint_00_TollLevel_02</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202626450708380/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202662876083700/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202677696411529/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1202503525669953/f</t>
+  </si>
+  <si>
+    <t>NGF_Networks_01</t>
+  </si>
+  <si>
+    <t>NGF_Networks_02</t>
+  </si>
+  <si>
+    <t>TM1_2015_Base_Network</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_64</t>
+  </si>
+  <si>
+    <t>existing_conditions\net_2035_NextGenFwy</t>
   </si>
 </sst>
 </file>
@@ -326,18 +353,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -348,23 +374,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,11 +403,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
@@ -739,193 +765,201 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="50.3984375" customWidth="1"/>
-    <col min="4" max="4" width="15.296875" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.8984375" customWidth="1"/>
+    <col min="6" max="6" width="70.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" style="5" customWidth="1"/>
-    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>2015</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="30"/>
-    </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>2015</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="6" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>2015</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="J4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>2015</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="J5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>2015</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="D6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="14"/>
+      <c r="I6" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="J6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -950,335 +984,369 @@
       <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="16">
+      <c r="I7" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="15">
         <v>2035</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="18" t="s">
+      <c r="I8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="24">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="23">
         <v>2035</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="D9" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="28"/>
+      <c r="I9" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="J9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="20">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="19">
         <v>2035</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="29" t="s">
+      <c r="D10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="28"/>
+      <c r="I10" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="J10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="20">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="19">
         <v>2035</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="29" t="s">
+      <c r="D11" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="28"/>
+      <c r="I11" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="J11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="20">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="19">
         <v>2035</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="29" t="s">
+      <c r="D12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="28"/>
+      <c r="I12" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="J12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="22">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="21">
         <v>2035</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="19" t="s">
+      <c r="D13" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="28"/>
+      <c r="I13" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="J13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="22">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="21">
         <v>2035</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="19" t="s">
+      <c r="D14" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="21" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="28"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="22">
+      <c r="I14" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="21">
         <v>2035</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="19" t="s">
+      <c r="D15" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="21" t="s">
         <v>31</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="28"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="22">
+      <c r="I15" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="21">
         <v>2035</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="D16" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="21" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="16">
+      <c r="I16" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="15">
         <v>2035</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="17" t="s">
+      <c r="D17" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="16">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="15">
         <v>2035</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="17" t="s">
+      <c r="D18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="18"/>
+      <c r="I18" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J17" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="J8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 2035_TM152_NGF_NP02_BPALTsegmented_00 and 2035_TM152_NGF_NP02
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natchison\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3103EB4-1420-4A20-B58F-82A3E828052A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA862C2-E192-4108-91AC-F0450F240AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1215" windowWidth="26430" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11805" yWindow="2820" windowWidth="16575" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
   <si>
     <t>No Project</t>
   </si>
@@ -173,9 +173,6 @@
     <t>2035_TM152_NGF_NP01</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_NP02_Blueprint_00_BlueprintSegmentedTest</t>
-  </si>
-  <si>
     <t>2035_TM152_NGF_NP02_Blueprint_00_SensDiscount_01</t>
   </si>
   <si>
@@ -225,6 +222,15 @@
   </si>
   <si>
     <t>existing_conditions\net_2035_NextGenFwy</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NoProject_03</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_00</t>
   </si>
 </sst>
 </file>
@@ -761,11 +767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -861,7 +867,7 @@
       </c>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
@@ -891,7 +897,7 @@
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
@@ -921,7 +927,7 @@
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
@@ -953,7 +959,7 @@
         <v>9</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
         <v>29</v>
@@ -985,7 +991,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1010,78 +1016,76 @@
       <c r="G8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>9</v>
-      </c>
+      <c r="H8" s="16"/>
       <c r="I8" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="23">
+      <c r="A9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="15">
         <v>2035</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="26" t="s">
+      <c r="C9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="25" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>40</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1092,7 +1096,7 @@
         <v>2035</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>26</v>
@@ -1113,7 +1117,7 @@
         <v>40</v>
       </c>
       <c r="J11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1124,7 +1128,7 @@
         <v>2035</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>26</v>
@@ -1145,39 +1149,39 @@
         <v>40</v>
       </c>
       <c r="J12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="21">
+      <c r="A13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="19">
         <v>2035</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="C13" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="27" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="27" t="s">
         <v>40</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1188,7 +1192,7 @@
         <v>2035</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>26</v>
@@ -1206,10 +1210,10 @@
         <v>9</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="J14" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1220,7 +1224,7 @@
         <v>2035</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>26</v>
@@ -1238,10 +1242,10 @@
         <v>9</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="J15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1252,7 +1256,7 @@
         <v>2035</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>26</v>
@@ -1273,39 +1277,39 @@
         <v>40</v>
       </c>
       <c r="J16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="15">
+      <c r="A17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="21">
         <v>2035</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="16" t="s">
+      <c r="C17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="J17" s="30" t="s">
-        <v>38</v>
+      <c r="J17" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1315,8 +1319,8 @@
       <c r="B18" s="15">
         <v>2035</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>45</v>
+      <c r="C18" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>26</v>
@@ -1334,16 +1338,48 @@
         <v>9</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>57</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J17" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="J18" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="J8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Model Run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natchison\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA862C2-E192-4108-91AC-F0450F240AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD569AD-16DD-41C8-832B-6D7FD057EFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11805" yWindow="2820" windowWidth="16575" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="69">
   <si>
     <t>No Project</t>
   </si>
@@ -231,6 +231,18 @@
   </si>
   <si>
     <t>2035_TM152_NGF_NP02_BPALTsegmented_00</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_02</t>
+  </si>
+  <si>
+    <t>NGF_Networks_03</t>
+  </si>
+  <si>
+    <t>NGF_Networks_XX</t>
   </si>
 </sst>
 </file>
@@ -359,7 +371,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,6 +427,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -767,11 +789,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1242,7 +1264,7 @@
         <v>9</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="J15" t="s">
         <v>53</v>
@@ -1345,34 +1367,98 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="15">
+      <c r="A19" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="32">
         <v>2035</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="D19" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="33" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>57</v>
       </c>
       <c r="J19" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="35">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="17" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding 2035_TM152_NGF_NP02_BPALTsegmented_03 to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B6FFB8-608E-401C-BF79-DF0ACCD2CA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CF152C-EE0F-4A67-AA57-7517B7C6BD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="77">
   <si>
     <t>No Project</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>NGF_Networks_05</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1201809392759895/1203154340231009</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -453,11 +456,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1506,28 +1505,28 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="36" t="s">
+      <c r="A23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="12">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="36" t="s">
+      <c r="D23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="36"/>
+      <c r="F23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="13"/>
       <c r="I23" s="13" t="s">
         <v>67</v>
       </c>
@@ -1563,15 +1562,18 @@
       <c r="I24" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="17"/>
+      <c r="J24" s="34" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J19" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="J8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
+    <hyperlink ref="J24" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn01 to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CF152C-EE0F-4A67-AA57-7517B7C6BD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDBAAD9-FE4B-4581-BF08-AACEF57B2994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="79">
   <si>
     <t>No Project</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1201809392759895/1203154340231009</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn01</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -335,7 +341,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +363,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,7 +407,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -425,7 +437,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -451,12 +462,31 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -809,11 +839,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -883,7 +913,7 @@
       <c r="H2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="29"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -1032,7 +1062,7 @@
       <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1062,7 +1092,7 @@
       <c r="I8" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="29" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1094,484 +1124,516 @@
       <c r="I9" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="29" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C10" s="25" t="s">
+    <row r="10" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="31">
+        <v>2035</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="31">
+        <v>2035</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="37">
+        <v>2035</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="38"/>
+      <c r="I12" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="31">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="26" t="s">
+      <c r="D16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="25" t="s">
+      <c r="F16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I16" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C11" s="27" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="28" t="s">
+      <c r="D17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="27" t="s">
+      <c r="F17" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I17" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C12" s="27" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="28" t="s">
+      <c r="D18" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="27" t="s">
+      <c r="F18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I18" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C13" s="27" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="28" t="s">
+      <c r="D19" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="27" t="s">
+      <c r="F19" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I19" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C14" s="3" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="41">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="18" t="s">
+      <c r="D20" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="F20" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I20" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C15" s="3" t="s">
+    <row r="21" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="41">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="D21" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="27" t="s">
+      <c r="F21" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J21" s="44" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="3" t="s">
+    <row r="22" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="41">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="D22" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="27" t="s">
+      <c r="F22" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J22" s="44" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="3" t="s">
+    <row r="23" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="41">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="18" t="s">
+      <c r="D23" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="F23" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I23" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J23" s="44" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="3" t="s">
+    <row r="24" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="41">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="18" t="s">
+      <c r="D24" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="F24" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I24" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J24" s="44" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="12">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="12">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="13" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="34" t="s">
-        <v>76</v>
+      <c r="J25" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J19" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="J10" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="J8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="J24" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="J15" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>

</xml_diff>

<commit_message>
added various sensitivity tests to model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDBAAD9-FE4B-4581-BF08-AACEF57B2994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91FBA4A-C1E8-4087-BAB5-E58E8D07366F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="81">
   <si>
     <t>No Project</t>
   </si>
@@ -242,9 +242,6 @@
     <t>NGF_Networks_03</t>
   </si>
   <si>
-    <t>NGF_Networks_XX</t>
-  </si>
-  <si>
     <t>2035_TM152_NGF_NP02_Blueprint_01</t>
   </si>
   <si>
@@ -254,12 +251,6 @@
     <t>NGF_Networks_Blueprint_02</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_NP02_Blueprint_00_SensExtent_02</t>
-  </si>
-  <si>
-    <t>NGF_Networks_04</t>
-  </si>
-  <si>
     <t>2035_TM152_NGF_NP02_BPALTsegmented_03</t>
   </si>
   <si>
@@ -273,6 +264,21 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>an old version of NGF_Networks_02</t>
+  </si>
+  <si>
+    <t>NGF_Networks_06</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensExtent01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn02</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn03</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -478,15 +484,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -839,21 +836,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="50.3984375" customWidth="1"/>
+    <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="70.8984375" customWidth="1"/>
     <col min="7" max="7" width="15" style="5" customWidth="1"/>
-    <col min="9" max="9" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1166,7 +1163,7 @@
         <v>2035</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>26</v>
@@ -1184,10 +1181,10 @@
         <v>9</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -1288,7 +1285,7 @@
         <v>2035</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D15" s="32" t="s">
         <v>26</v>
@@ -1306,10 +1303,10 @@
         <v>9</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1441,28 +1438,28 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="41">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="42" t="s">
+      <c r="A20" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="43" t="s">
+      <c r="D20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="42" t="s">
+      <c r="F20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="26" t="s">
         <v>9</v>
       </c>
       <c r="I20" s="26" t="s">
@@ -1472,159 +1469,223 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="41">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="42" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="43" t="s">
+      <c r="D21" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="J21" s="44" t="s">
+      <c r="F21" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="41">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="42" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="43" t="s">
+      <c r="J25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="J22" s="44" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="41">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="43" t="s">
+      <c r="F26" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="J26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" s="44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="41">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="J24" s="44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I25" s="42" t="s">
+      <c r="F27" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J25" t="s">
+      <c r="I27" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1634,8 +1695,9 @@
     <hyperlink ref="J10" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="J8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
     <hyperlink ref="J15" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="J22" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the extent test to the model run log (also added short names)
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91FBA4A-C1E8-4087-BAB5-E58E8D07366F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B14E7C8-A8A2-435A-A000-3C4F0A92022E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$I$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="95">
   <si>
     <t>No Project</t>
   </si>
@@ -279,6 +279,48 @@
   </si>
   <si>
     <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn03</t>
+  </si>
+  <si>
+    <t>Blueprint rerun</t>
+  </si>
+  <si>
+    <t>short_name</t>
+  </si>
+  <si>
+    <t>no toll discount</t>
+  </si>
+  <si>
+    <t>70% toll discount for Q1</t>
+  </si>
+  <si>
+    <t>50% toll discount for Q1</t>
+  </si>
+  <si>
+    <t>100% toll discount for Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% toll discount for Q1 + no discount for HOVs </t>
+  </si>
+  <si>
+    <t>Doubling the tolls</t>
+  </si>
+  <si>
+    <t>Tripling the tolls</t>
+  </si>
+  <si>
+    <t>ALT along Caltrain and Bart</t>
+  </si>
+  <si>
+    <t>No ALT</t>
+  </si>
+  <si>
+    <t>2015 base year (IPA</t>
+  </si>
+  <si>
+    <t>2015 base year</t>
+  </si>
+  <si>
+    <t>Blueprint rerun with ALT segments</t>
   </si>
 </sst>
 </file>
@@ -836,11 +878,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -848,12 +890,13 @@
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.8984375" customWidth="1"/>
-    <col min="7" max="7" width="15" style="5" customWidth="1"/>
-    <col min="9" max="9" width="37.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.296875" customWidth="1"/>
+    <col min="7" max="7" width="43.69921875" customWidth="1"/>
+    <col min="8" max="8" width="15" style="5" customWidth="1"/>
+    <col min="10" max="10" width="37.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -870,22 +913,25 @@
         <v>1</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -902,17 +948,20 @@
         <v>6</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J2" s="28"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -928,21 +977,22 @@
       <c r="E3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="13"/>
+      <c r="J3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -958,21 +1008,22 @@
       <c r="E4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="13"/>
+      <c r="J4" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
@@ -988,21 +1039,22 @@
       <c r="E5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
@@ -1019,22 +1071,25 @@
         <v>6</v>
       </c>
       <c r="F6" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1051,19 +1106,22 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="J7" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>43</v>
       </c>
@@ -1079,21 +1137,22 @@
       <c r="E8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="13" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="K8" s="29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -1110,22 +1169,25 @@
         <v>0</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="K9" s="29" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>43</v>
       </c>
@@ -1141,21 +1203,22 @@
       <c r="E10" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33" t="s">
+      <c r="F10" s="32"/>
+      <c r="G10" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="32"/>
+      <c r="J10" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="34" t="s">
+      <c r="K10" s="34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>43</v>
       </c>
@@ -1172,22 +1235,25 @@
         <v>41</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="J11" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="K11" s="34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>43</v>
       </c>
@@ -1203,21 +1269,22 @@
       <c r="E12" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="38"/>
-      <c r="I12" s="33" t="s">
+      <c r="F12" s="38"/>
+      <c r="G12" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="38"/>
+      <c r="J12" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="K12" s="33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>43</v>
       </c>
@@ -1233,21 +1300,22 @@
       <c r="E13" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33" t="s">
+      <c r="F13" s="33"/>
+      <c r="G13" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="K13" s="33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>43</v>
       </c>
@@ -1263,21 +1331,22 @@
       <c r="E14" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33" t="s">
+      <c r="F14" s="33"/>
+      <c r="G14" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="K14" s="33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>43</v>
       </c>
@@ -1294,22 +1363,25 @@
         <v>41</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="J15" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="34" t="s">
+      <c r="K15" s="34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>43</v>
       </c>
@@ -1325,23 +1397,26 @@
       <c r="E16" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="24" t="s">
+      <c r="F16" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="J16" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>43</v>
       </c>
@@ -1357,23 +1432,26 @@
       <c r="E17" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="26" t="s">
+      <c r="F17" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="26" t="s">
+      <c r="J17" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>43</v>
       </c>
@@ -1389,23 +1467,26 @@
       <c r="E18" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="26" t="s">
+      <c r="F18" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="26" t="s">
+      <c r="J18" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>43</v>
       </c>
@@ -1421,23 +1502,26 @@
       <c r="E19" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="26" t="s">
+      <c r="F19" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="J19" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>43</v>
       </c>
@@ -1453,23 +1537,26 @@
       <c r="E20" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="26" t="s">
+      <c r="F20" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="26" t="s">
+      <c r="J20" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>43</v>
       </c>
@@ -1485,21 +1572,22 @@
       <c r="E21" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26" t="s">
+      <c r="F21" s="27"/>
+      <c r="G21" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>43</v>
       </c>
@@ -1515,21 +1603,26 @@
       <c r="E22" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="26"/>
+      <c r="F22" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="I22" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="K22" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>43</v>
       </c>
@@ -1545,23 +1638,26 @@
       <c r="E23" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="26" t="s">
+      <c r="F23" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="J23" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>43</v>
       </c>
@@ -1577,23 +1673,26 @@
       <c r="E24" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="26" t="s">
+      <c r="F24" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I24" s="26" t="s">
+      <c r="J24" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>43</v>
       </c>
@@ -1609,23 +1708,24 @@
       <c r="E25" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="26" t="s">
+      <c r="F25" s="27"/>
+      <c r="G25" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="I25" s="26" t="s">
+      <c r="J25" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>43</v>
       </c>
@@ -1641,23 +1741,24 @@
       <c r="E26" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" s="26" t="s">
+      <c r="F26" s="27"/>
+      <c r="G26" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="I26" s="26" t="s">
+      <c r="J26" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>43</v>
       </c>
@@ -1673,29 +1774,30 @@
       <c r="E27" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="F27" s="17"/>
+      <c r="G27" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I27" s="26" t="s">
+      <c r="J27" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J10" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
-    <hyperlink ref="J8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="J15" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="J22" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="K8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
+    <hyperlink ref="K15" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="K22" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>

</xml_diff>

<commit_message>
add the series of sensitivity tests that pivots from BP ALT with min tolls
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B14E7C8-A8A2-435A-A000-3C4F0A92022E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD67A7F-A3B3-4B0B-96A3-375B110C82B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="105">
   <si>
     <t>No Project</t>
   </si>
@@ -314,13 +314,43 @@
     <t>No ALT</t>
   </si>
   <si>
-    <t>2015 base year (IPA</t>
-  </si>
-  <si>
     <t>2015 base year</t>
   </si>
   <si>
     <t>Blueprint rerun with ALT segments</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn00</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn00_1</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn00_2</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn00_3</t>
+  </si>
+  <si>
+    <t>2015 base year (IPA)</t>
+  </si>
+  <si>
+    <t>Base year</t>
+  </si>
+  <si>
+    <t>Blueprint ALT with min tolls</t>
+  </si>
+  <si>
+    <t>Dynamic - target 45mph, max $5 per mile</t>
+  </si>
+  <si>
+    <t>Dynamic - target 45mph, max $1 per mile</t>
+  </si>
+  <si>
+    <t>Dynamic - target 30mph, max $5 per mile</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/572982923864207/1203210486755114</t>
   </si>
 </sst>
 </file>
@@ -421,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -447,6 +477,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -455,12 +496,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -496,14 +533,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -518,14 +547,42 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -878,11 +935,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -890,102 +947,102 @@
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="33.296875" customWidth="1"/>
+    <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.69921875" customWidth="1"/>
-    <col min="8" max="8" width="15" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15" style="3" customWidth="1"/>
     <col min="10" max="10" width="37.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>2015</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="E2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="28"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="10">
         <v>2015</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="D3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11" t="s">
         <v>59</v>
       </c>
       <c r="K3" t="s">
@@ -993,30 +1050,30 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="12">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="10">
         <v>2015</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="D4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13" t="s">
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
         <v>59</v>
       </c>
       <c r="K4" t="s">
@@ -1024,30 +1081,30 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="12">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="10">
         <v>2015</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
+      <c r="D5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
         <v>59</v>
       </c>
       <c r="K5" t="s">
@@ -1055,361 +1112,361 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="12">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="10">
         <v>2015</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="13" t="s">
+      <c r="D6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="11" t="s">
         <v>59</v>
       </c>
       <c r="K6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
-        <v>2035</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="46">
+        <v>2035</v>
+      </c>
+      <c r="C7" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C8" s="16" t="s">
+    <row r="8" spans="1:11" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="37">
+        <v>2035</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="13" t="s">
+      <c r="F8" s="38"/>
+      <c r="G8" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C9" s="16" t="s">
+    <row r="9" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="D9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="16" t="s">
+      <c r="G9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="31">
-        <v>2035</v>
-      </c>
-      <c r="C10" s="32" t="s">
+    <row r="10" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="42">
+        <v>2035</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="32" t="s">
+      <c r="D10" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="33" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="43"/>
+      <c r="J10" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="31">
-        <v>2035</v>
-      </c>
-      <c r="C11" s="32" t="s">
+    <row r="11" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="42">
+        <v>2035</v>
+      </c>
+      <c r="C11" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="32" t="s">
+      <c r="D11" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="32" t="s">
+      <c r="G11" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="33" t="s">
+      <c r="J11" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="37">
-        <v>2035</v>
-      </c>
-      <c r="C12" s="38" t="s">
+    <row r="12" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="42">
+        <v>2035</v>
+      </c>
+      <c r="C12" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="38" t="s">
+      <c r="D12" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="33" t="s">
+      <c r="F12" s="43"/>
+      <c r="G12" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="43"/>
+      <c r="J12" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="33" t="s">
+      <c r="K12" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C13" s="33" t="s">
+    <row r="13" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="33" t="s">
+      <c r="D13" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33" t="s">
+      <c r="F13" s="27"/>
+      <c r="G13" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="33" t="s">
+      <c r="K13" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C14" s="33" t="s">
+    <row r="14" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="33" t="s">
+      <c r="D14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="33" t="s">
+      <c r="K14" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="31">
-        <v>2035</v>
-      </c>
-      <c r="C15" s="32" t="s">
+    <row r="15" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="25">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="32" t="s">
+      <c r="D15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="32" t="s">
+      <c r="F15" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="34" t="s">
+      <c r="K15" s="51" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="A16" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="25" t="s">
+      <c r="D16" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="24" t="s">
+      <c r="G16" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K16" t="s">
@@ -1417,34 +1474,34 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="26" t="s">
+      <c r="A17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="27" t="s">
+      <c r="D17" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="26" t="s">
+      <c r="G17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K17" t="s">
@@ -1452,34 +1509,34 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="26" t="s">
+      <c r="A18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="27" t="s">
+      <c r="D18" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="26" t="s">
+      <c r="G18" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K18" t="s">
@@ -1487,34 +1544,34 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="26" t="s">
+      <c r="A19" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="27" t="s">
+      <c r="D19" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="26" t="s">
+      <c r="G19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="J19" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K19" t="s">
@@ -1522,34 +1579,34 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="26" t="s">
+      <c r="A20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="27" t="s">
+      <c r="D20" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="26" t="s">
+      <c r="G20" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="26" t="s">
+      <c r="J20" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K20" t="s">
@@ -1557,30 +1614,30 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="26" t="s">
+      <c r="A21" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="27" t="s">
+      <c r="D21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26" t="s">
+      <c r="F21" s="21"/>
+      <c r="G21" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20" t="s">
         <v>76</v>
       </c>
       <c r="K21" t="s">
@@ -1588,69 +1645,69 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="26" t="s">
+      <c r="A22" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="27" t="s">
+      <c r="D22" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="G22" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="26" t="s">
+      <c r="G22" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="23" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="26" t="s">
+      <c r="A23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="27" t="s">
+      <c r="D23" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="26" t="s">
+      <c r="G23" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K23" t="s">
@@ -1658,34 +1715,34 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="26" t="s">
+      <c r="A24" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="27" t="s">
+      <c r="D24" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="G24" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="26" t="s">
+      <c r="G24" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="26" t="s">
+      <c r="J24" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K24" t="s">
@@ -1693,32 +1750,30 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="26" t="s">
+      <c r="A25" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="27" t="s">
+      <c r="D25" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="J25" s="26" t="s">
+      <c r="F25" s="21"/>
+      <c r="G25" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20" t="s">
         <v>72</v>
       </c>
       <c r="K25" t="s">
@@ -1726,70 +1781,200 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="26" t="s">
+      <c r="A26" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="27" t="s">
+      <c r="D26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="J26" s="26" t="s">
+      <c r="F26" s="21"/>
+      <c r="G26" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20" t="s">
         <v>72</v>
       </c>
       <c r="K26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="3" t="s">
+    <row r="27" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="3" t="s">
+      <c r="F27" s="34"/>
+      <c r="G27" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="K28" s="52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J29" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K27" t="s">
-        <v>55</v>
-      </c>
+      <c r="K29" s="53"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J30" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" s="53"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" s="53"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1798,8 +1983,9 @@
     <hyperlink ref="K8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
     <hyperlink ref="K15" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
     <hyperlink ref="K22" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K28" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add model3-a and model3-b test runs to ModelRuns.xlsx
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD67A7F-A3B3-4B0B-96A3-375B110C82B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E529652-04B0-4253-9B6C-35D4CAFA2E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1070" yWindow="2020" windowWidth="20130" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="111">
   <si>
     <t>No Project</t>
   </si>
@@ -351,6 +351,24 @@
   </si>
   <si>
     <t>https://app.asana.com/0/572982923864207/1203210486755114</t>
+  </si>
+  <si>
+    <t>Test New Machine</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_model3aTEST</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_model3bTEST</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1201809392759895/1203117364345675/f</t>
+  </si>
+  <si>
+    <t>Blueprint rerun with ALT segments TEST3a</t>
+  </si>
+  <si>
+    <t>Blueprint rerun with ALT segments TEST3b</t>
   </si>
 </sst>
 </file>
@@ -935,18 +953,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.69921875" customWidth="1"/>
     <col min="8" max="8" width="15" style="3" customWidth="1"/>
@@ -1403,144 +1421,144 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C15" s="26" t="s">
+    <row r="15" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="42">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="26" t="s">
+      <c r="D15" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="26" t="s">
+      <c r="G15" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="51" t="s">
+      <c r="K15" s="44" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="33" t="s">
+    <row r="16" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="42">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="25">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="34" t="s">
+      <c r="D18" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F18" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="20" t="s">
+      <c r="G18" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="33" t="s">
         <v>9</v>
       </c>
       <c r="J18" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1551,7 +1569,7 @@
         <v>2035</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>26</v>
@@ -1560,7 +1578,7 @@
         <v>33</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>30</v>
@@ -1575,7 +1593,7 @@
         <v>40</v>
       </c>
       <c r="K19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1586,7 +1604,7 @@
         <v>2035</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>26</v>
@@ -1595,7 +1613,7 @@
         <v>33</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>30</v>
@@ -1610,7 +1628,7 @@
         <v>40</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1621,7 +1639,7 @@
         <v>2035</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>26</v>
@@ -1629,19 +1647,23 @@
       <c r="E21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="21"/>
+      <c r="F21" s="21" t="s">
+        <v>86</v>
+      </c>
       <c r="G21" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="20"/>
+      <c r="I21" s="20" t="s">
+        <v>9</v>
+      </c>
       <c r="J21" s="20" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="K21" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1652,7 +1674,7 @@
         <v>2035</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>26</v>
@@ -1661,7 +1683,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>30</v>
@@ -1673,10 +1695,10 @@
         <v>9</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="K22" s="23" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="K22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1687,7 +1709,7 @@
         <v>2035</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>26</v>
@@ -1695,23 +1717,19 @@
       <c r="E23" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="21" t="s">
-        <v>88</v>
-      </c>
+      <c r="F23" s="21"/>
       <c r="G23" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="I23" s="20"/>
       <c r="J23" s="20" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="K23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1722,7 +1740,7 @@
         <v>2035</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>26</v>
@@ -1731,7 +1749,7 @@
         <v>33</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>30</v>
@@ -1743,10 +1761,10 @@
         <v>9</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K24" t="s">
-        <v>55</v>
+        <v>77</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1757,7 +1775,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>26</v>
@@ -1765,19 +1783,23 @@
       <c r="E25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="21"/>
+      <c r="F25" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="G25" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="20"/>
+      <c r="I25" s="20" t="s">
+        <v>9</v>
+      </c>
       <c r="J25" s="20" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="K25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1788,7 +1810,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>26</v>
@@ -1796,49 +1818,53 @@
       <c r="E26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="21"/>
+      <c r="F26" s="21" t="s">
+        <v>89</v>
+      </c>
       <c r="G26" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="20"/>
+      <c r="I26" s="20" t="s">
+        <v>9</v>
+      </c>
       <c r="J26" s="20" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="K26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="34" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33" t="s">
+      <c r="F27" s="21"/>
+      <c r="G27" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="35" t="s">
+      <c r="K27" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1850,65 +1876,59 @@
         <v>2035</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="G28" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" s="33" t="s">
+      <c r="F28" s="21"/>
+      <c r="G28" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K28" s="52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="21" t="s">
+      <c r="K28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="J29" s="20" t="s">
+      <c r="F29" s="34"/>
+      <c r="G29" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="53"/>
+      <c r="K29" s="35" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
@@ -1918,63 +1938,131 @@
         <v>2035</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="J30" s="20" t="s">
+      <c r="F30" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="53"/>
+      <c r="K30" s="52" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="15" t="s">
+      <c r="A31" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="1" t="s">
+      <c r="F31" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="20" t="s">
         <v>75</v>
       </c>
       <c r="J31" s="20" t="s">
         <v>72</v>
       </c>
       <c r="K31" s="53"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K32" s="53"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K33" s="53"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1982,10 +2070,12 @@
     <hyperlink ref="K10" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="K8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
     <hyperlink ref="K15" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K22" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K28" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K24" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K30" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K16" r:id="rId6" xr:uid="{CD6F2AB8-F8E9-45D8-8A10-4B484D7EE55C}"/>
+    <hyperlink ref="K17" r:id="rId7" xr:uid="{61852A28-3E94-44D8-B0F8-B5368743A630}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "add model3-a and model3-b test runs to ModelRuns.xlsx"
This reverts commit 3276350df834a0f829f364b64cca9d697f077833.
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E529652-04B0-4253-9B6C-35D4CAFA2E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD67A7F-A3B3-4B0B-96A3-375B110C82B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1070" yWindow="2020" windowWidth="20130" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="105">
   <si>
     <t>No Project</t>
   </si>
@@ -351,24 +351,6 @@
   </si>
   <si>
     <t>https://app.asana.com/0/572982923864207/1203210486755114</t>
-  </si>
-  <si>
-    <t>Test New Machine</t>
-  </si>
-  <si>
-    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_model3aTEST</t>
-  </si>
-  <si>
-    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_model3bTEST</t>
-  </si>
-  <si>
-    <t>https://app.asana.com/0/1201809392759895/1203117364345675/f</t>
-  </si>
-  <si>
-    <t>Blueprint rerun with ALT segments TEST3a</t>
-  </si>
-  <si>
-    <t>Blueprint rerun with ALT segments TEST3b</t>
   </si>
 </sst>
 </file>
@@ -953,18 +935,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.69921875" customWidth="1"/>
     <col min="8" max="8" width="15" style="3" customWidth="1"/>
@@ -1421,144 +1403,144 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="42">
-        <v>2035</v>
-      </c>
-      <c r="C15" s="43" t="s">
+    <row r="15" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="25">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="43" t="s">
+      <c r="D15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="43" t="s">
+      <c r="G15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="43" t="s">
+      <c r="J15" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="44" t="s">
+      <c r="K15" s="51" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="42">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="43" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="K16" s="44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="26" t="s">
+      <c r="J16" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="K17" s="51" t="s">
-        <v>108</v>
+      <c r="J17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="34" t="s">
+      <c r="A18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="33" t="s">
+      <c r="F18" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="20" t="s">
         <v>9</v>
       </c>
       <c r="J18" s="20" t="s">
         <v>40</v>
       </c>
       <c r="K18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1569,7 +1551,7 @@
         <v>2035</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>26</v>
@@ -1578,7 +1560,7 @@
         <v>33</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>30</v>
@@ -1593,7 +1575,7 @@
         <v>40</v>
       </c>
       <c r="K19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1604,7 +1586,7 @@
         <v>2035</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>26</v>
@@ -1613,7 +1595,7 @@
         <v>33</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>30</v>
@@ -1628,7 +1610,7 @@
         <v>40</v>
       </c>
       <c r="K20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1639,7 +1621,7 @@
         <v>2035</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>26</v>
@@ -1647,23 +1629,19 @@
       <c r="E21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="21" t="s">
-        <v>86</v>
-      </c>
+      <c r="F21" s="21"/>
       <c r="G21" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="I21" s="20"/>
       <c r="J21" s="20" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="K21" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1674,7 +1652,7 @@
         <v>2035</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>26</v>
@@ -1683,7 +1661,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>30</v>
@@ -1695,10 +1673,10 @@
         <v>9</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" t="s">
-        <v>37</v>
+        <v>77</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1709,7 +1687,7 @@
         <v>2035</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>26</v>
@@ -1717,19 +1695,23 @@
       <c r="E23" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="21"/>
+      <c r="F23" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="G23" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="20" t="s">
+        <v>9</v>
+      </c>
       <c r="J23" s="20" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="K23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1740,7 +1722,7 @@
         <v>2035</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>26</v>
@@ -1749,7 +1731,7 @@
         <v>33</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>30</v>
@@ -1761,10 +1743,10 @@
         <v>9</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="K24" s="23" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="K24" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1775,7 +1757,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>26</v>
@@ -1783,23 +1765,19 @@
       <c r="E25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>88</v>
-      </c>
+      <c r="F25" s="21"/>
       <c r="G25" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="I25" s="20"/>
       <c r="J25" s="20" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="K25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1810,7 +1788,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>26</v>
@@ -1818,53 +1796,49 @@
       <c r="E26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>89</v>
-      </c>
+      <c r="F26" s="21"/>
       <c r="G26" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="I26" s="20"/>
       <c r="J26" s="20" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="K26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="21" t="s">
+    <row r="27" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20" t="s">
+      <c r="F27" s="34"/>
+      <c r="G27" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="35" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1876,59 +1850,65 @@
         <v>2035</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20" t="s">
+      <c r="F28" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="K28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="34" t="s">
+      <c r="K28" s="52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33" t="s">
+      <c r="F29" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="35" t="s">
-        <v>55</v>
-      </c>
+      <c r="K29" s="53"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
@@ -1938,131 +1918,63 @@
         <v>2035</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="G30" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I30" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="33" t="s">
+      <c r="F30" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J30" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="52" t="s">
-        <v>104</v>
-      </c>
+      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="21" t="s">
+      <c r="A31" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="20" t="s">
+      <c r="F31" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>75</v>
       </c>
       <c r="J31" s="20" t="s">
         <v>72</v>
       </c>
       <c r="K31" s="53"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="J32" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="K32" s="53"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J33" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="K33" s="53"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2070,12 +1982,10 @@
     <hyperlink ref="K10" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="K8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
     <hyperlink ref="K15" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K24" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K30" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
-    <hyperlink ref="K16" r:id="rId6" xr:uid="{CD6F2AB8-F8E9-45D8-8A10-4B484D7EE55C}"/>
-    <hyperlink ref="K17" r:id="rId7" xr:uid="{61852A28-3E94-44D8-B0F8-B5368743A630}"/>
+    <hyperlink ref="K22" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K28" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding mock pathway runs to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD67A7F-A3B3-4B0B-96A3-375B110C82B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB571B5-5467-4EFD-B3DA-D3AC20D985FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="117">
   <si>
     <t>No Project</t>
   </si>
@@ -263,9 +263,6 @@
     <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SensDyn01</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>an old version of NGF_Networks_02</t>
   </si>
   <si>
@@ -351,6 +348,45 @@
   </si>
   <si>
     <t>https://app.asana.com/0/572982923864207/1203210486755114</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALT13Segments_01</t>
+  </si>
+  <si>
+    <t>Mock</t>
+  </si>
+  <si>
+    <t>Blueprint with 13 segments</t>
+  </si>
+  <si>
+    <t>NGF_Networks_10</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1201809392759895/1203387406064542</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SimpleTolls01</t>
+  </si>
+  <si>
+    <t>Blueprint with simplified tolls</t>
+  </si>
+  <si>
+    <t>NGF_Networks_07 but a new tolls.csv</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1201809392759895/1203387769299605</t>
   </si>
 </sst>
 </file>
@@ -496,7 +532,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -550,15 +586,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,11 +593,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -582,7 +604,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -935,11 +956,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -970,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>10</v>
@@ -1002,10 +1023,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>17</v>
@@ -1032,7 +1053,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
@@ -1063,7 +1084,7 @@
         <v>26</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
@@ -1094,7 +1115,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
@@ -1125,10 +1146,10 @@
         <v>26</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>17</v>
@@ -1146,70 +1167,70 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+    <row r="7" spans="1:11" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="46">
-        <v>2035</v>
-      </c>
-      <c r="C7" s="47" t="s">
+      <c r="B7" s="38">
+        <v>2035</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="G7" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="37">
-        <v>2035</v>
-      </c>
-      <c r="C8" s="38" t="s">
+    <row r="8" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C8" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="38" t="s">
+      <c r="D8" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38" t="s">
+      <c r="F8" s="33"/>
+      <c r="G8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="K8" s="34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>43</v>
       </c>
@@ -1226,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>30</v>
@@ -1240,34 +1261,34 @@
       <c r="J9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K9" s="49" t="s">
+      <c r="K9" s="41" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="42">
-        <v>2035</v>
-      </c>
-      <c r="C10" s="43" t="s">
+      <c r="A10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="43" t="s">
+      <c r="D10" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="43"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="27"/>
       <c r="J10" s="27" t="s">
         <v>40</v>
       </c>
@@ -1275,65 +1296,65 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="42">
-        <v>2035</v>
-      </c>
-      <c r="C11" s="43" t="s">
+    <row r="11" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="43" t="s">
+      <c r="D11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="43" t="s">
+      <c r="F11" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="43" t="s">
+      <c r="J11" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="44" t="s">
+      <c r="K11" s="36" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="42">
-        <v>2035</v>
-      </c>
-      <c r="C12" s="43" t="s">
+      <c r="A12" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="43" t="s">
+      <c r="D12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="43"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="27"/>
       <c r="J12" s="27" t="s">
         <v>57</v>
       </c>
@@ -1420,7 +1441,7 @@
         <v>41</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G15" s="26" t="s">
         <v>30</v>
@@ -1434,36 +1455,36 @@
       <c r="J15" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="51" t="s">
+      <c r="K15" s="43" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="33" t="s">
+      <c r="A16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="34" t="s">
+      <c r="D16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="33" t="s">
+      <c r="F16" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>9</v>
       </c>
       <c r="J16" s="20" t="s">
@@ -1490,7 +1511,7 @@
         <v>33</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>30</v>
@@ -1525,7 +1546,7 @@
         <v>33</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>30</v>
@@ -1560,7 +1581,7 @@
         <v>33</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>30</v>
@@ -1595,7 +1616,7 @@
         <v>33</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>30</v>
@@ -1638,7 +1659,7 @@
       </c>
       <c r="I21" s="20"/>
       <c r="J21" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K21" t="s">
         <v>53</v>
@@ -1652,7 +1673,7 @@
         <v>2035</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>26</v>
@@ -1661,7 +1682,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>30</v>
@@ -1673,7 +1694,7 @@
         <v>9</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K22" s="23" t="s">
         <v>53</v>
@@ -1696,7 +1717,7 @@
         <v>33</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>30</v>
@@ -1731,7 +1752,7 @@
         <v>33</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>30</v>
@@ -1788,7 +1809,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>26</v>
@@ -1811,34 +1832,34 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="34" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33" t="s">
+      <c r="F27" s="21"/>
+      <c r="G27" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="35" t="s">
+      <c r="K27" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1850,31 +1871,31 @@
         <v>2035</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="G28" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="33" t="s">
+      <c r="F28" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="33" t="s">
+      <c r="J28" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K28" s="52" t="s">
-        <v>104</v>
+      <c r="K28" s="44" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1885,7 +1906,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>26</v>
@@ -1894,7 +1915,7 @@
         <v>33</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>30</v>
@@ -1902,13 +1923,10 @@
       <c r="H29" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I29" s="20" t="s">
-        <v>75</v>
-      </c>
+      <c r="I29" s="20"/>
       <c r="J29" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="53"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
@@ -1918,7 +1936,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>26</v>
@@ -1927,7 +1945,7 @@
         <v>33</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>30</v>
@@ -1935,13 +1953,10 @@
       <c r="H30" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="20" t="s">
-        <v>75</v>
-      </c>
+      <c r="I30" s="20"/>
       <c r="J30" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
@@ -1951,7 +1966,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>26</v>
@@ -1960,7 +1975,7 @@
         <v>33</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>30</v>
@@ -1968,13 +1983,80 @@
       <c r="H31" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="I31" s="1"/>
       <c r="J31" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="K31" s="53"/>
+    </row>
+    <row r="32" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
adding 2015_TM152_NGF_05 and staging for NoProject and P1b
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB571B5-5467-4EFD-B3DA-D3AC20D985FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4C89C1-AEE4-4F76-8753-297F2F5F8D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$I$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$I$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="125">
   <si>
     <t>No Project</t>
   </si>
@@ -365,18 +365,6 @@
     <t>https://app.asana.com/0/1201809392759895/1203387406064542</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>2035_TM152_NGF_NP02_BPALTsegmented_03_SimpleTolls01</t>
   </si>
   <si>
@@ -387,6 +375,42 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1201809392759895/1203387769299605</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07</t>
+  </si>
+  <si>
+    <t>Pathway 4: No "new" pricing</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1203880292726527/f</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NoProjectNoSFCordon_07</t>
+  </si>
+  <si>
+    <t>2015_TM152_NGF_05</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1201809392759895/1203246561643081/f</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>Pathways</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01</t>
+  </si>
+  <si>
+    <t>Pathway 1b: All-lane tolling + Focus on Affordability</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P1b_AllLaneTolling_Affordable_01</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1203644636776965/f</t>
   </si>
 </sst>
 </file>
@@ -455,7 +479,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +507,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,10 +568,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -549,10 +584,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -573,37 +604,58 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -956,11 +1008,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -970,1104 +1022,1182 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.69921875" customWidth="1"/>
-    <col min="8" max="8" width="15" style="3" customWidth="1"/>
-    <col min="10" max="10" width="37.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="2" customWidth="1"/>
+    <col min="10" max="10" width="47.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="26">
         <v>2015</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="22"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="10">
+      <c r="J2" s="28"/>
+    </row>
+    <row r="3" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="52">
         <v>2015</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="51" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="10">
+    <row r="4" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="52">
         <v>2015</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="51" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="10">
+    <row r="5" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="52">
         <v>2015</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11" t="s">
+      <c r="I5" s="17"/>
+      <c r="J5" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="51" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="10">
+    <row r="6" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="52">
         <v>2015</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="17"/>
+      <c r="J6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="52">
+        <v>2015</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J7" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="K7" s="53" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="38">
-        <v>2035</v>
-      </c>
-      <c r="C7" s="39" t="s">
+      <c r="B8" s="31">
+        <v>2035</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E8" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F8" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G8" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="38" t="s">
+      <c r="H8" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="39" t="s">
+      <c r="I8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J8" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C8" s="33" t="s">
+    <row r="9" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="43">
+        <v>2035</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="33" t="s">
+      <c r="D9" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33" t="s">
+      <c r="F9" s="44"/>
+      <c r="G9" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K9" s="45" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C9" s="14" t="s">
+    <row r="10" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C10" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="D10" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F10" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="14" t="s">
+      <c r="G10" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K10" s="49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C10" s="27" t="s">
+    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2035</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11" s="50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="K12" s="54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="D13" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27" t="s">
+      <c r="F13" s="35"/>
+      <c r="G13" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K13" s="36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C11" s="27" t="s">
+    <row r="14" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C14" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="27" t="s">
+      <c r="D14" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F14" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="27" t="s">
+      <c r="G14" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K14" s="37" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C12" s="27" t="s">
+    <row r="15" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="27" t="s">
+      <c r="D15" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27" t="s">
+      <c r="F15" s="35"/>
+      <c r="G15" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K15" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C13" s="27" t="s">
+    <row r="16" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="27" t="s">
+      <c r="D16" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="27" t="s">
+      <c r="K16" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C14" s="27" t="s">
+    <row r="17" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="27" t="s">
+      <c r="D17" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27" t="s">
+      <c r="F17" s="35"/>
+      <c r="G17" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="27" t="s">
+      <c r="K17" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C15" s="26" t="s">
+    <row r="18" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="26" t="s">
+      <c r="D18" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F18" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="26" t="s">
+      <c r="G18" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="43" t="s">
+      <c r="K18" s="41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="20" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="21" t="s">
+      <c r="D19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F19" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="20" t="s">
+      <c r="G19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="20" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="21" t="s">
+      <c r="D20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F20" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="20" t="s">
+      <c r="G20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="20" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="21" t="s">
+      <c r="D21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F21" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="20" t="s">
+      <c r="G21" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="20" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="21" t="s">
+      <c r="D22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F22" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="G19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="20" t="s">
+      <c r="G22" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="20" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="21" t="s">
+      <c r="D23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F23" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="20" t="s">
+      <c r="G23" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="20" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="21" t="s">
+      <c r="D24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20" t="s">
+      <c r="F24" s="18"/>
+      <c r="G24" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="20" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="21" t="s">
+      <c r="D25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F25" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="20" t="s">
+      <c r="G25" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="K22" s="23" t="s">
+      <c r="K25" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="20" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="21" t="s">
+      <c r="D26" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F26" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J23" s="20" t="s">
+      <c r="G26" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="20" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="21" t="s">
+      <c r="D27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F27" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="20" t="s">
+      <c r="G27" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="K24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="K25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="K26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20" t="s">
-        <v>72</v>
       </c>
       <c r="K27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C28" s="20" t="s">
+      <c r="A28" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="21" t="s">
+      <c r="D31" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F31" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="G28" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" s="20" t="s">
+      <c r="G31" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K28" s="44" t="s">
+      <c r="K31" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="20" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="21" t="s">
+      <c r="D32" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F32" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20" t="s">
+      <c r="G32" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C30" s="20" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="21" t="s">
+      <c r="D33" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F33" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G30" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20" t="s">
+      <c r="G33" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="1" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="15" t="s">
+      <c r="D34" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F34" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="G31" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="20" t="s">
+      <c r="G34" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="27" t="s">
+    <row r="35" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="27" t="s">
+      <c r="D35" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F35" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G32" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="27" t="s">
+      <c r="G35" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="K32" s="28" t="s">
+      <c r="K35" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="27" t="s">
+    <row r="36" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F33" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="I33" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="K33" s="28" t="s">
-        <v>116</v>
+      <c r="F36" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="K36" s="21" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
-    <hyperlink ref="K8" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="K15" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K22" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K28" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K13" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
+    <hyperlink ref="K18" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="K25" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K31" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K11" r:id="rId6" xr:uid="{F617EBD0-985C-4EA1-B75F-884D1AED06F6}"/>
+    <hyperlink ref="K7" r:id="rId7" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
+    <hyperlink ref="K12" r:id="rId8" xr:uid="{9DD30DA7-A7AD-43EC-BABA-F91175587CE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding no project to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4C89C1-AEE4-4F76-8753-297F2F5F8D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE63DD9F-7803-4FF5-BEAC-7D0A95408310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="126">
   <si>
     <t>No Project</t>
   </si>
@@ -377,15 +377,6 @@
     <t>https://app.asana.com/0/1201809392759895/1203387769299605</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_NP07</t>
-  </si>
-  <si>
-    <t>Pathway 4: No "new" pricing</t>
-  </si>
-  <si>
-    <t>https://app.asana.com/0/1203644633064654/1203880292726527/f</t>
-  </si>
-  <si>
     <t>NGF_Networks_NoProjectNoSFCordon_07</t>
   </si>
   <si>
@@ -411,6 +402,18 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1203644633064654/1203644636776965/f</t>
+  </si>
+  <si>
+    <t>NoProject</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_TollCalibrated02</t>
+  </si>
+  <si>
+    <t>✓ Run NoProject with calibrated tolls</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_TollCalibrated01</t>
   </si>
 </sst>
 </file>
@@ -643,19 +646,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1008,11 +1011,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1091,11 +1094,11 @@
       </c>
       <c r="J2" s="28"/>
     </row>
-    <row r="3" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="52">
+    <row r="3" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="51">
         <v>2015</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -1111,22 +1114,22 @@
       <c r="G3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="52">
+    <row r="4" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="51">
         <v>2015</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -1142,22 +1145,22 @@
       <c r="G4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="50" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="52">
+    <row r="5" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="51">
         <v>2015</v>
       </c>
       <c r="C5" s="17" t="s">
@@ -1173,22 +1176,22 @@
       <c r="G5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="51" t="s">
+      <c r="K5" s="50" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="52">
+    <row r="6" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="51">
         <v>2015</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -1206,26 +1209,26 @@
       <c r="G6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="51" t="s">
+      <c r="K6" s="50" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="52">
+    <row r="7" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="51">
         <v>2015</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>26</v>
@@ -1239,7 +1242,7 @@
       <c r="G7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="H7" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="17" t="s">
@@ -1248,8 +1251,8 @@
       <c r="J7" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="53" t="s">
-        <v>118</v>
+      <c r="K7" s="52" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -1348,105 +1351,107 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="7">
-        <v>2035</v>
-      </c>
-      <c r="C11" s="8" t="s">
+    <row r="11" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="K11" s="54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="7">
+        <v>2035</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="K11" s="50" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="10">
-        <v>2035</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>123</v>
+      <c r="G12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="K12" s="54" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="36" t="s">
-        <v>38</v>
+    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K13" s="53" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -1457,7 +1462,7 @@
         <v>2035</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D14" s="35" t="s">
         <v>26</v>
@@ -1465,9 +1470,7 @@
       <c r="E14" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="35" t="s">
-        <v>80</v>
-      </c>
+      <c r="F14" s="35"/>
       <c r="G14" s="35" t="s">
         <v>30</v>
       </c>
@@ -1476,10 +1479,10 @@
       </c>
       <c r="I14" s="35"/>
       <c r="J14" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" s="37" t="s">
-        <v>69</v>
+        <v>40</v>
+      </c>
+      <c r="K14" s="36" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -1490,7 +1493,7 @@
         <v>2035</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>26</v>
@@ -1498,7 +1501,9 @@
       <c r="E15" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="35"/>
+      <c r="F15" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="G15" s="35" t="s">
         <v>30</v>
       </c>
@@ -1507,10 +1512,10 @@
       </c>
       <c r="I15" s="35"/>
       <c r="J15" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>56</v>
+        <v>70</v>
+      </c>
+      <c r="K15" s="37" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -1521,7 +1526,7 @@
         <v>2035</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>26</v>
@@ -1538,7 +1543,7 @@
       </c>
       <c r="I16" s="35"/>
       <c r="J16" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K16" s="35" t="s">
         <v>56</v>
@@ -1552,7 +1557,7 @@
         <v>2035</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="35" t="s">
         <v>26</v>
@@ -1569,76 +1574,74 @@
       </c>
       <c r="I17" s="35"/>
       <c r="J17" s="35" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="K17" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="40" t="s">
+    <row r="18" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="40" t="s">
+      <c r="D19" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F19" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40" t="s">
+      <c r="G19" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="K18" s="41" t="s">
+      <c r="K19" s="41" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1649,7 +1652,7 @@
         <v>2035</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>26</v>
@@ -1658,7 +1661,7 @@
         <v>33</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>30</v>
@@ -1671,7 +1674,7 @@
         <v>40</v>
       </c>
       <c r="K20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1682,7 +1685,7 @@
         <v>2035</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>26</v>
@@ -1691,7 +1694,7 @@
         <v>33</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>30</v>
@@ -1704,7 +1707,7 @@
         <v>40</v>
       </c>
       <c r="K21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1715,7 +1718,7 @@
         <v>2035</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>26</v>
@@ -1724,7 +1727,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>30</v>
@@ -1737,7 +1740,7 @@
         <v>40</v>
       </c>
       <c r="K22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1748,7 +1751,7 @@
         <v>2035</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>26</v>
@@ -1757,7 +1760,7 @@
         <v>33</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>30</v>
@@ -1770,7 +1773,7 @@
         <v>40</v>
       </c>
       <c r="K23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1781,7 +1784,7 @@
         <v>2035</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>26</v>
@@ -1789,7 +1792,9 @@
       <c r="E24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="18"/>
+      <c r="F24" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="G24" s="14" t="s">
         <v>30</v>
       </c>
@@ -1798,10 +1803,10 @@
       </c>
       <c r="I24" s="17"/>
       <c r="J24" s="17" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="K24" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1812,7 +1817,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>26</v>
@@ -1820,9 +1825,7 @@
       <c r="E25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="18" t="s">
-        <v>89</v>
-      </c>
+      <c r="F25" s="18"/>
       <c r="G25" s="14" t="s">
         <v>30</v>
       </c>
@@ -1831,9 +1834,9 @@
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="K25" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K25" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1845,7 +1848,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>26</v>
@@ -1854,7 +1857,7 @@
         <v>33</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>30</v>
@@ -1864,10 +1867,10 @@
       </c>
       <c r="I26" s="17"/>
       <c r="J26" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1878,7 +1881,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>26</v>
@@ -1887,7 +1890,7 @@
         <v>33</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>30</v>
@@ -1900,7 +1903,7 @@
         <v>40</v>
       </c>
       <c r="K27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1911,7 +1914,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>26</v>
@@ -1919,7 +1922,9 @@
       <c r="E28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="18"/>
+      <c r="F28" s="18" t="s">
+        <v>88</v>
+      </c>
       <c r="G28" s="14" t="s">
         <v>30</v>
       </c>
@@ -1928,7 +1933,7 @@
       </c>
       <c r="I28" s="17"/>
       <c r="J28" s="17" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="K28" t="s">
         <v>55</v>
@@ -1942,7 +1947,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>26</v>
@@ -1973,7 +1978,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>26</v>
@@ -2004,7 +2009,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>26</v>
@@ -2012,9 +2017,7 @@
       <c r="E31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="18" t="s">
-        <v>99</v>
-      </c>
+      <c r="F31" s="18"/>
       <c r="G31" s="14" t="s">
         <v>30</v>
       </c>
@@ -2025,8 +2028,8 @@
       <c r="J31" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K31" s="24" t="s">
-        <v>103</v>
+      <c r="K31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -2037,7 +2040,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>26</v>
@@ -2046,7 +2049,7 @@
         <v>33</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>30</v>
@@ -2058,6 +2061,9 @@
       <c r="J32" s="17" t="s">
         <v>72</v>
       </c>
+      <c r="K32" s="24" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
@@ -2067,7 +2073,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>26</v>
@@ -2076,7 +2082,7 @@
         <v>33</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G33" s="14" t="s">
         <v>30</v>
@@ -2090,66 +2096,63 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="12" t="s">
+      <c r="A34" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="1"/>
+      <c r="F34" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="17"/>
       <c r="J34" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="K35" s="21" t="s">
-        <v>108</v>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -2160,7 +2163,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>26</v>
@@ -2169,7 +2172,7 @@
         <v>105</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>30</v>
@@ -2179,25 +2182,59 @@
       </c>
       <c r="I36" s="20"/>
       <c r="J36" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="K36" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="K36" s="21" t="s">
+      <c r="K37" s="21" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K13" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="K14" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="K9" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="K18" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K25" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K31" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
-    <hyperlink ref="K11" r:id="rId6" xr:uid="{F617EBD0-985C-4EA1-B75F-884D1AED06F6}"/>
-    <hyperlink ref="K7" r:id="rId7" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
-    <hyperlink ref="K12" r:id="rId8" xr:uid="{9DD30DA7-A7AD-43EC-BABA-F91175587CE9}"/>
+    <hyperlink ref="K19" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="K26" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K32" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K7" r:id="rId6" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
+    <hyperlink ref="K13" r:id="rId7" xr:uid="{9DD30DA7-A7AD-43EC-BABA-F91175587CE9}"/>
+    <hyperlink ref="K11" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
+    <hyperlink ref="K12" r:id="rId9" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE63DD9F-7803-4FF5-BEAC-7D0A95408310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866B0527-64D1-4220-B5ED-7C6FD95A9B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="140">
   <si>
     <t>No Project</t>
   </si>
@@ -392,18 +392,12 @@
     <t>Pathways</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_NP07_Path1b_01</t>
-  </si>
-  <si>
     <t>Pathway 1b: All-lane tolling + Focus on Affordability</t>
   </si>
   <si>
     <t>NGF_Networks_P1b_AllLaneTolling_Affordable_01</t>
   </si>
   <si>
-    <t>https://app.asana.com/0/1203644633064654/1203644636776965/f</t>
-  </si>
-  <si>
     <t>NoProject</t>
   </si>
   <si>
@@ -414,6 +408,54 @@
   </si>
   <si>
     <t>2035_TM152_NGF_NP07_TollCalibrated01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_MinToll</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_MinToll_test</t>
+  </si>
+  <si>
+    <t>NoProject - Test taskkill voyager</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_MinToll_ReproduceProblem</t>
+  </si>
+  <si>
+    <t>✓ Run NoProject with minimum tolls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoProject - voyager holding onto loadam.net </t>
+  </si>
+  <si>
+    <t>NoProject - some express lanes are priced at 0</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_MinToll</t>
+  </si>
+  <si>
+    <t>✓ Run pathway 1b with minimum tolls</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_TollCalibrated01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_TollCalibration01_speedtest</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_TollCalibration01</t>
+  </si>
+  <si>
+    <t>✓ Run pathway 1b with toll calibration</t>
+  </si>
+  <si>
+    <t>to do</t>
+  </si>
+  <si>
+    <t>Run pathway 1b with calibrated tolls</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_Simpletolls01</t>
   </si>
 </sst>
 </file>
@@ -571,7 +613,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -659,6 +701,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1011,16 +1060,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
@@ -1359,7 +1408,7 @@
         <v>2035</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D11" s="48" t="s">
         <v>26</v>
@@ -1367,9 +1416,7 @@
       <c r="E11" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="48" t="s">
-        <v>122</v>
-      </c>
+      <c r="F11" s="48"/>
       <c r="G11" s="48" t="s">
         <v>30</v>
       </c>
@@ -1381,496 +1428,490 @@
         <v>113</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="7">
-        <v>2035</v>
-      </c>
-      <c r="C12" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="K13" s="54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C14" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="D14" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F14" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="K14" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="8" t="s">
+    </row>
+    <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J15" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="K12" s="54" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="10">
-        <v>2035</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="K15" s="54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="K16" s="59" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="K17" s="58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="K18" s="58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="K19" s="58" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="G20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="J20" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="K13" s="53" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C14" s="35" t="s">
+      <c r="K20" s="53"/>
+    </row>
+    <row r="21" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="35" t="s">
+      <c r="D21" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35" t="s">
+      <c r="F21" s="35"/>
+      <c r="G21" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="36" t="s">
+      <c r="K21" s="36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C15" s="35" t="s">
+    <row r="22" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="35" t="s">
+      <c r="D22" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F22" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35" t="s">
+      <c r="G22" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="37" t="s">
+      <c r="K22" s="37" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="35" t="s">
+    <row r="23" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="35" t="s">
+      <c r="D23" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35" t="s">
+      <c r="F23" s="35"/>
+      <c r="G23" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="35" t="s">
+      <c r="K23" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="35" t="s">
+    <row r="24" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="35" t="s">
+      <c r="D24" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35" t="s">
+      <c r="F24" s="35"/>
+      <c r="G24" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="K17" s="35" t="s">
+      <c r="K24" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="35" t="s">
+    <row r="25" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="35" t="s">
+      <c r="D25" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35" t="s">
+      <c r="F25" s="35"/>
+      <c r="G25" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="K18" s="35" t="s">
+      <c r="K25" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="40" t="s">
+    <row r="26" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="40" t="s">
+      <c r="D26" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F26" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40" t="s">
+      <c r="G26" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="K19" s="41" t="s">
+      <c r="K26" s="41" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="K25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="K26" s="19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1881,7 +1922,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>26</v>
@@ -1890,7 +1931,7 @@
         <v>33</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>30</v>
@@ -1903,7 +1944,7 @@
         <v>40</v>
       </c>
       <c r="K27" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1914,7 +1955,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>26</v>
@@ -1923,7 +1964,7 @@
         <v>33</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>30</v>
@@ -1936,7 +1977,7 @@
         <v>40</v>
       </c>
       <c r="K28" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1947,7 +1988,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>26</v>
@@ -1955,7 +1996,9 @@
       <c r="E29" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="18"/>
+      <c r="F29" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="G29" s="14" t="s">
         <v>30</v>
       </c>
@@ -1964,10 +2007,10 @@
       </c>
       <c r="I29" s="17"/>
       <c r="J29" s="17" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="K29" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1978,7 +2021,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>26</v>
@@ -1986,7 +2029,9 @@
       <c r="E30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="18"/>
+      <c r="F30" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="G30" s="14" t="s">
         <v>30</v>
       </c>
@@ -1995,10 +2040,10 @@
       </c>
       <c r="I30" s="17"/>
       <c r="J30" s="17" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="K30" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -2009,7 +2054,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>26</v>
@@ -2017,7 +2062,9 @@
       <c r="E31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="18"/>
+      <c r="F31" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="G31" s="14" t="s">
         <v>30</v>
       </c>
@@ -2026,10 +2073,10 @@
       </c>
       <c r="I31" s="17"/>
       <c r="J31" s="17" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="K31" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -2040,7 +2087,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>26</v>
@@ -2048,9 +2095,7 @@
       <c r="E32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="18" t="s">
-        <v>99</v>
-      </c>
+      <c r="F32" s="18"/>
       <c r="G32" s="14" t="s">
         <v>30</v>
       </c>
@@ -2059,10 +2104,10 @@
       </c>
       <c r="I32" s="17"/>
       <c r="J32" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="K32" s="24" t="s">
-        <v>103</v>
+        <v>75</v>
+      </c>
+      <c r="K32" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -2073,7 +2118,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>26</v>
@@ -2082,7 +2127,7 @@
         <v>33</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G33" s="14" t="s">
         <v>30</v>
@@ -2092,7 +2137,10 @@
       </c>
       <c r="I33" s="17"/>
       <c r="J33" s="17" t="s">
-        <v>72</v>
+        <v>76</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -2103,7 +2151,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>26</v>
@@ -2112,7 +2160,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G34" s="14" t="s">
         <v>30</v>
@@ -2122,119 +2170,347 @@
       </c>
       <c r="I34" s="17"/>
       <c r="J34" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="18"/>
+      <c r="G36" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="K36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="18"/>
+      <c r="G37" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="18"/>
+      <c r="G38" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K39" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="12" t="s">
+      <c r="D42" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F42" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="G35" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="17" t="s">
+      <c r="G42" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="20" t="s">
+    <row r="43" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D36" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="20" t="s">
+      <c r="D43" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F43" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G36" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20" t="s">
+      <c r="G43" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="K36" s="21" t="s">
+      <c r="K43" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C37" s="20" t="s">
+    <row r="44" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="20" t="s">
+      <c r="D44" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F44" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G37" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H37" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20" t="s">
+      <c r="G44" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="K37" s="21" t="s">
+      <c r="K44" s="21" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K14" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="K21" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="K9" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="K19" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K26" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K32" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K26" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="K33" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K39" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
     <hyperlink ref="K7" r:id="rId6" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
-    <hyperlink ref="K13" r:id="rId7" xr:uid="{9DD30DA7-A7AD-43EC-BABA-F91175587CE9}"/>
-    <hyperlink ref="K11" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
-    <hyperlink ref="K12" r:id="rId9" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
+    <hyperlink ref="K14" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
+    <hyperlink ref="K15" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
+    <hyperlink ref="K13" r:id="rId9" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{07D1B2DA-E517-4DD9-B4E8-AE0933FD4973}"/>
+    <hyperlink ref="K12" r:id="rId10" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{4A8E9582-524B-46F3-8A76-0C1F5220D214}"/>
+    <hyperlink ref="K11" r:id="rId11" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{E622471D-8EED-401F-9FFF-3C4854166AD2}"/>
+    <hyperlink ref="K16" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
+    <hyperlink ref="K17" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
+    <hyperlink ref="K18" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
+    <hyperlink ref="K19" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
re-committing the model run log from  9 hours ago
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4D7FDD-06F9-4F13-9CFC-93152AA20A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921BA80F-16F6-457F-A20A-19D5795FE2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="176">
   <si>
     <t>No Project</t>
   </si>
@@ -386,9 +386,6 @@
     <t>https://app.asana.com/0/1201809392759895/1203246561643081/f</t>
   </si>
   <si>
-    <t>Pathways</t>
-  </si>
-  <si>
     <t>Pathway 1b: All-lane tolling + Focus on Affordability</t>
   </si>
   <si>
@@ -446,9 +443,6 @@
     <t>✓ Run pathway 1b with toll calibration</t>
   </si>
   <si>
-    <t>to do</t>
-  </si>
-  <si>
     <t>Run pathway 1b with calibrated tolls</t>
   </si>
   <si>
@@ -458,37 +452,118 @@
     <t>Pathway 1b - run with calibrated tolls</t>
   </si>
   <si>
-    <t>2035_TM152_NGF_NP07_Path3a_01_Toll_189SJ_189OAK</t>
-  </si>
-  <si>
-    <t>Pathway3a</t>
-  </si>
-  <si>
-    <t>Path3a_01_Toll_189SJ_189OAK</t>
-  </si>
-  <si>
-    <t>Deleted</t>
-  </si>
-  <si>
-    <t>2035_TM152_NGF_NP07_Path3a_01_Toll_189SJ_378OAK</t>
-  </si>
-  <si>
-    <t>2035_TM152_NGF_NP07_Path3a_01_Toll_378SJ_189OAK</t>
-  </si>
-  <si>
-    <t>2035_TM152_NGF_NP07_Path3a_01_Toll_378SJ_378OAK</t>
-  </si>
-  <si>
-    <t>Path3a_01_Toll_189SJ_378OAK</t>
-  </si>
-  <si>
-    <t>Path3a_01_Toll_378SJ_189OAK</t>
-  </si>
-  <si>
-    <t>Path3a_01_Toll_378SJ_378OAK</t>
-  </si>
-  <si>
-    <t>https://app.asana.com/0/0/1204016996358516/f</t>
+    <t>2035_TM152_NGF_NP07_Path1b_01_LowestTolls01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_HighestTolls01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_UniformTolls01</t>
+  </si>
+  <si>
+    <t>Pathway 1b - lowest tolls</t>
+  </si>
+  <si>
+    <t>Pathway 1b - highest tolls</t>
+  </si>
+  <si>
+    <t>Pathway 1b - uniform tolls</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_UniformTolls02</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_HighestTolls02</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1b_01_LowestTolls02</t>
+  </si>
+  <si>
+    <t>Pathway 1b</t>
+  </si>
+  <si>
+    <t>Pathway 2b</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path2b_wP1bStaticTolls_01</t>
+  </si>
+  <si>
+    <t>Pathway 2b - with P1b simple tolls</t>
+  </si>
+  <si>
+    <t>Pathway 1a</t>
+  </si>
+  <si>
+    <t>Pathway 3b</t>
+  </si>
+  <si>
+    <t>Pathway 3a</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path3b_02</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path3a_02</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1a_01_MinToll</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1a_02_MinToll</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1a_03_MinToll</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1a_04_MinToll</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1a_05_MinToll</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1a_05_TollCalibration01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path1a_05_wP1bToll</t>
+  </si>
+  <si>
+    <t>Pathway 1a - with P1b tolls</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P1a_AllLaneTolling_ImproveTransit_05</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P1a_AllLaneTolling_ImproveTransit_01</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P1a_AllLaneTolling_ImproveTransit_02</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P1a_AllLaneTolling_ImproveTransit_03</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P1a_AllLaneTolling_ImproveTransit_04</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P2b_AllLaneTollingPlusArterials_Affordable_03</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P3b_3Cordons_Affordable_01</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P3a_3Cordons_ImproveTransit_01</t>
+  </si>
+  <si>
+    <t>lowest tolls - wrong parking costs</t>
+  </si>
+  <si>
+    <t>highest tolls - wrong parking costs</t>
+  </si>
+  <si>
+    <t>uniform tolls - wrong parking costs</t>
   </si>
 </sst>
 </file>
@@ -557,7 +632,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,6 +672,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,7 +727,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -741,17 +822,25 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1106,16 +1195,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -1455,7 +1543,7 @@
         <v>2035</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="48" t="s">
         <v>26</v>
@@ -1475,7 +1563,7 @@
         <v>113</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -1486,7 +1574,7 @@
         <v>2035</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="48" t="s">
         <v>26</v>
@@ -1495,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G12" s="48" t="s">
         <v>30</v>
@@ -1508,7 +1596,7 @@
         <v>113</v>
       </c>
       <c r="K12" s="54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -1519,7 +1607,7 @@
         <v>2035</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="48" t="s">
         <v>26</v>
@@ -1528,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G13" s="48" t="s">
         <v>30</v>
@@ -1541,7 +1629,7 @@
         <v>113</v>
       </c>
       <c r="K13" s="54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
@@ -1552,7 +1640,7 @@
         <v>2035</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="48" t="s">
         <v>26</v>
@@ -1561,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G14" s="48" t="s">
         <v>30</v>
@@ -1574,7 +1662,7 @@
         <v>113</v>
       </c>
       <c r="K14" s="54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1585,7 +1673,7 @@
         <v>2035</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>26</v>
@@ -1594,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>30</v>
@@ -1609,1083 +1697,1445 @@
         <v>113</v>
       </c>
       <c r="K15" s="54" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="56">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="57" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="74">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="K16" s="21"/>
+    </row>
+    <row r="17" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="74">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="70" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="K17" s="21"/>
+    </row>
+    <row r="18" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="74">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="74">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="K19" s="21"/>
+    </row>
+    <row r="20" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="74">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="K20" s="21"/>
+    </row>
+    <row r="21" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="74">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="K21" s="21"/>
+    </row>
+    <row r="22" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="74">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="70" t="s">
+        <v>163</v>
+      </c>
+      <c r="G22" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="K22" s="21"/>
+    </row>
+    <row r="23" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="57" t="s">
+    </row>
+    <row r="24" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K24" s="58" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K25" s="58" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K26" s="58" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F27" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="K16" s="59" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="56">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="D17" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="K17" s="58" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="56">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="57" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="K18" s="58" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="56">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="57" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="57" t="s">
+      <c r="G27" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K27" s="58"/>
+    </row>
+    <row r="28" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="G28" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K28" s="58"/>
+    </row>
+    <row r="29" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="G19" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="57" t="s">
+      <c r="D29" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K29" s="58"/>
+    </row>
+    <row r="30" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="61">
+        <v>2035</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="G30" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="60"/>
+      <c r="J30" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K30" s="62"/>
+    </row>
+    <row r="31" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="K19" s="58" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="10">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="11" t="s">
+      <c r="J31" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="K20" s="53"/>
-    </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="35" t="s">
+      <c r="K31" s="58"/>
+    </row>
+    <row r="32" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="K32" s="58"/>
+    </row>
+    <row r="33" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K33" s="53"/>
+    </row>
+    <row r="34" spans="1:11" s="69" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="65">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="F34" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="K34" s="68"/>
+    </row>
+    <row r="35" spans="1:11" s="73" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="J35" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="K35" s="49"/>
+    </row>
+    <row r="36" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" s="60" t="s">
+        <v>164</v>
+      </c>
+      <c r="J36" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="K36" s="62"/>
+    </row>
+    <row r="37" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="35" t="s">
+      <c r="D37" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35" t="s">
+      <c r="F37" s="35"/>
+      <c r="G37" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="K21" s="36" t="s">
+      <c r="K37" s="36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="35" t="s">
+    <row r="38" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="35" t="s">
+      <c r="D38" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F38" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35" t="s">
+      <c r="G38" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="K22" s="37" t="s">
+      <c r="K38" s="37" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="35" t="s">
+    <row r="39" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="35" t="s">
+      <c r="D39" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35" t="s">
+      <c r="F39" s="35"/>
+      <c r="G39" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="K23" s="35" t="s">
+      <c r="K39" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="35" t="s">
+    <row r="40" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="35" t="s">
+      <c r="D40" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35" t="s">
+      <c r="F40" s="35"/>
+      <c r="G40" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="K24" s="35" t="s">
+      <c r="K40" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="35" t="s">
+    <row r="41" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="35" t="s">
+      <c r="D41" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35" t="s">
+      <c r="F41" s="35"/>
+      <c r="G41" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="K25" s="35" t="s">
+      <c r="K41" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="40" t="s">
+    <row r="42" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="40" t="s">
+      <c r="D42" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F42" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="G26" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40" t="s">
+      <c r="G42" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="K26" s="41" t="s">
+      <c r="K42" s="41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="17" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="18" t="s">
+      <c r="D43" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F43" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="G27" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17" t="s">
+      <c r="G43" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C28" s="17" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="18" t="s">
+      <c r="D44" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F44" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="G28" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17" t="s">
+      <c r="G44" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="17" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="18" t="s">
+      <c r="D45" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F45" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17" t="s">
+      <c r="G45" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C30" s="17" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="18" t="s">
+      <c r="D46" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F46" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="G30" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17" t="s">
+      <c r="G46" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K46" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="17" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C47" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="18" t="s">
+      <c r="D47" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F47" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="G31" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17" t="s">
+      <c r="G47" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="17" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="18" t="s">
+      <c r="D48" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17" t="s">
+      <c r="F48" s="18"/>
+      <c r="G48" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K48" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="17" t="s">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C49" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="18" t="s">
+      <c r="D49" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F49" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17" t="s">
+      <c r="G49" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="K33" s="19" t="s">
+      <c r="K49" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="17" t="s">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="18" t="s">
+      <c r="D50" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F50" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G34" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17" t="s">
+      <c r="G50" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="17" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="18" t="s">
+      <c r="D51" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F51" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="G35" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17" t="s">
+      <c r="G51" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="17" t="s">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="18" t="s">
+      <c r="D52" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="18"/>
-      <c r="G36" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17" t="s">
+      <c r="F52" s="18"/>
+      <c r="G52" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C37" s="17" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="18" t="s">
+      <c r="D53" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17" t="s">
+      <c r="F53" s="18"/>
+      <c r="G53" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K53" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="17" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="18" t="s">
+      <c r="D54" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="18"/>
-      <c r="G38" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17" t="s">
+      <c r="F54" s="18"/>
+      <c r="G54" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="17" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C55" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39" s="18" t="s">
+      <c r="D55" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="F55" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="G39" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17" t="s">
+      <c r="G55" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K39" s="24" t="s">
+      <c r="K55" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="17" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" s="18" t="s">
+      <c r="D56" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F56" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G40" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17" t="s">
+      <c r="G56" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="17" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D41" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E41" s="18" t="s">
+      <c r="D57" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F57" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G41" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17" t="s">
+      <c r="G57" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C42" s="1" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D42" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E42" s="12" t="s">
+      <c r="D58" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F58" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="G42" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1" t="s">
+      <c r="G58" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I58" s="1"/>
+      <c r="J58" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C43" s="20" t="s">
+    <row r="59" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E43" s="20" t="s">
+      <c r="D59" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F59" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G43" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20" t="s">
+      <c r="G59" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="K43" s="21" t="s">
+      <c r="K59" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="60" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="60" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="61">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="62" t="s">
+    <row r="60" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="E44" s="62" t="s">
+      <c r="D60" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F44" s="62" t="s">
+      <c r="F60" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G44" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="H44" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="I44" s="62"/>
-      <c r="J44" s="62" t="s">
+      <c r="G60" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="K44" s="63" t="s">
+      <c r="K60" s="21" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="G45" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="J45" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="K45" s="33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="D46" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="G46" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H46" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="J46" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="K46" s="33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E47" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="F47" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="G47" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="J47" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="K47" s="33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="D48" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E48" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="G48" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H48" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="J48" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="K48" s="33" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K21" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="K37" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="K9" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="K26" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K33" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K39" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K42" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="K49" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K55" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
     <hyperlink ref="K7" r:id="rId6" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
     <hyperlink ref="K14" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
     <hyperlink ref="K15" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
     <hyperlink ref="K13" r:id="rId9" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{07D1B2DA-E517-4DD9-B4E8-AE0933FD4973}"/>
     <hyperlink ref="K12" r:id="rId10" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{4A8E9582-524B-46F3-8A76-0C1F5220D214}"/>
     <hyperlink ref="K11" r:id="rId11" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{E622471D-8EED-401F-9FFF-3C4854166AD2}"/>
-    <hyperlink ref="K16" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
-    <hyperlink ref="K17" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
-    <hyperlink ref="K18" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
-    <hyperlink ref="K19" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
+    <hyperlink ref="K23" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
+    <hyperlink ref="K24" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
+    <hyperlink ref="K25" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
+    <hyperlink ref="K26" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>

<commit_message>
Add pathway 3a_01 model runs
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921BA80F-16F6-457F-A20A-19D5795FE2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB52B81D-2C19-4AD9-A4C2-957268BAE734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="186">
   <si>
     <t>No Project</t>
   </si>
@@ -564,6 +564,36 @@
   </si>
   <si>
     <t>uniform tolls - wrong parking costs</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path3a_01_Toll_189SJ_189OAK</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path3a_01_Toll_189SJ_378OAK</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path3a_01_Toll_378SJ_189OAK</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path3a_01_Toll_378SJ_378OAK</t>
+  </si>
+  <si>
+    <t>Path3a_01_Toll_189SJ_189OAK</t>
+  </si>
+  <si>
+    <t>Path3a_01_Toll_189SJ_378OAK</t>
+  </si>
+  <si>
+    <t>Path3a_01_Toll_378SJ_189OAK</t>
+  </si>
+  <si>
+    <t>Path3a_01_Toll_378SJ_378OAK</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1204016996358516/f</t>
   </si>
 </sst>
 </file>
@@ -727,7 +757,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -822,25 +852,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1195,11 +1215,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1700,207 +1720,207 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="74">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="70" t="s">
+    <row r="16" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="20" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70" t="s">
+      <c r="F16" s="20"/>
+      <c r="G16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20" t="s">
         <v>166</v>
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="74">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="70" t="s">
+    <row r="17" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="D17" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="70" t="s">
+      <c r="D17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70" t="s">
+      <c r="F17" s="20"/>
+      <c r="G17" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20" t="s">
         <v>167</v>
       </c>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="74">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="70" t="s">
+    <row r="18" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="D18" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="70" t="s">
+      <c r="D18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70" t="s">
+      <c r="F18" s="20"/>
+      <c r="G18" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20" t="s">
         <v>168</v>
       </c>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="74">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="70" t="s">
+    <row r="19" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D19" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="70" t="s">
+      <c r="D19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="70"/>
-      <c r="J19" s="70" t="s">
+      <c r="F19" s="20"/>
+      <c r="G19" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20" t="s">
         <v>169</v>
       </c>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="74">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="70" t="s">
+    <row r="20" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="D20" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="70" t="s">
+      <c r="D20" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="70"/>
-      <c r="J20" s="70" t="s">
+      <c r="F20" s="20"/>
+      <c r="G20" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20" t="s">
         <v>165</v>
       </c>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="74">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="70" t="s">
+    <row r="21" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D21" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="70" t="s">
+      <c r="D21" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="70"/>
-      <c r="J21" s="70" t="s">
+      <c r="F21" s="20"/>
+      <c r="G21" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20" t="s">
         <v>165</v>
       </c>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="74">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="70" t="s">
+    <row r="22" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="D22" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="70" t="s">
+      <c r="D22" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="F22" s="70" t="s">
+      <c r="F22" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="G22" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70" t="s">
+      <c r="G22" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20" t="s">
         <v>165</v>
       </c>
       <c r="K22" s="21"/>
@@ -2126,17 +2146,17 @@
       </c>
       <c r="K29" s="58"/>
     </row>
-    <row r="30" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="61">
-        <v>2035</v>
-      </c>
-      <c r="C30" s="60" t="s">
+    <row r="30" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C30" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="57" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="57" t="s">
@@ -2151,11 +2171,11 @@
       <c r="H30" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="60"/>
+      <c r="I30" s="57"/>
       <c r="J30" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="K30" s="62"/>
+      <c r="K30" s="60"/>
     </row>
     <row r="31" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="55" t="s">
@@ -2256,47 +2276,47 @@
       </c>
       <c r="K33" s="53"/>
     </row>
-    <row r="34" spans="1:11" s="69" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="66" t="s">
+    <row r="34" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="D34" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="67" t="s">
+      <c r="D34" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="F34" s="67" t="s">
+      <c r="F34" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="G34" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="66" t="s">
+      <c r="G34" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="J34" s="67" t="s">
+      <c r="J34" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="K34" s="68"/>
-    </row>
-    <row r="35" spans="1:11" s="73" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K34" s="64"/>
+    </row>
+    <row r="35" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="46" t="s">
         <v>43</v>
       </c>
       <c r="B35" s="47">
         <v>2035</v>
       </c>
-      <c r="C35" s="72" t="s">
+      <c r="C35" s="48" t="s">
         <v>155</v>
       </c>
       <c r="D35" s="48" t="s">
@@ -2312,7 +2332,7 @@
       <c r="H35" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="72" t="s">
+      <c r="I35" s="48" t="s">
         <v>164</v>
       </c>
       <c r="J35" s="48" t="s">
@@ -2320,14 +2340,14 @@
       </c>
       <c r="K35" s="49"/>
     </row>
-    <row r="36" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="55" t="s">
         <v>43</v>
       </c>
       <c r="B36" s="56">
         <v>2035</v>
       </c>
-      <c r="C36" s="60" t="s">
+      <c r="C36" s="57" t="s">
         <v>154</v>
       </c>
       <c r="D36" s="57" t="s">
@@ -2343,13 +2363,13 @@
       <c r="H36" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="60" t="s">
+      <c r="I36" s="57" t="s">
         <v>164</v>
       </c>
       <c r="J36" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="K36" s="62"/>
+      <c r="K36" s="60"/>
     </row>
     <row r="37" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="33" t="s">
@@ -3116,6 +3136,138 @@
       </c>
       <c r="K60" s="21" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="66">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="65" t="s">
+        <v>176</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I61" s="17"/>
+      <c r="J61" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K61" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="66">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K62" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" s="66">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="65" t="s">
+        <v>178</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="66">
+        <v>2035</v>
+      </c>
+      <c r="C64" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K64" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ModeRuns.xlsx for pathway runs
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C5F60C-D2CC-462A-B43C-A67E03C633BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC831B1-25F6-459B-8B9A-0650451A60A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$I$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$64</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1214,8 +1214,8 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="A7:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3273,6 +3273,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K41" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>

</xml_diff>

<commit_message>
added the initial run for pathway 4, also added the blueprint 2035 run
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC831B1-25F6-459B-8B9A-0650451A60A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF56F1F-CE21-4D87-B37D-B5D07FA0A5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="188">
   <si>
     <t>No Project</t>
   </si>
@@ -77,15 +77,6 @@
     <t>FinalBlueprint</t>
   </si>
   <si>
-    <t>"EIR runs\Baseline Large (s25) runs\NP_v8"</t>
-  </si>
-  <si>
-    <t>run314</t>
-  </si>
-  <si>
-    <t>2035_TM152_FBP_NoProject_24</t>
-  </si>
-  <si>
     <t>2015_TM152_IPA_17</t>
   </si>
   <si>
@@ -218,9 +209,6 @@
     <t>TM1_2015_Base_Network</t>
   </si>
   <si>
-    <t>BlueprintNetworks_64</t>
-  </si>
-  <si>
     <t>existing_conditions\net_2035_NextGenFwy</t>
   </si>
   <si>
@@ -386,9 +374,6 @@
     <t>https://app.asana.com/0/1201809392759895/1203246561643081/f</t>
   </si>
   <si>
-    <t>Pathway 1b: All-lane tolling + Focus on Affordability</t>
-  </si>
-  <si>
     <t>NGF_Networks_P1b_AllLaneTolling_Affordable_01</t>
   </si>
   <si>
@@ -594,6 +579,27 @@
   </si>
   <si>
     <t>2035_TM152_NGF_NP07_Path1b_01_SimpleToll01</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP07_Path4_01</t>
+  </si>
+  <si>
+    <t>Pathway 4</t>
+  </si>
+  <si>
+    <t>Pathway 4 - No New Pricing</t>
+  </si>
+  <si>
+    <t>Pathway 1b - All-lane tolling + Focus on Affordability</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P4_NoNewPricing_01</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1201809392759895/1204133370132350/f</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_24</t>
   </si>
 </sst>
 </file>
@@ -757,7 +763,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -851,14 +857,38 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1211,15 +1241,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="A7:XFD38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -1246,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>10</v>
@@ -1258,10 +1289,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -1272,1306 +1303,1304 @@
         <v>2015</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I2" s="27"/>
       <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="51">
         <v>2015</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" s="51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K3" s="50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" s="51">
         <v>2015</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" s="51">
         <v>2015</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K5" s="50" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="51">
         <v>2015</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H6" s="51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K6" s="50" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="51">
         <v>2015</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K7" s="52" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B8" s="31">
         <v>2035</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32" t="s">
-        <v>60</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" s="43">
         <v>2035</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" s="44" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H9" s="43" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="44" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K9" s="45" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B10" s="47">
         <v>2035</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" s="48" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="48" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H10" s="47" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I10" s="48"/>
       <c r="J10" s="48" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K10" s="49" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" s="47">
         <v>2035</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="48" t="s">
         <v>0</v>
       </c>
       <c r="F11" s="48"/>
       <c r="G11" s="48" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H11" s="47" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I11" s="48"/>
       <c r="J11" s="48" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B12" s="47">
         <v>2035</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E12" s="48" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G12" s="48" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H12" s="47" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I12" s="48"/>
       <c r="J12" s="48" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K12" s="54" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" s="47">
         <v>2035</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" s="48" t="s">
         <v>0</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G13" s="48" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H13" s="47" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I13" s="48"/>
       <c r="J13" s="48" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K13" s="54" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="47">
         <v>2035</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E14" s="48" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G14" s="48" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H14" s="47" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I14" s="48"/>
       <c r="J14" s="48" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K14" s="54" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7">
         <v>2035</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K15" s="54" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="K16" s="60"/>
+    </row>
+    <row r="17" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="K17" s="60"/>
+    </row>
+    <row r="18" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="K18" s="60"/>
+    </row>
+    <row r="19" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="K19" s="60"/>
+    </row>
+    <row r="20" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="K20" s="60"/>
+    </row>
+    <row r="21" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="20" t="s">
+      <c r="D21" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="K21" s="60"/>
+    </row>
+    <row r="22" spans="1:11" s="64" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="65">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C18" s="20" t="s">
+      <c r="D22" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="K18" s="21"/>
-    </row>
-    <row r="19" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="20" t="s">
+      <c r="G22" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="K20" s="21"/>
-    </row>
-    <row r="21" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="K21" s="21"/>
-    </row>
-    <row r="22" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="K22" s="21"/>
+      <c r="K22" s="67"/>
     </row>
     <row r="23" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B23" s="56">
         <v>2035</v>
       </c>
       <c r="C23" s="57" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D23" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F23" s="57"/>
       <c r="G23" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H23" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I23" s="57"/>
       <c r="J23" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K23" s="59" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B24" s="56">
         <v>2035</v>
       </c>
       <c r="C24" s="57" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D24" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E24" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F24" s="57"/>
       <c r="G24" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H24" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I24" s="57"/>
       <c r="J24" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K24" s="58" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" s="56">
         <v>2035</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D25" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E25" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F25" s="57"/>
       <c r="G25" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H25" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I25" s="57"/>
       <c r="J25" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K25" s="58" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B26" s="56">
         <v>2035</v>
       </c>
       <c r="C26" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="57" t="s">
-        <v>136</v>
-      </c>
       <c r="G26" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H26" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I26" s="57"/>
       <c r="J26" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K26" s="58" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B27" s="56">
         <v>2035</v>
       </c>
       <c r="C27" s="57" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E27" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F27" s="57" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="G27" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H27" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I27" s="57" t="s">
         <v>9</v>
       </c>
       <c r="J27" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K27" s="58"/>
     </row>
     <row r="28" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B28" s="56">
         <v>2035</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D28" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E28" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F28" s="57" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G28" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H28" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I28" s="57"/>
       <c r="J28" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K28" s="58"/>
     </row>
     <row r="29" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B29" s="56">
         <v>2035</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D29" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E29" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F29" s="57" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G29" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H29" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I29" s="57"/>
       <c r="J29" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K29" s="58"/>
     </row>
     <row r="30" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B30" s="56">
         <v>2035</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D30" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E30" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F30" s="57" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G30" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H30" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I30" s="57"/>
       <c r="J30" s="57" t="s">
-        <v>117</v>
-      </c>
-      <c r="K30" s="60"/>
+        <v>112</v>
+      </c>
+      <c r="K30" s="59"/>
     </row>
     <row r="31" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31" s="56">
         <v>2035</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D31" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E31" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F31" s="57" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G31" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H31" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I31" s="57" t="s">
         <v>9</v>
       </c>
       <c r="J31" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K31" s="58"/>
     </row>
     <row r="32" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B32" s="56">
         <v>2035</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D32" s="57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E32" s="57" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F32" s="57" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G32" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H32" s="56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I32" s="57" t="s">
         <v>9</v>
       </c>
       <c r="J32" s="57" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K32" s="58"/>
     </row>
     <row r="33" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B33" s="10">
         <v>2035</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I33" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K33" s="53"/>
     </row>
-    <row r="34" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="62">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="63" t="s">
+    <row r="34" spans="1:11" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="69">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="70" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="G34" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="K34" s="71"/>
+    </row>
+    <row r="35" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="43">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H35" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="K35" s="45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="73">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="F36" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="J36" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="K36" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="73">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="F37" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="K37" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="73">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="F38" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="G38" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="J38" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="K38" s="49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="7">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K39" s="75"/>
+    </row>
+    <row r="40" spans="1:11" s="76" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="77">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="D34" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="63" t="s">
-        <v>147</v>
-      </c>
-      <c r="F34" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="G34" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34" s="63" t="s">
-        <v>169</v>
-      </c>
-      <c r="K34" s="64"/>
-    </row>
-    <row r="35" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="D35" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="F35" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="G35" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H35" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="I35" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="J35" s="48" t="s">
+      <c r="D40" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="H40" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="78"/>
+      <c r="J40" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="K40" s="79"/>
+    </row>
+    <row r="41" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="31">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="F41" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="K35" s="49" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="D36" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="F36" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="G36" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="I36" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="K36" s="49" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C37" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="D37" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="F37" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="G37" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H37" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="I37" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="J37" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="K37" s="49" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="D38" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="F38" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="G38" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="I38" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="K38" s="49" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="I39" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="J39" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="K39" s="49"/>
-    </row>
-    <row r="40" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="56">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="57" t="s">
-        <v>153</v>
-      </c>
-      <c r="D40" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" s="57" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="I40" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="J40" s="57" t="s">
-        <v>170</v>
-      </c>
-      <c r="K40" s="60"/>
-    </row>
-    <row r="41" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E41" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K41" s="36" t="s">
-        <v>38</v>
+      <c r="G41" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="K41" s="80" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B42" s="34">
         <v>2035</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="35" t="s">
-        <v>80</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F42" s="35"/>
       <c r="G42" s="35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H42" s="34" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I42" s="35"/>
       <c r="J42" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="K42" s="37" t="s">
-        <v>69</v>
+        <v>37</v>
+      </c>
+      <c r="K42" s="36" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B43" s="34">
         <v>2035</v>
@@ -2580,707 +2609,739 @@
         <v>64</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="35"/>
+        <v>38</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>76</v>
+      </c>
       <c r="G43" s="35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H43" s="34" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I43" s="35"/>
       <c r="J43" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="K43" s="35" t="s">
-        <v>56</v>
+        <v>66</v>
+      </c>
+      <c r="K43" s="37" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B44" s="34">
         <v>2035</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E44" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H44" s="34" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I44" s="35"/>
       <c r="J44" s="35" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K44" s="35" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B45" s="34">
         <v>2035</v>
       </c>
       <c r="C45" s="35" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H45" s="34" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I45" s="35"/>
       <c r="J45" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="K45" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C47" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="K45" s="35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="H46" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="K46" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K47" t="s">
-        <v>32</v>
+      <c r="D47" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="H47" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="K47" s="41" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B48" s="13">
         <v>2035</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I48" s="17"/>
       <c r="J48" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K48" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C49" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>47</v>
-      </c>
       <c r="D49" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K49" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B50" s="13">
         <v>2035</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I50" s="17"/>
       <c r="J50" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K50" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B51" s="13">
         <v>2035</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I51" s="17"/>
       <c r="J51" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K51" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B52" s="13">
         <v>2035</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F52" s="18"/>
+        <v>30</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="G52" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I52" s="17"/>
       <c r="J52" s="17" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="K52" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B53" s="13">
         <v>2035</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F53" s="18" t="s">
-        <v>89</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F53" s="18"/>
       <c r="G53" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I53" s="17"/>
       <c r="J53" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="K53" s="19" t="s">
-        <v>53</v>
+        <v>71</v>
+      </c>
+      <c r="K53" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B54" s="13">
         <v>2035</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I54" s="17"/>
       <c r="J54" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K54" t="s">
-        <v>54</v>
+        <v>72</v>
+      </c>
+      <c r="K54" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B55" s="13">
         <v>2035</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I55" s="17"/>
       <c r="J55" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K55" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B56" s="13">
         <v>2035</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F56" s="18"/>
+        <v>30</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="G56" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I56" s="17"/>
       <c r="J56" s="17" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="K56" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B57" s="13">
         <v>2035</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F57" s="18"/>
       <c r="G57" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I57" s="17"/>
       <c r="J57" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K57" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B58" s="13">
         <v>2035</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F58" s="18"/>
       <c r="G58" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I58" s="17"/>
       <c r="J58" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K58" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B59" s="13">
         <v>2035</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F59" s="18" t="s">
-        <v>99</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F59" s="18"/>
       <c r="G59" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I59" s="17"/>
       <c r="J59" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="K59" s="24" t="s">
-        <v>103</v>
+        <v>68</v>
+      </c>
+      <c r="K59" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B60" s="13">
         <v>2035</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I60" s="17"/>
       <c r="J60" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="K60" s="24" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B61" s="13">
         <v>2035</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F61" s="18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I61" s="17"/>
       <c r="J61" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B62" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D62" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F62" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="G62" s="16" t="s">
+      <c r="A62" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H62" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I62" s="1"/>
+      <c r="F62" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I62" s="17"/>
       <c r="J62" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" s="23">
-        <v>2035</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E63" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F63" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="G63" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H63" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="K63" s="21" t="s">
-        <v>108</v>
+      <c r="F63" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I63" s="1"/>
+      <c r="J63" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B64" s="23">
         <v>2035</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H64" s="23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I64" s="20"/>
       <c r="J64" s="20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K64" s="21" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H65" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="K65" s="21" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K41" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="K42" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
     <hyperlink ref="K9" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="K46" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K53" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K59" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K47" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="K54" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K60" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
     <hyperlink ref="K7" r:id="rId6" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
     <hyperlink ref="K14" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
     <hyperlink ref="K15" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
@@ -3291,8 +3352,9 @@
     <hyperlink ref="K24" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
     <hyperlink ref="K25" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
     <hyperlink ref="K26" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
+    <hyperlink ref="K41" r:id="rId16" xr:uid="{C5D42A4A-7D1E-4E61-A6D8-57E8258064CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add pathway 4 to ModelRuns.xlsx
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FCF072-4F0B-4F00-8FEB-4A6FFD26EE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A66414-759A-4269-A82D-459EEFDFEE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="198">
   <si>
     <t>No Project</t>
   </si>
@@ -510,9 +510,6 @@
   </si>
   <si>
     <t>Pathway 1a - with P1b tolls</t>
-  </si>
-  <si>
-    <t>in progress</t>
   </si>
   <si>
     <t>NGF_Networks_P1a_AllLaneTolling_ImproveTransit_05</t>
@@ -796,7 +793,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -900,16 +897,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1264,9 +1251,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1513,7 +1500,7 @@
         <v>2035</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>12</v>
@@ -1789,7 +1776,7 @@
       </c>
       <c r="I16" s="17"/>
       <c r="J16" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K16" s="56"/>
     </row>
@@ -1818,7 +1805,7 @@
       </c>
       <c r="I17" s="17"/>
       <c r="J17" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K17" s="56"/>
     </row>
@@ -1847,7 +1834,7 @@
       </c>
       <c r="I18" s="17"/>
       <c r="J18" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K18" s="56"/>
     </row>
@@ -1876,7 +1863,7 @@
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K19" s="56"/>
     </row>
@@ -1905,7 +1892,7 @@
       </c>
       <c r="I20" s="17"/>
       <c r="J20" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K20" s="56"/>
     </row>
@@ -1934,7 +1921,7 @@
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K21" s="56"/>
     </row>
@@ -1967,7 +1954,7 @@
         <v>9</v>
       </c>
       <c r="J22" s="59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K22" s="60"/>
     </row>
@@ -2105,7 +2092,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D27" s="53" t="s">
         <v>23</v>
@@ -2114,7 +2101,7 @@
         <v>141</v>
       </c>
       <c r="F27" s="53" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G27" s="53" t="s">
         <v>27</v>
@@ -2147,7 +2134,7 @@
         <v>141</v>
       </c>
       <c r="F28" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G28" s="53" t="s">
         <v>27</v>
@@ -2178,7 +2165,7 @@
         <v>141</v>
       </c>
       <c r="F29" s="53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G29" s="53" t="s">
         <v>27</v>
@@ -2209,7 +2196,7 @@
         <v>141</v>
       </c>
       <c r="F30" s="53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G30" s="53" t="s">
         <v>27</v>
@@ -2262,7 +2249,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D32" s="53" t="s">
         <v>23</v>
@@ -2283,10 +2270,10 @@
         <v>9</v>
       </c>
       <c r="J32" s="53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K32" s="54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
@@ -2322,33 +2309,33 @@
       </c>
       <c r="K33" s="54"/>
     </row>
-    <row r="34" spans="1:11" s="67" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="68">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="69" t="s">
+    <row r="34" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="52">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="69" t="s">
+      <c r="D34" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="G34" s="69" t="s">
-        <v>27</v>
-      </c>
-      <c r="H34" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69" t="s">
+      <c r="G34" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53" t="s">
         <v>112</v>
       </c>
       <c r="K34" s="55"/>
@@ -2361,7 +2348,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D35" s="53" t="s">
         <v>23</v>
@@ -2382,10 +2369,10 @@
         <v>9</v>
       </c>
       <c r="J35" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="K35" s="55" t="s">
         <v>195</v>
-      </c>
-      <c r="K35" s="55" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.3">
@@ -2417,7 +2404,7 @@
         <v>9</v>
       </c>
       <c r="J36" s="63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K36" s="64"/>
     </row>
@@ -2429,7 +2416,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D37" s="41" t="s">
         <v>23</v>
@@ -2438,7 +2425,7 @@
         <v>147</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G37" s="41" t="s">
         <v>27</v>
@@ -2448,10 +2435,10 @@
       </c>
       <c r="I37" s="41"/>
       <c r="J37" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="K37" s="42" t="s">
         <v>178</v>
-      </c>
-      <c r="K37" s="42" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.3">
@@ -2462,7 +2449,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>23</v>
@@ -2471,7 +2458,7 @@
         <v>147</v>
       </c>
       <c r="F38" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G38" s="45" t="s">
         <v>27</v>
@@ -2481,10 +2468,10 @@
       </c>
       <c r="I38" s="45"/>
       <c r="J38" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="K38" s="46" t="s">
         <v>178</v>
-      </c>
-      <c r="K38" s="46" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.3">
@@ -2495,7 +2482,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>23</v>
@@ -2504,7 +2491,7 @@
         <v>147</v>
       </c>
       <c r="F39" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G39" s="45" t="s">
         <v>27</v>
@@ -2514,10 +2501,10 @@
       </c>
       <c r="I39" s="45"/>
       <c r="J39" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="K39" s="46" t="s">
         <v>178</v>
-      </c>
-      <c r="K39" s="46" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.3">
@@ -2528,7 +2515,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>23</v>
@@ -2537,7 +2524,7 @@
         <v>147</v>
       </c>
       <c r="F40" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G40" s="45" t="s">
         <v>27</v>
@@ -2547,40 +2534,40 @@
       </c>
       <c r="I40" s="45"/>
       <c r="J40" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="K40" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="K40" s="46" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" s="70" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="71">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="72" t="s">
+    </row>
+    <row r="41" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="44">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="72" t="s">
+      <c r="D41" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="F41" s="72" t="s">
+      <c r="F41" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="72"/>
-      <c r="J41" s="72" t="s">
-        <v>166</v>
+      <c r="G41" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="H41" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45" t="s">
+        <v>165</v>
       </c>
       <c r="K41" s="46"/>
     </row>
@@ -2592,7 +2579,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>23</v>
@@ -2613,40 +2600,40 @@
         <v>9</v>
       </c>
       <c r="J42" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="K42" s="65" t="s">
         <v>192</v>
       </c>
-      <c r="K42" s="65" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="67" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="68">
-        <v>2035</v>
-      </c>
-      <c r="C43" s="69" t="s">
+    </row>
+    <row r="43" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="52">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="D43" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="E43" s="69" t="s">
+      <c r="D43" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="F43" s="69" t="s">
+      <c r="F43" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="G43" s="69" t="s">
-        <v>27</v>
-      </c>
-      <c r="H43" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" s="69"/>
-      <c r="J43" s="69" t="s">
-        <v>165</v>
+      <c r="G43" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="H43" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53" t="s">
+        <v>164</v>
       </c>
       <c r="K43" s="55"/>
     </row>
@@ -2658,7 +2645,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D44" s="53" t="s">
         <v>23</v>
@@ -2679,10 +2666,10 @@
         <v>9</v>
       </c>
       <c r="J44" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="K44" s="55" t="s">
         <v>189</v>
-      </c>
-      <c r="K44" s="55" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.3">
@@ -2693,17 +2680,17 @@
         <v>2035</v>
       </c>
       <c r="C45" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="D45" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="29" t="s">
+      <c r="F45" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="F45" s="29" t="s">
-        <v>183</v>
-      </c>
       <c r="G45" s="29" t="s">
         <v>27</v>
       </c>
@@ -2711,13 +2698,13 @@
         <v>28</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>158</v>
+        <v>9</v>
       </c>
       <c r="J45" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="K45" s="66" t="s">
         <v>185</v>
-      </c>
-      <c r="K45" s="66" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
making the short name unique
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDD3594-9F49-4647-99EE-343FE0B7A32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5777868-01C2-4C33-95FE-DF88A01C61C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="210">
   <si>
     <t>No Project</t>
   </si>
@@ -443,15 +443,6 @@
     <t>2035_TM152_NGF_NP07_Path1b_01_UniformTolls01</t>
   </si>
   <si>
-    <t>Pathway 1b - lowest tolls</t>
-  </si>
-  <si>
-    <t>Pathway 1b - highest tolls</t>
-  </si>
-  <si>
-    <t>Pathway 1b - uniform tolls</t>
-  </si>
-  <si>
     <t>2035_TM152_NGF_NP07_Path1b_01_UniformTolls02</t>
   </si>
   <si>
@@ -660,6 +651,21 @@
   </si>
   <si>
     <t>✓ Rerun Pathway 3a with Vision Zero arterial speed fix + Transit Prioity Cordon</t>
+  </si>
+  <si>
+    <t>Pathway 1b - lowest tolls (before VZ fix)</t>
+  </si>
+  <si>
+    <t>Pathway 1b - lowest tolls (with VZ fix #1)</t>
+  </si>
+  <si>
+    <t>Pathway 1b - highest tolls (before VZ fix)</t>
+  </si>
+  <si>
+    <t>Pathway 1b - uniform tolls (before VZ fix)</t>
+  </si>
+  <si>
+    <t>Pathway 1b - uniform tolls (with VZ fix #1)</t>
   </si>
 </sst>
 </file>
@@ -794,65 +800,64 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1209,24 +1214,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.796875" style="34"/>
-    <col min="3" max="3" width="64" style="34" customWidth="1"/>
-    <col min="4" max="4" width="15.296875" style="34" customWidth="1"/>
-    <col min="5" max="5" width="15" style="34" customWidth="1"/>
-    <col min="6" max="6" width="42" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.69921875" style="34" customWidth="1"/>
-    <col min="8" max="8" width="15" style="37" customWidth="1"/>
-    <col min="9" max="9" width="8.796875" style="34"/>
-    <col min="10" max="10" width="47.3984375" style="34" customWidth="1"/>
-    <col min="11" max="16384" width="8.796875" style="34"/>
+    <col min="1" max="1" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64" customWidth="1"/>
+    <col min="4" max="4" width="15.296875" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.69921875" customWidth="1"/>
+    <col min="8" max="8" width="15" style="36" customWidth="1"/>
+    <col min="10" max="10" width="47.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1461,7 +1463,7 @@
         <v>2035</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>12</v>
@@ -1720,13 +1722,13 @@
         <v>2035</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="s">
@@ -1737,7 +1739,7 @@
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K16" s="4"/>
     </row>
@@ -1749,13 +1751,13 @@
         <v>2035</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
@@ -1766,7 +1768,7 @@
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K17" s="4"/>
     </row>
@@ -1778,13 +1780,13 @@
         <v>2035</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
@@ -1795,7 +1797,7 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K18" s="4"/>
     </row>
@@ -1807,13 +1809,13 @@
         <v>2035</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7" t="s">
@@ -1824,7 +1826,7 @@
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K19" s="4"/>
     </row>
@@ -1836,13 +1838,13 @@
         <v>2035</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7" t="s">
@@ -1853,7 +1855,7 @@
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K20" s="4"/>
     </row>
@@ -1865,13 +1867,13 @@
         <v>2035</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
@@ -1882,7 +1884,7 @@
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K21" s="4"/>
     </row>
@@ -1894,16 +1896,16 @@
         <v>2035</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>27</v>
@@ -1913,7 +1915,7 @@
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K22" s="4"/>
     </row>
@@ -1925,16 +1927,16 @@
         <v>2035</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>27</v>
@@ -1946,10 +1948,10 @@
         <v>9</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -1966,7 +1968,7 @@
         <v>23</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F24" s="23"/>
       <c r="G24" s="23" t="s">
@@ -1997,7 +1999,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25" s="23" t="s">
@@ -2028,7 +2030,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="23" t="s">
@@ -2059,7 +2061,7 @@
         <v>23</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F27" s="23" t="s">
         <v>131</v>
@@ -2086,16 +2088,16 @@
         <v>2035</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D28" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G28" s="23" t="s">
         <v>27</v>
@@ -2117,16 +2119,16 @@
         <v>2035</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G29" s="23" t="s">
         <v>27</v>
@@ -2138,10 +2140,10 @@
         <v>9</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -2158,10 +2160,10 @@
         <v>23</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G30" s="23" t="s">
         <v>27</v>
@@ -2189,10 +2191,10 @@
         <v>23</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>27</v>
@@ -2220,10 +2222,10 @@
         <v>23</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G32" s="23" t="s">
         <v>27</v>
@@ -2245,16 +2247,16 @@
         <v>2035</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D33" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>135</v>
+        <v>205</v>
       </c>
       <c r="G33" s="23" t="s">
         <v>27</v>
@@ -2276,16 +2278,16 @@
         <v>2035</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>135</v>
+        <v>206</v>
       </c>
       <c r="G34" s="23" t="s">
         <v>27</v>
@@ -2297,10 +2299,10 @@
         <v>9</v>
       </c>
       <c r="J34" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="K34" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -2311,16 +2313,16 @@
         <v>2035</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="G35" s="23" t="s">
         <v>27</v>
@@ -2344,16 +2346,16 @@
         <v>2035</v>
       </c>
       <c r="C36" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D36" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>141</v>
-      </c>
       <c r="F36" s="23" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="G36" s="23" t="s">
         <v>27</v>
@@ -2375,16 +2377,16 @@
         <v>2035</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>137</v>
+        <v>209</v>
       </c>
       <c r="G37" s="23" t="s">
         <v>27</v>
@@ -2396,10 +2398,10 @@
         <v>9</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
@@ -2410,16 +2412,16 @@
         <v>2035</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D38" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G38" s="26" t="s">
         <v>27</v>
@@ -2431,7 +2433,7 @@
         <v>9</v>
       </c>
       <c r="J38" s="26" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K38" s="27"/>
     </row>
@@ -2443,16 +2445,16 @@
         <v>2035</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>27</v>
@@ -2462,10 +2464,10 @@
       </c>
       <c r="I39" s="20"/>
       <c r="J39" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -2476,16 +2478,16 @@
         <v>2035</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>23</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>27</v>
@@ -2495,10 +2497,10 @@
       </c>
       <c r="I40" s="20"/>
       <c r="J40" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -2509,16 +2511,16 @@
         <v>2035</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D41" s="20" t="s">
         <v>23</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>27</v>
@@ -2528,10 +2530,10 @@
       </c>
       <c r="I41" s="20"/>
       <c r="J41" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -2542,16 +2544,16 @@
         <v>2035</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>23</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>27</v>
@@ -2561,10 +2563,10 @@
       </c>
       <c r="I42" s="20"/>
       <c r="J42" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -2575,16 +2577,16 @@
         <v>2035</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>23</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>27</v>
@@ -2594,7 +2596,7 @@
       </c>
       <c r="I43" s="20"/>
       <c r="J43" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K43" s="2"/>
     </row>
@@ -2606,16 +2608,16 @@
         <v>2035</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>23</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>27</v>
@@ -2625,10 +2627,10 @@
       </c>
       <c r="I44" s="20"/>
       <c r="J44" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -2639,16 +2641,16 @@
         <v>2035</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>23</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>27</v>
@@ -2660,10 +2662,10 @@
         <v>9</v>
       </c>
       <c r="J45" s="20" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -2674,16 +2676,16 @@
         <v>2035</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G46" s="23" t="s">
         <v>27</v>
@@ -2693,7 +2695,7 @@
       </c>
       <c r="I46" s="23"/>
       <c r="J46" s="23" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K46" s="3"/>
     </row>
@@ -2705,16 +2707,16 @@
         <v>2035</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D47" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G47" s="23" t="s">
         <v>27</v>
@@ -2726,10 +2728,10 @@
         <v>9</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2740,16 +2742,16 @@
         <v>2035</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>27</v>
@@ -2761,10 +2763,10 @@
         <v>9</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -2986,7 +2988,7 @@
       <c r="J55" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K55" s="34" t="s">
+      <c r="K55" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3019,7 +3021,7 @@
       <c r="J56" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K56" s="34" t="s">
+      <c r="K56" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3052,7 +3054,7 @@
       <c r="J57" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K57" s="34" t="s">
+      <c r="K57" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3085,7 +3087,7 @@
       <c r="J58" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K58" s="34" t="s">
+      <c r="K58" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3118,7 +3120,7 @@
       <c r="J59" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K59" s="34" t="s">
+      <c r="K59" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3149,7 +3151,7 @@
       <c r="J60" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="K60" s="34" t="s">
+      <c r="K60" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3182,7 +3184,7 @@
       <c r="J61" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="K61" s="35" t="s">
+      <c r="K61" s="34" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3215,7 +3217,7 @@
       <c r="J62" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K62" s="34" t="s">
+      <c r="K62" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3248,7 +3250,7 @@
       <c r="J63" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K63" s="34" t="s">
+      <c r="K63" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3279,7 +3281,7 @@
       <c r="J64" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K64" s="34" t="s">
+      <c r="K64" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3310,7 +3312,7 @@
       <c r="J65" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K65" s="34" t="s">
+      <c r="K65" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3341,7 +3343,7 @@
       <c r="J66" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K66" s="34" t="s">
+      <c r="K66" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3374,7 +3376,7 @@
       <c r="J67" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K67" s="36" t="s">
+      <c r="K67" s="35" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ModelRun with Blueprint with TM1.5.2.5
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5777868-01C2-4C33-95FE-DF88A01C61C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBA5576-D532-4103-B445-D660D5564E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27300" yWindow="2070" windowWidth="24795" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="214">
   <si>
     <t>No Project</t>
   </si>
@@ -666,6 +666,18 @@
   </si>
   <si>
     <t>Pathway 1b - uniform tolls (with VZ fix #1)</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_24_rerunTM1.5.2.5</t>
+  </si>
+  <si>
+    <t>Blueprint with TM1.5.2.5</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_24\INPUT</t>
+  </si>
+  <si>
+    <t>Rerun Blueprint with TM1.5.2.5 and no changes to the network</t>
   </si>
 </sst>
 </file>
@@ -1212,11 +1224,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1485,35 +1497,36 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>24</v>
+    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -1524,7 +1537,7 @@
         <v>2035</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>23</v>
@@ -1532,9 +1545,7 @@
       <c r="E10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>86</v>
-      </c>
+      <c r="F10" s="20"/>
       <c r="G10" s="20" t="s">
         <v>27</v>
       </c>
@@ -1543,10 +1554,10 @@
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -1557,7 +1568,7 @@
         <v>2035</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>23</v>
@@ -1565,7 +1576,9 @@
       <c r="E11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="20" t="s">
+        <v>86</v>
+      </c>
       <c r="G11" s="20" t="s">
         <v>27</v>
       </c>
@@ -1574,10 +1587,10 @@
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="20" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -1588,7 +1601,7 @@
         <v>2035</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>23</v>
@@ -1596,9 +1609,7 @@
       <c r="E12" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>119</v>
-      </c>
+      <c r="F12" s="20"/>
       <c r="G12" s="20" t="s">
         <v>27</v>
       </c>
@@ -1621,7 +1632,7 @@
         <v>2035</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>23</v>
@@ -1630,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>27</v>
@@ -1654,7 +1665,7 @@
         <v>2035</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>23</v>
@@ -1663,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>27</v>
@@ -1676,7 +1687,7 @@
         <v>109</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -1687,7 +1698,7 @@
         <v>2035</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>23</v>
@@ -1696,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>27</v>
@@ -1704,9 +1715,7 @@
       <c r="H15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="I15" s="20"/>
       <c r="J15" s="20" t="s">
         <v>109</v>
       </c>
@@ -1714,34 +1723,40 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="6">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="K16" s="4"/>
+    <row r="16" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
@@ -1751,7 +1766,7 @@
         <v>2035</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>23</v>
@@ -1768,7 +1783,7 @@
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K17" s="4"/>
     </row>
@@ -1780,7 +1795,7 @@
         <v>2035</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>23</v>
@@ -1797,7 +1812,7 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K18" s="4"/>
     </row>
@@ -1809,7 +1824,7 @@
         <v>2035</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>23</v>
@@ -1826,7 +1841,7 @@
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K19" s="4"/>
     </row>
@@ -1838,7 +1853,7 @@
         <v>2035</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>23</v>
@@ -1855,7 +1870,7 @@
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="K20" s="4"/>
     </row>
@@ -1867,7 +1882,7 @@
         <v>2035</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>23</v>
@@ -1896,7 +1911,7 @@
         <v>2035</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>23</v>
@@ -1904,9 +1919,7 @@
       <c r="E22" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
         <v>27</v>
       </c>
@@ -1927,7 +1940,7 @@
         <v>2035</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>23</v>
@@ -1936,53 +1949,53 @@
         <v>142</v>
       </c>
       <c r="F23" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="7" t="s">
+      <c r="G24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J24" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H24" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -1993,7 +2006,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>23</v>
@@ -2013,7 +2026,7 @@
         <v>112</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -2024,7 +2037,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>23</v>
@@ -2055,7 +2068,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>23</v>
@@ -2063,9 +2076,7 @@
       <c r="E27" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="F27" s="23" t="s">
-        <v>131</v>
-      </c>
+      <c r="F27" s="23"/>
       <c r="G27" s="23" t="s">
         <v>27</v>
       </c>
@@ -2077,7 +2088,7 @@
         <v>112</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -2088,7 +2099,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="D28" s="23" t="s">
         <v>23</v>
@@ -2097,7 +2108,7 @@
         <v>138</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="G28" s="23" t="s">
         <v>27</v>
@@ -2109,7 +2120,9 @@
       <c r="J28" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="K28" s="3"/>
+      <c r="K28" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="29" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
@@ -2119,7 +2132,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>23</v>
@@ -2136,15 +2149,11 @@
       <c r="H29" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="I29" s="23"/>
       <c r="J29" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>200</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
@@ -2154,7 +2163,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>132</v>
+        <v>199</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>23</v>
@@ -2163,7 +2172,7 @@
         <v>138</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="G30" s="23" t="s">
         <v>27</v>
@@ -2171,11 +2180,15 @@
       <c r="H30" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="23"/>
+      <c r="I30" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="J30" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K30" s="3"/>
+        <v>201</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="31" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
@@ -2185,7 +2198,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>23</v>
@@ -2194,7 +2207,7 @@
         <v>138</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>27</v>
@@ -2216,7 +2229,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>23</v>
@@ -2225,7 +2238,7 @@
         <v>138</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G32" s="23" t="s">
         <v>27</v>
@@ -2247,7 +2260,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D33" s="23" t="s">
         <v>23</v>
@@ -2256,7 +2269,7 @@
         <v>138</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="G33" s="23" t="s">
         <v>27</v>
@@ -2278,7 +2291,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>23</v>
@@ -2287,7 +2300,7 @@
         <v>138</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G34" s="23" t="s">
         <v>27</v>
@@ -2295,15 +2308,11 @@
       <c r="H34" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="I34" s="23"/>
       <c r="J34" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>194</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
@@ -2313,7 +2322,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>23</v>
@@ -2322,7 +2331,7 @@
         <v>138</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G35" s="23" t="s">
         <v>27</v>
@@ -2334,9 +2343,11 @@
         <v>9</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K35" s="3"/>
+        <v>191</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="36" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
@@ -2346,7 +2357,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>23</v>
@@ -2355,7 +2366,7 @@
         <v>138</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G36" s="23" t="s">
         <v>27</v>
@@ -2363,7 +2374,9 @@
       <c r="H36" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="23"/>
+      <c r="I36" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="J36" s="23" t="s">
         <v>112</v>
       </c>
@@ -2377,7 +2390,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>23</v>
@@ -2386,89 +2399,87 @@
         <v>138</v>
       </c>
       <c r="F37" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="G37" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="G37" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H37" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="23" t="s">
+      <c r="G38" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J37" s="23" t="s">
+      <c r="J38" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="K37" s="3" t="s">
+      <c r="K38" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="26" t="s">
+    <row r="39" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="25">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="26" t="s">
+      <c r="D39" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F39" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="G38" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="26" t="s">
+      <c r="G39" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J38" s="26" t="s">
+      <c r="J39" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="K38" s="27"/>
-    </row>
-    <row r="39" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>175</v>
-      </c>
+      <c r="K39" s="27"/>
     </row>
     <row r="40" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
@@ -2478,7 +2489,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>23</v>
@@ -2487,7 +2498,7 @@
         <v>144</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>27</v>
@@ -2511,7 +2522,7 @@
         <v>2035</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D41" s="20" t="s">
         <v>23</v>
@@ -2520,7 +2531,7 @@
         <v>144</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>27</v>
@@ -2544,7 +2555,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>23</v>
@@ -2553,7 +2564,7 @@
         <v>144</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>27</v>
@@ -2577,7 +2588,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>23</v>
@@ -2586,7 +2597,7 @@
         <v>144</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>27</v>
@@ -2596,9 +2607,11 @@
       </c>
       <c r="I43" s="20"/>
       <c r="J43" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="K43" s="2"/>
+        <v>174</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="44" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
@@ -2608,7 +2621,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>23</v>
@@ -2627,11 +2640,9 @@
       </c>
       <c r="I44" s="20"/>
       <c r="J44" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>189</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
@@ -2641,7 +2652,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>23</v>
@@ -2658,46 +2669,48 @@
       <c r="H45" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I45" s="20" t="s">
+      <c r="I45" s="20"/>
+      <c r="J45" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J45" s="20" t="s">
+      <c r="J46" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="K46" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="F46" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="G46" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H46" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
@@ -2707,7 +2720,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="D47" s="23" t="s">
         <v>23</v>
@@ -2724,80 +2737,80 @@
       <c r="H47" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="23" t="s">
+      <c r="I47" s="23"/>
+      <c r="J47" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H48" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J47" s="23" t="s">
+      <c r="J48" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="K48" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" s="6">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="7" t="s">
+    <row r="49" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E48" s="7" t="s">
+      <c r="D49" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="G48" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="7" t="s">
+      <c r="G49" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J48" s="7" t="s">
+      <c r="J49" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K49" s="4" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B49" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C49" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E49" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H49" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -2808,7 +2821,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D50" s="30" t="s">
         <v>23</v>
@@ -2816,9 +2829,7 @@
       <c r="E50" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F50" s="30" t="s">
-        <v>76</v>
-      </c>
+      <c r="F50" s="30"/>
       <c r="G50" s="30" t="s">
         <v>27</v>
       </c>
@@ -2827,10 +2838,10 @@
       </c>
       <c r="I50" s="30"/>
       <c r="J50" s="30" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -2841,7 +2852,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D51" s="30" t="s">
         <v>23</v>
@@ -2849,7 +2860,9 @@
       <c r="E51" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F51" s="30"/>
+      <c r="F51" s="30" t="s">
+        <v>76</v>
+      </c>
       <c r="G51" s="30" t="s">
         <v>27</v>
       </c>
@@ -2858,10 +2871,10 @@
       </c>
       <c r="I51" s="30"/>
       <c r="J51" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="K51" s="30" t="s">
-        <v>53</v>
+        <v>66</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -2872,7 +2885,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" s="30" t="s">
         <v>23</v>
@@ -2889,7 +2902,7 @@
       </c>
       <c r="I52" s="30"/>
       <c r="J52" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K52" s="30" t="s">
         <v>53</v>
@@ -2903,7 +2916,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" s="30" t="s">
         <v>23</v>
@@ -2920,7 +2933,7 @@
       </c>
       <c r="I53" s="30"/>
       <c r="J53" s="30" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K53" s="30" t="s">
         <v>53</v>
@@ -2934,7 +2947,7 @@
         <v>2035</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D54" s="30" t="s">
         <v>23</v>
@@ -2942,9 +2955,7 @@
       <c r="E54" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F54" s="30" t="s">
-        <v>88</v>
-      </c>
+      <c r="F54" s="30"/>
       <c r="G54" s="30" t="s">
         <v>27</v>
       </c>
@@ -2953,43 +2964,43 @@
       </c>
       <c r="I54" s="30"/>
       <c r="J54" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="K54" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G55" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" s="30"/>
+      <c r="J55" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B55" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E55" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="F55" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="G55" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H55" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" s="16"/>
-      <c r="J55" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="K55" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
@@ -3000,7 +3011,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D56" s="31" t="s">
         <v>23</v>
@@ -3009,7 +3020,7 @@
         <v>30</v>
       </c>
       <c r="F56" s="33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G56" s="31" t="s">
         <v>27</v>
@@ -3022,7 +3033,7 @@
         <v>37</v>
       </c>
       <c r="K56" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -3033,7 +3044,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D57" s="31" t="s">
         <v>23</v>
@@ -3042,7 +3053,7 @@
         <v>30</v>
       </c>
       <c r="F57" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G57" s="31" t="s">
         <v>27</v>
@@ -3055,7 +3066,7 @@
         <v>37</v>
       </c>
       <c r="K57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
@@ -3066,7 +3077,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D58" s="31" t="s">
         <v>23</v>
@@ -3075,7 +3086,7 @@
         <v>30</v>
       </c>
       <c r="F58" s="33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G58" s="31" t="s">
         <v>27</v>
@@ -3088,7 +3099,7 @@
         <v>37</v>
       </c>
       <c r="K58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
@@ -3099,7 +3110,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D59" s="31" t="s">
         <v>23</v>
@@ -3108,7 +3119,7 @@
         <v>30</v>
       </c>
       <c r="F59" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G59" s="31" t="s">
         <v>27</v>
@@ -3121,7 +3132,7 @@
         <v>37</v>
       </c>
       <c r="K59" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
@@ -3132,7 +3143,7 @@
         <v>2035</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D60" s="31" t="s">
         <v>23</v>
@@ -3140,7 +3151,9 @@
       <c r="E60" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F60" s="33"/>
+      <c r="F60" s="33" t="s">
+        <v>82</v>
+      </c>
       <c r="G60" s="31" t="s">
         <v>27</v>
       </c>
@@ -3149,10 +3162,10 @@
       </c>
       <c r="I60" s="16"/>
       <c r="J60" s="16" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="K60" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
@@ -3163,7 +3176,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="D61" s="31" t="s">
         <v>23</v>
@@ -3171,9 +3184,7 @@
       <c r="E61" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F61" s="33" t="s">
-        <v>85</v>
-      </c>
+      <c r="F61" s="33"/>
       <c r="G61" s="31" t="s">
         <v>27</v>
       </c>
@@ -3182,9 +3193,9 @@
       </c>
       <c r="I61" s="16"/>
       <c r="J61" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K61" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="K61" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3196,7 +3207,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="D62" s="31" t="s">
         <v>23</v>
@@ -3205,7 +3216,7 @@
         <v>30</v>
       </c>
       <c r="F62" s="33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G62" s="31" t="s">
         <v>27</v>
@@ -3215,10 +3226,10 @@
       </c>
       <c r="I62" s="16"/>
       <c r="J62" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="K62" t="s">
-        <v>51</v>
+        <v>72</v>
+      </c>
+      <c r="K62" s="34" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
@@ -3229,7 +3240,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D63" s="31" t="s">
         <v>23</v>
@@ -3238,7 +3249,7 @@
         <v>30</v>
       </c>
       <c r="F63" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G63" s="31" t="s">
         <v>27</v>
@@ -3251,7 +3262,7 @@
         <v>37</v>
       </c>
       <c r="K63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
@@ -3262,7 +3273,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D64" s="31" t="s">
         <v>23</v>
@@ -3270,7 +3281,9 @@
       <c r="E64" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F64" s="33"/>
+      <c r="F64" s="33" t="s">
+        <v>84</v>
+      </c>
       <c r="G64" s="31" t="s">
         <v>27</v>
       </c>
@@ -3279,7 +3292,7 @@
       </c>
       <c r="I64" s="16"/>
       <c r="J64" s="16" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="K64" t="s">
         <v>52</v>
@@ -3293,7 +3306,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D65" s="31" t="s">
         <v>23</v>
@@ -3324,7 +3337,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D66" s="31" t="s">
         <v>23</v>
@@ -3355,7 +3368,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D67" s="31" t="s">
         <v>23</v>
@@ -3363,9 +3376,7 @@
       <c r="E67" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F67" s="33" t="s">
-        <v>95</v>
-      </c>
+      <c r="F67" s="33"/>
       <c r="G67" s="31" t="s">
         <v>27</v>
       </c>
@@ -3376,8 +3387,8 @@
       <c r="J67" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K67" s="35" t="s">
-        <v>99</v>
+      <c r="K67" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -3388,7 +3399,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D68" s="31" t="s">
         <v>23</v>
@@ -3397,7 +3408,7 @@
         <v>30</v>
       </c>
       <c r="F68" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G68" s="31" t="s">
         <v>27</v>
@@ -3409,6 +3420,9 @@
       <c r="J68" s="16" t="s">
         <v>68</v>
       </c>
+      <c r="K68" s="35" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="31" t="s">
@@ -3418,7 +3432,7 @@
         <v>2035</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" s="31" t="s">
         <v>23</v>
@@ -3427,7 +3441,7 @@
         <v>30</v>
       </c>
       <c r="F69" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G69" s="31" t="s">
         <v>27</v>
@@ -3448,7 +3462,7 @@
         <v>2035</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D70" s="31" t="s">
         <v>23</v>
@@ -3457,7 +3471,7 @@
         <v>30</v>
       </c>
       <c r="F70" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G70" s="31" t="s">
         <v>27</v>
@@ -3470,37 +3484,34 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B71" s="6">
-        <v>2035</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G71" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="K71" s="4" t="s">
-        <v>104</v>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B71" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G71" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="H71" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3511,7 +3522,7 @@
         <v>2035</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>23</v>
@@ -3520,7 +3531,7 @@
         <v>101</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>27</v>
@@ -3530,36 +3541,70 @@
       </c>
       <c r="I72" s="7"/>
       <c r="J72" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B73" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="K72" s="4" t="s">
+      <c r="K73" s="4" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K49" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
-    <hyperlink ref="K9" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="K54" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K61" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K67" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="K50" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="K10" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
+    <hyperlink ref="K55" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="K62" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="K68" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
     <hyperlink ref="K7" r:id="rId6" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
-    <hyperlink ref="K14" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
-    <hyperlink ref="K15" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
-    <hyperlink ref="K13" r:id="rId9" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{07D1B2DA-E517-4DD9-B4E8-AE0933FD4973}"/>
-    <hyperlink ref="K12" r:id="rId10" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{4A8E9582-524B-46F3-8A76-0C1F5220D214}"/>
-    <hyperlink ref="K11" r:id="rId11" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{E622471D-8EED-401F-9FFF-3C4854166AD2}"/>
-    <hyperlink ref="K24" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
-    <hyperlink ref="K25" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
-    <hyperlink ref="K26" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
-    <hyperlink ref="K27" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
-    <hyperlink ref="K48" r:id="rId16" xr:uid="{C5D42A4A-7D1E-4E61-A6D8-57E8258064CF}"/>
-    <hyperlink ref="K23" r:id="rId17" display="https://app.asana.com/0/1201809392759895/1204199508775563/f" xr:uid="{AD5B4BF6-019A-41E5-B4FF-144AB869AC79}"/>
-    <hyperlink ref="K29" r:id="rId18" display="https://app.asana.com/0/1201809392759895/1204199508775567/f" xr:uid="{4D75E071-693C-4E6B-9BC3-F13FF7899650}"/>
-    <hyperlink ref="K45" r:id="rId19" display="https://app.asana.com/0/1201809392759895/1204199508775554/f" xr:uid="{93FEBC25-3D8F-4C29-A30C-17379D746E6A}"/>
+    <hyperlink ref="K15" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
+    <hyperlink ref="K16" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
+    <hyperlink ref="K14" r:id="rId9" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{07D1B2DA-E517-4DD9-B4E8-AE0933FD4973}"/>
+    <hyperlink ref="K13" r:id="rId10" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{4A8E9582-524B-46F3-8A76-0C1F5220D214}"/>
+    <hyperlink ref="K12" r:id="rId11" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{E622471D-8EED-401F-9FFF-3C4854166AD2}"/>
+    <hyperlink ref="K25" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
+    <hyperlink ref="K26" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
+    <hyperlink ref="K27" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
+    <hyperlink ref="K28" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
+    <hyperlink ref="K49" r:id="rId16" xr:uid="{C5D42A4A-7D1E-4E61-A6D8-57E8258064CF}"/>
+    <hyperlink ref="K24" r:id="rId17" display="https://app.asana.com/0/1201809392759895/1204199508775563/f" xr:uid="{AD5B4BF6-019A-41E5-B4FF-144AB869AC79}"/>
+    <hyperlink ref="K30" r:id="rId18" display="https://app.asana.com/0/1201809392759895/1204199508775567/f" xr:uid="{4D75E071-693C-4E6B-9BC3-F13FF7899650}"/>
+    <hyperlink ref="K46" r:id="rId19" display="https://app.asana.com/0/1201809392759895/1204199508775554/f" xr:uid="{93FEBC25-3D8F-4C29-A30C-17379D746E6A}"/>
+    <hyperlink ref="K9" r:id="rId20" display="https://app.asana.com/0/0/1204199508775527/f" xr:uid="{F74BF0A2-72BF-4CE6-B53E-B781F9178384}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
demoting "uniform tolls" from being current
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0299498-CE5D-4278-BC31-F1C7CF75B1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF34616D-8A3A-42AF-B280-F9EC51B936CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="307">
   <si>
     <t>No Project</t>
   </si>
@@ -1507,24 +1507,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.69921875" customWidth="1"/>
     <col min="8" max="8" width="15" style="36" customWidth="1"/>
-    <col min="10" max="10" width="47.42578125" customWidth="1"/>
+    <col min="10" max="10" width="47.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>40</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>40</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>40</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>40</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>40</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>40</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>40</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>40</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>40</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>40</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>40</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>40</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>40</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>40</v>
       </c>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -2222,7 +2222,7 @@
       </c>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>40</v>
       </c>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>40</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>40</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>40</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>40</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>40</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>40</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>40</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>40</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>40</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>40</v>
       </c>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>40</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>40</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>40</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
         <v>40</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>40</v>
       </c>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
         <v>40</v>
       </c>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="21" t="s">
         <v>40</v>
       </c>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
         <v>40</v>
       </c>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="21" t="s">
         <v>40</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>40</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
         <v>40</v>
       </c>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>40</v>
       </c>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="21" t="s">
         <v>40</v>
       </c>
@@ -3046,9 +3046,7 @@
       <c r="H48" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I48" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="I48" s="23"/>
       <c r="J48" s="23" t="s">
         <v>190</v>
       </c>
@@ -3056,7 +3054,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>40</v>
       </c>
@@ -3089,7 +3087,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>40</v>
       </c>
@@ -3122,7 +3120,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>40</v>
       </c>
@@ -3157,7 +3155,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>40</v>
       </c>
@@ -3192,7 +3190,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>40</v>
       </c>
@@ -3227,7 +3225,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>40</v>
       </c>
@@ -3262,7 +3260,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>40</v>
       </c>
@@ -3293,7 +3291,7 @@
       </c>
       <c r="K55" s="27"/>
     </row>
-    <row r="56" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
         <v>40</v>
       </c>
@@ -3326,7 +3324,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
         <v>40</v>
       </c>
@@ -3359,7 +3357,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
         <v>40</v>
       </c>
@@ -3394,7 +3392,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24" t="s">
         <v>40</v>
       </c>
@@ -3429,7 +3427,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="24" t="s">
         <v>40</v>
       </c>
@@ -3464,7 +3462,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="24" t="s">
         <v>40</v>
       </c>
@@ -3499,7 +3497,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18" t="s">
         <v>40</v>
       </c>
@@ -3532,7 +3530,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18" t="s">
         <v>40</v>
       </c>
@@ -3565,7 +3563,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
         <v>40</v>
       </c>
@@ -3598,7 +3596,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18" t="s">
         <v>40</v>
       </c>
@@ -3631,7 +3629,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18" t="s">
         <v>40</v>
       </c>
@@ -3662,7 +3660,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
         <v>40</v>
       </c>
@@ -3695,7 +3693,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18" t="s">
         <v>40</v>
       </c>
@@ -3728,7 +3726,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
         <v>40</v>
       </c>
@@ -3761,7 +3759,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
         <v>40</v>
       </c>
@@ -3796,7 +3794,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="21" t="s">
         <v>40</v>
       </c>
@@ -3827,7 +3825,7 @@
       </c>
       <c r="K71" s="3"/>
     </row>
-    <row r="72" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="21" t="s">
         <v>40</v>
       </c>
@@ -3860,7 +3858,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="21" t="s">
         <v>40</v>
       </c>
@@ -3893,7 +3891,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="21" t="s">
         <v>40</v>
       </c>
@@ -3926,7 +3924,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="21" t="s">
         <v>40</v>
       </c>
@@ -3961,7 +3959,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>40</v>
       </c>
@@ -3994,7 +3992,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>40</v>
       </c>
@@ -4027,7 +4025,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>40</v>
       </c>
@@ -4060,7 +4058,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>40</v>
       </c>
@@ -4095,7 +4093,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="28" t="s">
         <v>40</v>
       </c>
@@ -4126,7 +4124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="28" t="s">
         <v>40</v>
       </c>
@@ -4159,7 +4157,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="28" t="s">
         <v>40</v>
       </c>
@@ -4190,7 +4188,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="28" t="s">
         <v>40</v>
       </c>
@@ -4221,7 +4219,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="28" t="s">
         <v>40</v>
       </c>
@@ -4252,7 +4250,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="28" t="s">
         <v>40</v>
       </c>
@@ -4285,7 +4283,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="31" t="s">
         <v>40</v>
       </c>
@@ -4318,7 +4316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="31" t="s">
         <v>40</v>
       </c>
@@ -4351,7 +4349,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="31" t="s">
         <v>40</v>
       </c>
@@ -4384,7 +4382,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="31" t="s">
         <v>40</v>
       </c>
@@ -4417,7 +4415,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="31" t="s">
         <v>40</v>
       </c>
@@ -4450,7 +4448,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="31" t="s">
         <v>40</v>
       </c>
@@ -4481,7 +4479,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="31" t="s">
         <v>40</v>
       </c>
@@ -4514,7 +4512,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="31" t="s">
         <v>40</v>
       </c>
@@ -4547,7 +4545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="31" t="s">
         <v>40</v>
       </c>
@@ -4580,7 +4578,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="31" t="s">
         <v>40</v>
       </c>
@@ -4611,7 +4609,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="31" t="s">
         <v>40</v>
       </c>
@@ -4642,7 +4640,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="31" t="s">
         <v>40</v>
       </c>
@@ -4673,7 +4671,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="31" t="s">
         <v>40</v>
       </c>
@@ -4706,7 +4704,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="31" t="s">
         <v>40</v>
       </c>
@@ -4736,7 +4734,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="31" t="s">
         <v>40</v>
       </c>
@@ -4766,7 +4764,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="31" t="s">
         <v>40</v>
       </c>
@@ -4796,7 +4794,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>40</v>
       </c>
@@ -4829,7 +4827,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Rename short name for recent round of runs to be more human readable
e.g. Pathway 1a (NP10) instead of NP10_Path1a_01
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC2A0CE-2D9C-4615-ACC0-8381E55C2FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570A14BF-6DA2-433E-A947-5E518924E769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="4350" windowWidth="26730" windowHeight="15825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$I$113</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -950,18 +950,12 @@
     <t>2035_TM152_NGF_NP10_Path3a_01</t>
   </si>
   <si>
-    <t>NP10_Path3a_01</t>
-  </si>
-  <si>
     <t>Rerun Pathway 3a to incorporate EN7 fix</t>
   </si>
   <si>
     <t>2035_TM152_NGF_NP10_Path1b_01</t>
   </si>
   <si>
-    <t>NP10_Path1b_01</t>
-  </si>
-  <si>
     <t>Rerun Pathway 1b to incorporate EN7 fix</t>
   </si>
   <si>
@@ -971,15 +965,9 @@
     <t>Rerun Pathway 3b to incorporate EN7 fix</t>
   </si>
   <si>
-    <t>NP10_Path3b_01</t>
-  </si>
-  <si>
     <t>2035_TM152_NGF_NP10_Path2a_01</t>
   </si>
   <si>
-    <t>NP10_Path2a_01</t>
-  </si>
-  <si>
     <t>Rerun Pathway 2a to incorporate EN7 fix</t>
   </si>
   <si>
@@ -989,54 +977,33 @@
     <t>2035_TM152_NGF_NP10_Path2b_01</t>
   </si>
   <si>
-    <t>NP10_Path2b_01</t>
-  </si>
-  <si>
     <t>2035_TM152_NGF_NP10_Path4_01</t>
   </si>
   <si>
-    <t>NP10_Path4_01</t>
-  </si>
-  <si>
     <t>Rerun Pathway 4 to incorporate EN7 fix</t>
   </si>
   <si>
     <t>2035_TM152_NGF_NP10_Path1a_01</t>
   </si>
   <si>
-    <t>NP10_Path1a_01</t>
-  </si>
-  <si>
     <t>Rerun Pathway 1a to incorporate EN7 fix</t>
   </si>
   <si>
     <t>2035_TM152_NGF_NP10</t>
   </si>
   <si>
-    <t>NoProject_09</t>
-  </si>
-  <si>
-    <t>NoProject_10</t>
-  </si>
-  <si>
     <t>Rerun NGF NoProject to incorporate EN7 fix</t>
   </si>
   <si>
     <t>2035_TM152_NGF_NP10_Path2b_01_10pc</t>
   </si>
   <si>
-    <t>NP10_Path2b_01_10pc</t>
-  </si>
-  <si>
     <t>✓ Rerun Pathway 2b (with arteial tolls at 10%) to incorporate EN7 fix</t>
   </si>
   <si>
     <t>2035_TM152_NGF_NP10_Path2a_01_10pc</t>
   </si>
   <si>
-    <t>NP10_Path2a_01_10pc</t>
-  </si>
-  <si>
     <t>Rerun Pathway 2a (with arteial tolls at 10%) to incorporate EN7 fix</t>
   </si>
   <si>
@@ -1050,6 +1017,39 @@
   </si>
   <si>
     <t>Pathway 2b_03_10pc (simple toll)</t>
+  </si>
+  <si>
+    <t>NoProject v9</t>
+  </si>
+  <si>
+    <t>NoProject v10</t>
+  </si>
+  <si>
+    <t>Pathway1a (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 1b (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 2a with 10pct art toll (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 2b with 10pct art toll (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 3a (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 3b (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 4 - No New Pricing (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 2b with 20pct art toll (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 2a with 20pct art toll (NP10)</t>
   </si>
 </sst>
 </file>
@@ -1601,8 +1601,8 @@
   <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1611,10 +1611,10 @@
     <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15" style="36" customWidth="1"/>
-    <col min="10" max="10" width="47.42578125" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15" style="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -1637,19 +1637,19 @@
         <v>77</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1671,14 +1671,14 @@
       <c r="F2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="J2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -1697,18 +1697,18 @@
         <v>94</v>
       </c>
       <c r="F3" s="16"/>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1728,18 +1728,18 @@
         <v>94</v>
       </c>
       <c r="F4" s="16"/>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="16"/>
+      <c r="H4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1759,18 +1759,18 @@
         <v>94</v>
       </c>
       <c r="F5" s="16"/>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="K5" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1792,18 +1792,18 @@
       <c r="F6" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="16"/>
+      <c r="H6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="K6" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1826,19 +1826,19 @@
         <v>87</v>
       </c>
       <c r="G7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="K7" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1861,15 +1861,15 @@
         <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="J8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1890,18 +1890,18 @@
       <c r="F9" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="J9" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>211</v>
+        <v>27</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1921,18 +1921,18 @@
         <v>0</v>
       </c>
       <c r="F10" s="20"/>
-      <c r="G10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="J10" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1954,18 +1954,18 @@
       <c r="F11" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J11" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -1985,18 +1985,18 @@
         <v>0</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="J12" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>121</v>
+        <v>27</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -2018,18 +2018,18 @@
       <c r="F13" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="J13" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>121</v>
+        <v>27</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -2051,18 +2051,18 @@
       <c r="F14" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="J14" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>121</v>
+        <v>27</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -2084,18 +2084,18 @@
       <c r="F15" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="J15" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>115</v>
+        <v>27</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -2117,18 +2117,18 @@
       <c r="F16" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="G16" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="J16" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>115</v>
+        <v>27</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -2150,18 +2150,18 @@
       <c r="F17" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>241</v>
+      </c>
       <c r="J17" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>241</v>
+        <v>27</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -2181,22 +2181,22 @@
         <v>0</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="20" t="s">
         <v>9</v>
       </c>
+      <c r="H18" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="J18" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>282</v>
+        <v>27</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -2207,7 +2207,7 @@
         <v>2035</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>23</v>
@@ -2216,22 +2216,22 @@
         <v>0</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="20" t="s">
         <v>9</v>
       </c>
+      <c r="H19" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="J19" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>327</v>
+        <v>27</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2251,17 +2251,17 @@
         <v>142</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" s="4"/>
       <c r="J20" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="K20" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -2280,17 +2280,17 @@
         <v>142</v>
       </c>
       <c r="F21" s="7"/>
-      <c r="G21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I21" s="4"/>
       <c r="J21" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="K21" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -2309,17 +2309,17 @@
         <v>142</v>
       </c>
       <c r="F22" s="7"/>
-      <c r="G22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I22" s="4"/>
       <c r="J22" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="K22" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
@@ -2338,17 +2338,17 @@
         <v>142</v>
       </c>
       <c r="F23" s="7"/>
-      <c r="G23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="K23" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -2367,17 +2367,17 @@
         <v>142</v>
       </c>
       <c r="F24" s="7"/>
-      <c r="G24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I24" s="4"/>
       <c r="J24" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="K24" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
@@ -2396,17 +2396,17 @@
         <v>142</v>
       </c>
       <c r="F25" s="7"/>
-      <c r="G25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I25" s="4"/>
       <c r="J25" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="K25" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -2425,17 +2425,17 @@
         <v>142</v>
       </c>
       <c r="F26" s="7"/>
-      <c r="G26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I26" s="4"/>
       <c r="J26" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="K26" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
@@ -2454,18 +2454,18 @@
         <v>142</v>
       </c>
       <c r="F27" s="7"/>
-      <c r="G27" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="J27" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>196</v>
+        <v>27</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2487,18 +2487,18 @@
       <c r="F28" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="J28" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>226</v>
+        <v>27</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2520,18 +2520,18 @@
       <c r="F29" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="J29" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>248</v>
+        <v>27</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2554,19 +2554,19 @@
         <v>269</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="H30" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>270</v>
+      </c>
       <c r="J30" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>270</v>
+        <v>27</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2589,19 +2589,19 @@
         <v>286</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="H31" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>287</v>
+      </c>
       <c r="J31" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>287</v>
+        <v>27</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2612,7 +2612,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>23</v>
@@ -2621,22 +2621,22 @@
         <v>142</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="H32" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>316</v>
+      </c>
       <c r="J32" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>323</v>
+        <v>27</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2656,18 +2656,18 @@
         <v>138</v>
       </c>
       <c r="F33" s="23"/>
-      <c r="G33" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="J33" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>125</v>
+        <v>27</v>
+      </c>
+      <c r="K33" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2687,18 +2687,18 @@
         <v>138</v>
       </c>
       <c r="F34" s="23"/>
-      <c r="G34" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="J34" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>129</v>
+        <v>27</v>
+      </c>
+      <c r="K34" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2718,18 +2718,18 @@
         <v>138</v>
       </c>
       <c r="F35" s="23"/>
-      <c r="G35" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H35" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="J35" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>129</v>
+        <v>27</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2751,18 +2751,18 @@
       <c r="F36" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="G36" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="J36" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>130</v>
+        <v>27</v>
+      </c>
+      <c r="K36" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2784,17 +2784,17 @@
       <c r="F37" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="G37" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H37" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I37" s="3"/>
       <c r="J37" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K37" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="K37" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="38" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
@@ -2815,18 +2815,18 @@
       <c r="F38" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="G38" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H38" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="J38" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>198</v>
+        <v>27</v>
+      </c>
+      <c r="K38" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2848,18 +2848,18 @@
       <c r="F39" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="G39" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>229</v>
+      </c>
       <c r="J39" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>229</v>
+        <v>27</v>
+      </c>
+      <c r="K39" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2881,18 +2881,18 @@
       <c r="F40" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="G40" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H40" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>250</v>
+      </c>
       <c r="J40" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>250</v>
+        <v>27</v>
+      </c>
+      <c r="K40" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2915,19 +2915,19 @@
         <v>272</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="23" t="s">
         <v>9</v>
       </c>
+      <c r="H41" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="J41" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>273</v>
+        <v>27</v>
+      </c>
+      <c r="K41" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2949,17 +2949,17 @@
       <c r="F42" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="G42" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H42" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I42" s="3"/>
       <c r="J42" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K42" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="K42" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="43" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
@@ -2980,17 +2980,17 @@
       <c r="F43" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="G43" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I43" s="3"/>
       <c r="J43" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K43" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="K43" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="44" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
@@ -3011,17 +3011,17 @@
       <c r="F44" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="G44" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H44" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I44" s="3"/>
       <c r="J44" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K44" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="K44" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="45" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
@@ -3042,17 +3042,17 @@
       <c r="F45" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="G45" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H45" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I45" s="3"/>
       <c r="J45" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K45" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="K45" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
@@ -3073,18 +3073,18 @@
       <c r="F46" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="G46" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H46" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="J46" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>193</v>
+        <v>27</v>
+      </c>
+      <c r="K46" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -3107,19 +3107,19 @@
         <v>289</v>
       </c>
       <c r="G47" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H47" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I47" s="23" t="s">
         <v>9</v>
       </c>
+      <c r="H47" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>290</v>
+      </c>
       <c r="J47" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>290</v>
+        <v>27</v>
+      </c>
+      <c r="K47" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -3141,17 +3141,17 @@
       <c r="F48" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="G48" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H48" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I48" s="3"/>
       <c r="J48" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K48" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="K48" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="49" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
@@ -3172,17 +3172,17 @@
       <c r="F49" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="G49" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H49" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I49" s="3"/>
       <c r="J49" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="K49" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="K49" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="50" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
@@ -3203,18 +3203,18 @@
       <c r="F50" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="G50" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="J50" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>191</v>
+        <v>27</v>
+      </c>
+      <c r="K50" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -3225,7 +3225,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D51" s="23" t="s">
         <v>23</v>
@@ -3234,22 +3234,22 @@
         <v>138</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="G51" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H51" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I51" s="23" t="s">
         <v>9</v>
       </c>
+      <c r="H51" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>306</v>
+      </c>
       <c r="J51" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>308</v>
+        <v>27</v>
+      </c>
+      <c r="K51" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3271,18 +3271,18 @@
       <c r="F52" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="G52" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I52" s="37" t="s">
+        <v>221</v>
+      </c>
       <c r="J52" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K52" s="37" t="s">
-        <v>221</v>
+        <v>27</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3304,18 +3304,18 @@
       <c r="F53" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="G53" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H53" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I53" s="37" t="s">
+        <v>235</v>
+      </c>
       <c r="J53" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K53" s="37" t="s">
-        <v>235</v>
+        <v>27</v>
+      </c>
+      <c r="K53" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3335,22 +3335,22 @@
         <v>219</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H54" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I54" s="13" t="s">
         <v>9</v>
       </c>
+      <c r="H54" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I54" s="37" t="s">
+        <v>244</v>
+      </c>
       <c r="J54" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K54" s="37" t="s">
-        <v>244</v>
+        <v>27</v>
+      </c>
+      <c r="K54" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3370,22 +3370,22 @@
         <v>219</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H55" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" s="13" t="s">
         <v>9</v>
       </c>
+      <c r="H55" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I55" s="37" t="s">
+        <v>264</v>
+      </c>
       <c r="J55" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K55" s="37" t="s">
-        <v>264</v>
+        <v>27</v>
+      </c>
+      <c r="K55" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3408,19 +3408,19 @@
         <v>293</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H56" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I56" s="13" t="s">
         <v>9</v>
       </c>
+      <c r="H56" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I56" s="37" t="s">
+        <v>295</v>
+      </c>
       <c r="J56" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K56" s="37" t="s">
-        <v>295</v>
+        <v>27</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3443,19 +3443,19 @@
         <v>294</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H57" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I57" s="13" t="s">
         <v>9</v>
       </c>
+      <c r="H57" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I57" s="37" t="s">
+        <v>296</v>
+      </c>
       <c r="J57" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K57" s="37" t="s">
-        <v>296</v>
+        <v>27</v>
+      </c>
+      <c r="K57" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3466,7 +3466,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D58" s="13" t="s">
         <v>23</v>
@@ -3475,22 +3475,22 @@
         <v>219</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>313</v>
+        <v>337</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H58" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I58" s="13" t="s">
         <v>9</v>
       </c>
+      <c r="H58" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I58" s="37" t="s">
+        <v>310</v>
+      </c>
       <c r="J58" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K58" s="37" t="s">
-        <v>314</v>
+        <v>27</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3501,7 +3501,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="D59" s="13" t="s">
         <v>23</v>
@@ -3510,22 +3510,22 @@
         <v>219</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I59" s="13" t="s">
         <v>9</v>
       </c>
+      <c r="H59" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I59" s="37" t="s">
+        <v>322</v>
+      </c>
       <c r="J59" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="K59" s="37" t="s">
-        <v>333</v>
+        <v>27</v>
+      </c>
+      <c r="K59" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3547,17 +3547,17 @@
       <c r="F60" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="G60" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H60" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="I60" s="27"/>
       <c r="J60" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="K60" s="27"/>
+        <v>27</v>
+      </c>
+      <c r="K60" s="25" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="61" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="24" t="s">
@@ -3578,18 +3578,18 @@
       <c r="F61" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="G61" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H61" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="I61" s="38" t="s">
+        <v>224</v>
+      </c>
       <c r="J61" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="K61" s="38" t="s">
-        <v>224</v>
+        <v>27</v>
+      </c>
+      <c r="K61" s="25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3611,18 +3611,18 @@
       <c r="F62" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="G62" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H62" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="I62" s="38" t="s">
+        <v>231</v>
+      </c>
       <c r="J62" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="K62" s="38" t="s">
-        <v>231</v>
+        <v>27</v>
+      </c>
+      <c r="K62" s="25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3642,22 +3642,22 @@
         <v>139</v>
       </c>
       <c r="F63" s="26" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="G63" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H63" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I63" s="26" t="s">
         <v>9</v>
       </c>
+      <c r="H63" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="I63" s="38" t="s">
+        <v>246</v>
+      </c>
       <c r="J63" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="K63" s="38" t="s">
-        <v>246</v>
+        <v>27</v>
+      </c>
+      <c r="K63" s="25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3677,22 +3677,22 @@
         <v>139</v>
       </c>
       <c r="F64" s="26" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H64" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I64" s="26" t="s">
         <v>9</v>
       </c>
+      <c r="H64" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="I64" s="38" t="s">
+        <v>267</v>
+      </c>
       <c r="J64" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="K64" s="38" t="s">
-        <v>267</v>
+        <v>27</v>
+      </c>
+      <c r="K64" s="25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3715,19 +3715,19 @@
         <v>299</v>
       </c>
       <c r="G65" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H65" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I65" s="26" t="s">
         <v>9</v>
       </c>
+      <c r="H65" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="I65" s="38" t="s">
+        <v>301</v>
+      </c>
       <c r="J65" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="K65" s="38" t="s">
-        <v>301</v>
+        <v>27</v>
+      </c>
+      <c r="K65" s="25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3750,19 +3750,19 @@
         <v>300</v>
       </c>
       <c r="G66" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H66" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I66" s="26" t="s">
         <v>9</v>
       </c>
+      <c r="H66" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="I66" s="38" t="s">
+        <v>302</v>
+      </c>
       <c r="J66" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="K66" s="38" t="s">
-        <v>302</v>
+        <v>27</v>
+      </c>
+      <c r="K66" s="25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3773,7 +3773,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D67" s="26" t="s">
         <v>23</v>
@@ -3782,22 +3782,22 @@
         <v>139</v>
       </c>
       <c r="F67" s="26" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="G67" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H67" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I67" s="26" t="s">
         <v>9</v>
       </c>
+      <c r="H67" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="I67" s="38" t="s">
+        <v>311</v>
+      </c>
       <c r="J67" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="K67" s="38" t="s">
-        <v>315</v>
+        <v>27</v>
+      </c>
+      <c r="K67" s="25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3808,7 +3808,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D68" s="26" t="s">
         <v>23</v>
@@ -3817,22 +3817,22 @@
         <v>139</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="G68" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H68" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I68" s="26" t="s">
         <v>9</v>
       </c>
+      <c r="H68" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="I68" s="38" t="s">
+        <v>320</v>
+      </c>
       <c r="J68" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="K68" s="38" t="s">
-        <v>330</v>
+        <v>27</v>
+      </c>
+      <c r="K68" s="25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -3854,18 +3854,18 @@
       <c r="F69" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="G69" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H69" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="J69" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>174</v>
+        <v>27</v>
+      </c>
+      <c r="K69" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -3887,18 +3887,18 @@
       <c r="F70" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="G70" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H70" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="J70" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>174</v>
+        <v>27</v>
+      </c>
+      <c r="K70" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -3920,18 +3920,18 @@
       <c r="F71" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="G71" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H71" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="J71" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>174</v>
+        <v>27</v>
+      </c>
+      <c r="K71" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -3953,18 +3953,18 @@
       <c r="F72" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="G72" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H72" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I72" s="20"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="J72" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>174</v>
+        <v>27</v>
+      </c>
+      <c r="K72" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -3986,17 +3986,17 @@
       <c r="F73" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="G73" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H73" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I73" s="20"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="I73" s="2"/>
       <c r="J73" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="K73" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="K73" s="19" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="74" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="18" t="s">
@@ -4017,18 +4017,18 @@
       <c r="F74" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="G74" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H74" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="J74" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>188</v>
+        <v>27</v>
+      </c>
+      <c r="K74" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -4050,18 +4050,18 @@
       <c r="F75" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="G75" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H75" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I75" s="20"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="J75" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>202</v>
+        <v>27</v>
+      </c>
+      <c r="K75" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -4083,18 +4083,18 @@
       <c r="F76" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="G76" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H76" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I76" s="20"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="J76" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>239</v>
+        <v>27</v>
+      </c>
+      <c r="K76" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -4117,19 +4117,19 @@
         <v>277</v>
       </c>
       <c r="G77" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H77" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I77" s="20" t="s">
         <v>9</v>
       </c>
+      <c r="H77" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>279</v>
+      </c>
       <c r="J77" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>279</v>
+        <v>27</v>
+      </c>
+      <c r="K77" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -4149,22 +4149,22 @@
         <v>144</v>
       </c>
       <c r="F78" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H78" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="I78" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="G78" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H78" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I78" s="20" t="s">
-        <v>9</v>
-      </c>
       <c r="J78" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>305</v>
+        <v>27</v>
+      </c>
+      <c r="K78" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -4186,17 +4186,17 @@
       <c r="F79" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="G79" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H79" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I79" s="23"/>
+      <c r="G79" s="23"/>
+      <c r="H79" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="I79" s="3"/>
       <c r="J79" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="K79" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="K79" s="22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="80" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="21" t="s">
@@ -4217,18 +4217,18 @@
       <c r="F80" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="G80" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H80" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="J80" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="K80" s="3" t="s">
-        <v>185</v>
+        <v>27</v>
+      </c>
+      <c r="K80" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -4250,18 +4250,18 @@
       <c r="F81" s="23" t="s">
         <v>259</v>
       </c>
-      <c r="G81" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H81" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I81" s="23"/>
+      <c r="G81" s="23"/>
+      <c r="H81" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>214</v>
+      </c>
       <c r="J81" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>214</v>
+        <v>27</v>
+      </c>
+      <c r="K81" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -4283,18 +4283,18 @@
       <c r="F82" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="G82" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H82" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>238</v>
+      </c>
       <c r="J82" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="K82" s="3" t="s">
-        <v>238</v>
+        <v>27</v>
+      </c>
+      <c r="K82" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -4317,19 +4317,19 @@
         <v>278</v>
       </c>
       <c r="G83" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H83" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I83" s="23" t="s">
         <v>9</v>
       </c>
+      <c r="H83" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>280</v>
+      </c>
       <c r="J83" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="K83" s="3" t="s">
-        <v>280</v>
+        <v>27</v>
+      </c>
+      <c r="K83" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -4340,7 +4340,7 @@
         <v>2035</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D84" s="23" t="s">
         <v>23</v>
@@ -4349,22 +4349,22 @@
         <v>143</v>
       </c>
       <c r="F84" s="23" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="G84" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H84" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I84" s="23" t="s">
         <v>9</v>
       </c>
+      <c r="H84" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>308</v>
+      </c>
       <c r="J84" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="K84" s="3" t="s">
-        <v>310</v>
+        <v>27</v>
+      </c>
+      <c r="K84" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4386,18 +4386,18 @@
       <c r="F85" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="G85" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H85" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="J85" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>181</v>
+        <v>27</v>
+      </c>
+      <c r="K85" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4419,18 +4419,18 @@
       <c r="F86" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="G86" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H86" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="J86" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>217</v>
+        <v>27</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4452,18 +4452,18 @@
       <c r="F87" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="G87" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H87" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="J87" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="K87" s="4" t="s">
-        <v>233</v>
+        <v>27</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4486,19 +4486,19 @@
         <v>275</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H88" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I88" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="H88" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>276</v>
+      </c>
       <c r="J88" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="K88" s="4" t="s">
-        <v>276</v>
+        <v>27</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4509,7 +4509,7 @@
         <v>2035</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>23</v>
@@ -4518,22 +4518,22 @@
         <v>177</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H89" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I89" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="H89" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>314</v>
+      </c>
       <c r="J89" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="K89" s="4" t="s">
-        <v>320</v>
+        <v>27</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
@@ -4553,18 +4553,18 @@
         <v>38</v>
       </c>
       <c r="F90" s="30"/>
-      <c r="G90" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H90" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I90" s="30"/>
+      <c r="G90" s="30"/>
+      <c r="H90" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="J90" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="K90" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+      <c r="K90" s="29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
@@ -4586,18 +4586,18 @@
       <c r="F91" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="G91" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H91" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I91" s="30"/>
+      <c r="G91" s="30"/>
+      <c r="H91" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="J91" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="K91" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
+      </c>
+      <c r="K91" s="29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
@@ -4617,18 +4617,18 @@
         <v>38</v>
       </c>
       <c r="F92" s="30"/>
-      <c r="G92" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H92" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I92" s="30"/>
+      <c r="G92" s="30"/>
+      <c r="H92" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I92" s="30" t="s">
+        <v>53</v>
+      </c>
       <c r="J92" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="K92" s="30" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="K92" s="29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="93" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
@@ -4648,18 +4648,18 @@
         <v>38</v>
       </c>
       <c r="F93" s="30"/>
-      <c r="G93" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H93" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I93" s="30"/>
+      <c r="G93" s="30"/>
+      <c r="H93" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="I93" s="30" t="s">
+        <v>53</v>
+      </c>
       <c r="J93" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="K93" s="30" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="K93" s="29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
@@ -4679,18 +4679,18 @@
         <v>38</v>
       </c>
       <c r="F94" s="30"/>
-      <c r="G94" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H94" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I94" s="30"/>
+      <c r="G94" s="30"/>
+      <c r="H94" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I94" s="30" t="s">
+        <v>53</v>
+      </c>
       <c r="J94" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="K94" s="30" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="K94" s="29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="95" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
@@ -4712,18 +4712,18 @@
       <c r="F95" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="G95" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H95" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I95" s="30"/>
+      <c r="G95" s="30"/>
+      <c r="H95" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="J95" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="K95" s="1" t="s">
-        <v>69</v>
+        <v>27</v>
+      </c>
+      <c r="K95" s="29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
@@ -4745,18 +4745,18 @@
       <c r="F96" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="G96" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H96" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I96" s="16"/>
-      <c r="J96" s="16" t="s">
+      <c r="G96" s="16"/>
+      <c r="H96" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K96" t="s">
+      <c r="I96" t="s">
         <v>29</v>
+      </c>
+      <c r="J96" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K96" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -4778,18 +4778,18 @@
       <c r="F97" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="G97" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H97" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I97" s="16"/>
-      <c r="J97" s="16" t="s">
+      <c r="G97" s="16"/>
+      <c r="H97" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K97" t="s">
+      <c r="I97" t="s">
         <v>31</v>
+      </c>
+      <c r="J97" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K97" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -4811,18 +4811,18 @@
       <c r="F98" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G98" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H98" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I98" s="16"/>
-      <c r="J98" s="16" t="s">
+      <c r="G98" s="16"/>
+      <c r="H98" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K98" t="s">
+      <c r="I98" t="s">
         <v>32</v>
+      </c>
+      <c r="J98" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K98" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
@@ -4844,18 +4844,18 @@
       <c r="F99" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="G99" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H99" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I99" s="16"/>
-      <c r="J99" s="16" t="s">
+      <c r="G99" s="16"/>
+      <c r="H99" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K99" t="s">
+      <c r="I99" t="s">
         <v>33</v>
+      </c>
+      <c r="J99" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K99" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
@@ -4877,18 +4877,18 @@
       <c r="F100" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="G100" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H100" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I100" s="16"/>
-      <c r="J100" s="16" t="s">
+      <c r="G100" s="16"/>
+      <c r="H100" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K100" t="s">
+      <c r="I100" t="s">
         <v>34</v>
+      </c>
+      <c r="J100" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K100" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
@@ -4908,18 +4908,18 @@
         <v>30</v>
       </c>
       <c r="F101" s="33"/>
-      <c r="G101" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H101" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I101" s="16"/>
-      <c r="J101" s="16" t="s">
+      <c r="G101" s="16"/>
+      <c r="H101" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="K101" t="s">
+      <c r="I101" t="s">
         <v>50</v>
+      </c>
+      <c r="J101" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K101" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
@@ -4941,18 +4941,18 @@
       <c r="F102" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="G102" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H102" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I102" s="16"/>
-      <c r="J102" s="16" t="s">
+      <c r="G102" s="16"/>
+      <c r="H102" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="K102" s="34" t="s">
+      <c r="I102" s="34" t="s">
         <v>50</v>
+      </c>
+      <c r="J102" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K102" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
@@ -4974,18 +4974,18 @@
       <c r="F103" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="G103" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H103" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I103" s="16"/>
-      <c r="J103" s="16" t="s">
+      <c r="G103" s="16"/>
+      <c r="H103" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K103" t="s">
+      <c r="I103" t="s">
         <v>51</v>
+      </c>
+      <c r="J103" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K103" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
@@ -5007,18 +5007,18 @@
       <c r="F104" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="G104" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H104" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I104" s="16"/>
-      <c r="J104" s="16" t="s">
+      <c r="G104" s="16"/>
+      <c r="H104" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K104" t="s">
+      <c r="I104" t="s">
         <v>52</v>
+      </c>
+      <c r="J104" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K104" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
@@ -5038,18 +5038,18 @@
         <v>30</v>
       </c>
       <c r="F105" s="33"/>
-      <c r="G105" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H105" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I105" s="16"/>
-      <c r="J105" s="16" t="s">
+      <c r="G105" s="16"/>
+      <c r="H105" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K105" t="s">
+      <c r="I105" t="s">
         <v>52</v>
+      </c>
+      <c r="J105" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K105" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
@@ -5069,18 +5069,18 @@
         <v>30</v>
       </c>
       <c r="F106" s="33"/>
-      <c r="G106" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H106" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I106" s="16"/>
-      <c r="J106" s="16" t="s">
+      <c r="G106" s="16"/>
+      <c r="H106" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K106" t="s">
+      <c r="I106" t="s">
         <v>52</v>
+      </c>
+      <c r="J106" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K106" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
@@ -5100,18 +5100,18 @@
         <v>30</v>
       </c>
       <c r="F107" s="33"/>
-      <c r="G107" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H107" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I107" s="16"/>
-      <c r="J107" s="16" t="s">
+      <c r="G107" s="16"/>
+      <c r="H107" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K107" t="s">
+      <c r="I107" t="s">
         <v>52</v>
+      </c>
+      <c r="J107" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K107" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
@@ -5133,18 +5133,18 @@
       <c r="F108" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="G108" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H108" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I108" s="16"/>
-      <c r="J108" s="16" t="s">
+      <c r="G108" s="16"/>
+      <c r="H108" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="K108" s="35" t="s">
+      <c r="I108" s="35" t="s">
         <v>99</v>
+      </c>
+      <c r="J108" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K108" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
@@ -5166,15 +5166,15 @@
       <c r="F109" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="G109" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H109" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I109" s="16"/>
-      <c r="J109" s="16" t="s">
+      <c r="G109" s="16"/>
+      <c r="H109" s="16" t="s">
         <v>68</v>
+      </c>
+      <c r="J109" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K109" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
@@ -5196,15 +5196,15 @@
       <c r="F110" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="G110" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H110" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I110" s="16"/>
-      <c r="J110" s="16" t="s">
+      <c r="G110" s="16"/>
+      <c r="H110" s="16" t="s">
         <v>68</v>
+      </c>
+      <c r="J110" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K110" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
@@ -5226,15 +5226,15 @@
       <c r="F111" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G111" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H111" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="I111" s="16"/>
-      <c r="J111" s="16" t="s">
+      <c r="G111" s="16"/>
+      <c r="H111" s="16" t="s">
         <v>68</v>
+      </c>
+      <c r="J111" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K111" s="32" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="112" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -5256,18 +5256,18 @@
       <c r="F112" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G112" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H112" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I112" s="7"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I112" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="J112" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="K112" s="4" t="s">
-        <v>104</v>
+        <v>27</v>
+      </c>
+      <c r="K112" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="113" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -5289,58 +5289,58 @@
       <c r="F113" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G113" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H113" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I113" s="7"/>
+      <c r="G113" s="7"/>
+      <c r="H113" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I113" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="J113" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="K113" s="4" t="s">
-        <v>108</v>
+        <v>27</v>
+      </c>
+      <c r="K113" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K90" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
-    <hyperlink ref="K10" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="K95" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="K102" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="K108" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
-    <hyperlink ref="K7" r:id="rId6" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
-    <hyperlink ref="K15" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
-    <hyperlink ref="K16" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
-    <hyperlink ref="K14" r:id="rId9" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{07D1B2DA-E517-4DD9-B4E8-AE0933FD4973}"/>
-    <hyperlink ref="K13" r:id="rId10" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{4A8E9582-524B-46F3-8A76-0C1F5220D214}"/>
-    <hyperlink ref="K12" r:id="rId11" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{E622471D-8EED-401F-9FFF-3C4854166AD2}"/>
-    <hyperlink ref="K33" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
-    <hyperlink ref="K34" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
-    <hyperlink ref="K35" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
-    <hyperlink ref="K36" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
-    <hyperlink ref="K85" r:id="rId16" xr:uid="{C5D42A4A-7D1E-4E61-A6D8-57E8258064CF}"/>
-    <hyperlink ref="K27" r:id="rId17" display="https://app.asana.com/0/1201809392759895/1204199508775563/f" xr:uid="{AD5B4BF6-019A-41E5-B4FF-144AB869AC79}"/>
-    <hyperlink ref="K38" r:id="rId18" display="https://app.asana.com/0/1201809392759895/1204199508775567/f" xr:uid="{4D75E071-693C-4E6B-9BC3-F13FF7899650}"/>
-    <hyperlink ref="K75" r:id="rId19" display="https://app.asana.com/0/1201809392759895/1204199508775554/f" xr:uid="{93FEBC25-3D8F-4C29-A30C-17379D746E6A}"/>
-    <hyperlink ref="K9" r:id="rId20" display="https://app.asana.com/0/0/1204199508775527/f" xr:uid="{F74BF0A2-72BF-4CE6-B53E-B781F9178384}"/>
-    <hyperlink ref="K81" r:id="rId21" display="https://app.asana.com/0/1201809392759895/1204199508775559/f" xr:uid="{22B796F7-F10B-406F-9671-D0DD2372085C}"/>
-    <hyperlink ref="K86" r:id="rId22" display="https://app.asana.com/0/1201809392759895/1204199508775550/f" xr:uid="{7477F2BA-CE56-4250-ACD2-6910E3E300C3}"/>
-    <hyperlink ref="K52" r:id="rId23" display="https://app.asana.com/0/1201809392759895/1203498380299819/f" xr:uid="{D93F0873-C671-4938-A6C2-30B74CB13B5B}"/>
-    <hyperlink ref="K61" r:id="rId24" display="https://app.asana.com/0/1201809392759895/1204220790822201/f" xr:uid="{1F3B0FA4-6BBC-474D-88B3-E82D1113FB80}"/>
-    <hyperlink ref="K28" r:id="rId25" display="https://app.asana.com/0/1201809392759895/1204295579502963/f" xr:uid="{7875DFD5-B0A2-459C-ABF9-F11D4ADD4F71}"/>
-    <hyperlink ref="K39" r:id="rId26" display="https://app.asana.com/0/1201809392759895/1204295579502969/f" xr:uid="{B63AFD9E-EB13-4B90-9FAB-319386521DF8}"/>
-    <hyperlink ref="K62" r:id="rId27" display="https://app.asana.com/0/1201809392759895/1204295579502978/f" xr:uid="{D43A960D-5A0B-4CBA-902D-69F4EB319BB3}"/>
-    <hyperlink ref="K87" r:id="rId28" display="https://app.asana.com/0/1201809392759895/1204286896724186/f" xr:uid="{E7EC1047-9DA4-4F9C-9B0E-D17FAE0F1E7C}"/>
-    <hyperlink ref="K53" r:id="rId29" display="https://app.asana.com/0/1201809392759895/1204295579502973/f" xr:uid="{F1F5C8FB-27AF-4015-BE70-7BAE285B89BD}"/>
-    <hyperlink ref="K82" r:id="rId30" display="https://app.asana.com/0/1201809392759895/1204295579502982/f" xr:uid="{9733EDE0-72F9-4C80-9C31-A649304EDFB2}"/>
-    <hyperlink ref="K76" r:id="rId31" display="https://app.asana.com/0/1201809392759895/1204295579502980/f" xr:uid="{96530962-B1F6-43FD-8386-80D23BCD0DC5}"/>
-    <hyperlink ref="K17" r:id="rId32" display="https://app.asana.com/0/1201809392759895/1204295579503110/f" xr:uid="{D535BCFB-415F-4CB0-9E44-1802BFB9227E}"/>
-    <hyperlink ref="K54" r:id="rId33" display="https://app.asana.com/0/1201809392759895/1204311438003508" xr:uid="{2C5CE002-FBD3-497B-96C2-D3AE6CF1127A}"/>
-    <hyperlink ref="K29" r:id="rId34" display="https://app.asana.com/0/1201809392759895/1204311438003500/f" xr:uid="{CCE9A3E3-3E67-4CD0-9AFB-C48B52AC84C0}"/>
-    <hyperlink ref="K40" r:id="rId35" display="https://app.asana.com/0/1201809392759895/1204311438003504/f" xr:uid="{1BF2101D-1E81-4B8C-973E-389A06EF5483}"/>
+    <hyperlink ref="I90" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="I10" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
+    <hyperlink ref="I95" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="I102" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="I108" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
+    <hyperlink ref="I15" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
+    <hyperlink ref="I16" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
+    <hyperlink ref="I14" r:id="rId9" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{07D1B2DA-E517-4DD9-B4E8-AE0933FD4973}"/>
+    <hyperlink ref="I13" r:id="rId10" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{4A8E9582-524B-46F3-8A76-0C1F5220D214}"/>
+    <hyperlink ref="I12" r:id="rId11" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{E622471D-8EED-401F-9FFF-3C4854166AD2}"/>
+    <hyperlink ref="I33" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
+    <hyperlink ref="I34" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
+    <hyperlink ref="I35" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
+    <hyperlink ref="I36" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
+    <hyperlink ref="I85" r:id="rId16" xr:uid="{C5D42A4A-7D1E-4E61-A6D8-57E8258064CF}"/>
+    <hyperlink ref="I27" r:id="rId17" display="https://app.asana.com/0/1201809392759895/1204199508775563/f" xr:uid="{AD5B4BF6-019A-41E5-B4FF-144AB869AC79}"/>
+    <hyperlink ref="I38" r:id="rId18" display="https://app.asana.com/0/1201809392759895/1204199508775567/f" xr:uid="{4D75E071-693C-4E6B-9BC3-F13FF7899650}"/>
+    <hyperlink ref="I75" r:id="rId19" display="https://app.asana.com/0/1201809392759895/1204199508775554/f" xr:uid="{93FEBC25-3D8F-4C29-A30C-17379D746E6A}"/>
+    <hyperlink ref="I9" r:id="rId20" display="https://app.asana.com/0/0/1204199508775527/f" xr:uid="{F74BF0A2-72BF-4CE6-B53E-B781F9178384}"/>
+    <hyperlink ref="I81" r:id="rId21" display="https://app.asana.com/0/1201809392759895/1204199508775559/f" xr:uid="{22B796F7-F10B-406F-9671-D0DD2372085C}"/>
+    <hyperlink ref="I86" r:id="rId22" display="https://app.asana.com/0/1201809392759895/1204199508775550/f" xr:uid="{7477F2BA-CE56-4250-ACD2-6910E3E300C3}"/>
+    <hyperlink ref="I52" r:id="rId23" display="https://app.asana.com/0/1201809392759895/1203498380299819/f" xr:uid="{D93F0873-C671-4938-A6C2-30B74CB13B5B}"/>
+    <hyperlink ref="I61" r:id="rId24" display="https://app.asana.com/0/1201809392759895/1204220790822201/f" xr:uid="{1F3B0FA4-6BBC-474D-88B3-E82D1113FB80}"/>
+    <hyperlink ref="I28" r:id="rId25" display="https://app.asana.com/0/1201809392759895/1204295579502963/f" xr:uid="{7875DFD5-B0A2-459C-ABF9-F11D4ADD4F71}"/>
+    <hyperlink ref="I39" r:id="rId26" display="https://app.asana.com/0/1201809392759895/1204295579502969/f" xr:uid="{B63AFD9E-EB13-4B90-9FAB-319386521DF8}"/>
+    <hyperlink ref="I62" r:id="rId27" display="https://app.asana.com/0/1201809392759895/1204295579502978/f" xr:uid="{D43A960D-5A0B-4CBA-902D-69F4EB319BB3}"/>
+    <hyperlink ref="I87" r:id="rId28" display="https://app.asana.com/0/1201809392759895/1204286896724186/f" xr:uid="{E7EC1047-9DA4-4F9C-9B0E-D17FAE0F1E7C}"/>
+    <hyperlink ref="I53" r:id="rId29" display="https://app.asana.com/0/1201809392759895/1204295579502973/f" xr:uid="{F1F5C8FB-27AF-4015-BE70-7BAE285B89BD}"/>
+    <hyperlink ref="I82" r:id="rId30" display="https://app.asana.com/0/1201809392759895/1204295579502982/f" xr:uid="{9733EDE0-72F9-4C80-9C31-A649304EDFB2}"/>
+    <hyperlink ref="I76" r:id="rId31" display="https://app.asana.com/0/1201809392759895/1204295579502980/f" xr:uid="{96530962-B1F6-43FD-8386-80D23BCD0DC5}"/>
+    <hyperlink ref="I17" r:id="rId32" display="https://app.asana.com/0/1201809392759895/1204295579503110/f" xr:uid="{D535BCFB-415F-4CB0-9E44-1802BFB9227E}"/>
+    <hyperlink ref="I54" r:id="rId33" display="https://app.asana.com/0/1201809392759895/1204311438003508" xr:uid="{2C5CE002-FBD3-497B-96C2-D3AE6CF1127A}"/>
+    <hyperlink ref="I29" r:id="rId34" display="https://app.asana.com/0/1201809392759895/1204311438003500/f" xr:uid="{CCE9A3E3-3E67-4CD0-9AFB-C48B52AC84C0}"/>
+    <hyperlink ref="I40" r:id="rId35" display="https://app.asana.com/0/1201809392759895/1204311438003504/f" xr:uid="{1BF2101D-1E81-4B8C-973E-389A06EF5483}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId36"/>

</xml_diff>

<commit_message>
Missing space in Pathway 1a short name
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570A14BF-6DA2-433E-A947-5E518924E769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E558D149-15C4-4CF3-9480-EFEEE9E60102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="4350" windowWidth="26730" windowHeight="15825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="4350" windowWidth="23565" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -1025,9 +1025,6 @@
     <t>NoProject v10</t>
   </si>
   <si>
-    <t>Pathway1a (NP10)</t>
-  </si>
-  <si>
     <t>Pathway 1b (NP10)</t>
   </si>
   <si>
@@ -1050,6 +1047,9 @@
   </si>
   <si>
     <t>Pathway 2a with 20pct art toll (NP10)</t>
+  </si>
+  <si>
+    <t>Pathway 1a (NP10)</t>
   </si>
 </sst>
 </file>
@@ -1601,8 +1601,8 @@
   <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2621,7 +2621,7 @@
         <v>142</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>9</v>
@@ -3234,7 +3234,7 @@
         <v>138</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G51" s="23" t="s">
         <v>9</v>
@@ -3475,7 +3475,7 @@
         <v>219</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>9</v>
@@ -3510,7 +3510,7 @@
         <v>219</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G59" s="13" t="s">
         <v>9</v>
@@ -3782,7 +3782,7 @@
         <v>139</v>
       </c>
       <c r="F67" s="26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G67" s="26" t="s">
         <v>9</v>
@@ -3817,7 +3817,7 @@
         <v>139</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G68" s="26" t="s">
         <v>9</v>
@@ -4149,7 +4149,7 @@
         <v>144</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>9</v>
@@ -4349,7 +4349,7 @@
         <v>143</v>
       </c>
       <c r="F84" s="23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G84" s="23" t="s">
         <v>9</v>
@@ -4518,7 +4518,7 @@
         <v>177</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Demoting some runs from current
https://app.asana.com/0/1201809392759895/1204436956308953/f
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E558D149-15C4-4CF3-9480-EFEEE9E60102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F941BD-9326-43F8-9937-39E48B055B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="4350" windowWidth="23565" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7410" yWindow="1575" windowWidth="22350" windowHeight="18090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$I$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$113</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="338">
   <si>
     <t>No Project</t>
   </si>
@@ -1601,15 +1601,15 @@
   <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="38.28515625" customWidth="1"/>
     <col min="8" max="8" width="47.42578125" customWidth="1"/>
@@ -2183,9 +2183,7 @@
       <c r="F18" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="G18" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="G18" s="20"/>
       <c r="H18" s="20" t="s">
         <v>240</v>
       </c>
@@ -2588,9 +2586,7 @@
       <c r="F31" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
         <v>227</v>
       </c>
@@ -3106,9 +3102,7 @@
       <c r="F47" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="G47" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="G47" s="23"/>
       <c r="H47" s="23" t="s">
         <v>190</v>
       </c>
@@ -3337,9 +3331,7 @@
       <c r="F54" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="G54" s="13" t="s">
-        <v>9</v>
-      </c>
+      <c r="G54" s="13"/>
       <c r="H54" s="13" t="s">
         <v>220</v>
       </c>
@@ -3372,9 +3364,7 @@
       <c r="F55" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="G55" s="13" t="s">
-        <v>9</v>
-      </c>
+      <c r="G55" s="13"/>
       <c r="H55" s="13" t="s">
         <v>220</v>
       </c>
@@ -3407,9 +3397,7 @@
       <c r="F56" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="G56" s="13" t="s">
-        <v>9</v>
-      </c>
+      <c r="G56" s="13"/>
       <c r="H56" s="13" t="s">
         <v>220</v>
       </c>
@@ -3442,9 +3430,7 @@
       <c r="F57" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="G57" s="13" t="s">
-        <v>9</v>
-      </c>
+      <c r="G57" s="13"/>
       <c r="H57" s="13" t="s">
         <v>220</v>
       </c>
@@ -3644,9 +3630,7 @@
       <c r="F63" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="G63" s="26" t="s">
-        <v>9</v>
-      </c>
+      <c r="G63" s="26"/>
       <c r="H63" s="26" t="s">
         <v>223</v>
       </c>
@@ -3679,9 +3663,7 @@
       <c r="F64" s="26" t="s">
         <v>326</v>
       </c>
-      <c r="G64" s="26" t="s">
-        <v>9</v>
-      </c>
+      <c r="G64" s="26"/>
       <c r="H64" s="26" t="s">
         <v>223</v>
       </c>
@@ -3714,9 +3696,7 @@
       <c r="F65" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="G65" s="26" t="s">
-        <v>9</v>
-      </c>
+      <c r="G65" s="26"/>
       <c r="H65" s="26" t="s">
         <v>223</v>
       </c>
@@ -3749,9 +3729,7 @@
       <c r="F66" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="G66" s="26" t="s">
-        <v>9</v>
-      </c>
+      <c r="G66" s="26"/>
       <c r="H66" s="26" t="s">
         <v>223</v>
       </c>
@@ -4116,9 +4094,7 @@
       <c r="F77" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="G77" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="G77" s="20"/>
       <c r="H77" s="20" t="s">
         <v>201</v>
       </c>
@@ -4316,9 +4292,7 @@
       <c r="F83" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="G83" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="G83" s="23"/>
       <c r="H83" s="23" t="s">
         <v>213</v>
       </c>
@@ -4485,9 +4459,7 @@
       <c r="F88" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="G88" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="G88" s="7"/>
       <c r="H88" s="7" t="s">
         <v>216</v>
       </c>
@@ -5304,6 +5276,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K113" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I90" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>

</xml_diff>

<commit_message>
Adding back a few to current per Anup
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F941BD-9326-43F8-9937-39E48B055B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6422CC-A4C6-466B-BA20-D40CE96135D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="1575" windowWidth="22350" windowHeight="18090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15075" yWindow="4605" windowWidth="22935" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="338">
   <si>
     <t>No Project</t>
   </si>
@@ -1602,7 +1602,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2518,7 +2518,9 @@
       <c r="F29" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="G29" s="7"/>
+      <c r="G29" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H29" s="7" t="s">
         <v>227</v>
       </c>
@@ -2877,7 +2879,9 @@
       <c r="F40" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="G40" s="23"/>
+      <c r="G40" s="23" t="s">
+        <v>9</v>
+      </c>
       <c r="H40" s="23" t="s">
         <v>199</v>
       </c>
@@ -3364,7 +3368,9 @@
       <c r="F55" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="G55" s="13"/>
+      <c r="G55" s="13" t="s">
+        <v>9</v>
+      </c>
       <c r="H55" s="13" t="s">
         <v>220</v>
       </c>
@@ -3663,7 +3669,9 @@
       <c r="F64" s="26" t="s">
         <v>326</v>
       </c>
-      <c r="G64" s="26"/>
+      <c r="G64" s="26" t="s">
+        <v>9</v>
+      </c>
       <c r="H64" s="26" t="s">
         <v>223</v>
       </c>
@@ -4459,7 +4467,9 @@
       <c r="F88" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="G88" s="7"/>
+      <c r="G88" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H88" s="7" t="s">
         <v>216</v>
       </c>

</xml_diff>

<commit_message>
Remove NP10 from short names
The NP is in the directory and it's not meaningful to most ppl
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F060594-CACF-4979-86AB-DD09FC9FD064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEAB1B4-DE42-4825-B136-0DA76E373137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="-1440" windowWidth="14400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="23760" windowHeight="14130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="370">
   <si>
     <t>No Project</t>
   </si>
@@ -1022,33 +1022,6 @@
     <t>NoProject v10</t>
   </si>
   <si>
-    <t>Pathway 1b (NP10)</t>
-  </si>
-  <si>
-    <t>Pathway 2a with 10pct art toll (NP10)</t>
-  </si>
-  <si>
-    <t>Pathway 2b with 10pct art toll (NP10)</t>
-  </si>
-  <si>
-    <t>Pathway 3a (NP10)</t>
-  </si>
-  <si>
-    <t>Pathway 3b (NP10)</t>
-  </si>
-  <si>
-    <t>Pathway 4 - No New Pricing (NP10)</t>
-  </si>
-  <si>
-    <t>Pathway 2b with 20pct art toll (NP10)</t>
-  </si>
-  <si>
-    <t>Pathway 2a with 20pct art toll (NP10)</t>
-  </si>
-  <si>
-    <t>Pathway 1a (NP10)</t>
-  </si>
-  <si>
     <t>2035_TM152_NGF_NP10_Path1a_02</t>
   </si>
   <si>
@@ -1127,31 +1100,52 @@
     <t>directory</t>
   </si>
   <si>
-    <t>Pathway 1a (NP10, more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 1b (NP10, more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 2a with 20pct art toll (NP10, more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 2a with 10pct art toll (NP10, more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 2b with 20pct art toll (NP10, more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 2b with 10pct art toll (NP10, more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 3a (NP10, more VZ, less trn)</t>
-  </si>
-  <si>
-    <t>Pathway 3b (NP10, more VZ, less trn)</t>
-  </si>
-  <si>
-    <t>Pathway 4 - No New Pricing  (NP10, more VZ, less trn)</t>
+    <t>Pathway 1a (more VZ, less trn, lower toll)</t>
+  </si>
+  <si>
+    <t>Pathway 1b (more VZ, less trn, lower toll)</t>
+  </si>
+  <si>
+    <t>Pathway 2a with 20pct art toll</t>
+  </si>
+  <si>
+    <t>Pathway 2a with 10pct art toll</t>
+  </si>
+  <si>
+    <t>Pathway 2a with 20pct art toll (more VZ, less trn, lower toll)</t>
+  </si>
+  <si>
+    <t>Pathway 2a with 10pct art toll (more VZ, less trn, lower toll)</t>
+  </si>
+  <si>
+    <t>Pathway 2b with 20pct art toll</t>
+  </si>
+  <si>
+    <t>Pathway 2b with 10pct art toll</t>
+  </si>
+  <si>
+    <t>Pathway 2b with 20pct art toll (more VZ, less trn, lower toll)</t>
+  </si>
+  <si>
+    <t>Pathway 2b with 10pct art toll (more VZ, less trn, lower toll)</t>
+  </si>
+  <si>
+    <t>Pathway 3a (NP07)</t>
+  </si>
+  <si>
+    <t>Pathway 3a (more VZ, less trn)</t>
+  </si>
+  <si>
+    <t>Pathway 3b (NP07)</t>
+  </si>
+  <si>
+    <t>Pathway 3b (more VZ, less trn)</t>
+  </si>
+  <si>
+    <t>Pathway 4 - No New Pricing (NP07)</t>
+  </si>
+  <si>
+    <t>Pathway 4 - No New Pricing (more VZ, less trn)</t>
   </si>
 </sst>
 </file>
@@ -1702,9 +1696,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1727,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>4</v>
@@ -2721,7 +2715,7 @@
         <v>141</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>336</v>
+        <v>141</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>8</v>
@@ -2747,7 +2741,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>22</v>
@@ -2756,16 +2750,16 @@
         <v>141</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="J33" s="7" t="s">
         <v>26</v>
@@ -3369,7 +3363,7 @@
         <v>137</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>328</v>
+        <v>137</v>
       </c>
       <c r="G52" s="23" t="s">
         <v>8</v>
@@ -3395,7 +3389,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>22</v>
@@ -3404,16 +3398,16 @@
         <v>137</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="G53" s="23" t="s">
         <v>8</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="J53" s="23" t="s">
         <v>26</v>
@@ -3637,7 +3631,7 @@
         <v>218</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>335</v>
+        <v>356</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>8</v>
@@ -3672,7 +3666,7 @@
         <v>218</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>329</v>
+        <v>357</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>8</v>
@@ -3698,7 +3692,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D62" s="13" t="s">
         <v>22</v>
@@ -3707,16 +3701,16 @@
         <v>218</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>8</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="I62" s="37" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="J62" s="13" t="s">
         <v>26</v>
@@ -3733,7 +3727,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>22</v>
@@ -3742,16 +3736,16 @@
         <v>218</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>8</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="I63" s="37" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="J63" s="13" t="s">
         <v>26</v>
@@ -4006,7 +4000,7 @@
         <v>138</v>
       </c>
       <c r="F71" s="26" t="s">
-        <v>334</v>
+        <v>360</v>
       </c>
       <c r="G71" s="26" t="s">
         <v>8</v>
@@ -4041,7 +4035,7 @@
         <v>138</v>
       </c>
       <c r="F72" s="26" t="s">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="G72" s="26" t="s">
         <v>8</v>
@@ -4067,7 +4061,7 @@
         <v>2035</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D73" s="26" t="s">
         <v>22</v>
@@ -4076,16 +4070,16 @@
         <v>138</v>
       </c>
       <c r="F73" s="26" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="G73" s="26" t="s">
         <v>8</v>
       </c>
       <c r="H73" s="26" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="I73" s="38" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="J73" s="26" t="s">
         <v>26</v>
@@ -4102,7 +4096,7 @@
         <v>2035</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D74" s="26" t="s">
         <v>22</v>
@@ -4111,16 +4105,16 @@
         <v>138</v>
       </c>
       <c r="F74" s="26" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="G74" s="26" t="s">
         <v>8</v>
       </c>
       <c r="H74" s="26" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="I74" s="38" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="J74" s="26" t="s">
         <v>26</v>
@@ -4278,7 +4272,7 @@
         <v>143</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>143</v>
+        <v>364</v>
       </c>
       <c r="G79" s="20"/>
       <c r="H79" s="20" t="s">
@@ -4309,7 +4303,7 @@
         <v>143</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>143</v>
+        <v>364</v>
       </c>
       <c r="G80" s="20"/>
       <c r="H80" s="20" t="s">
@@ -4441,7 +4435,7 @@
         <v>143</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>331</v>
+        <v>143</v>
       </c>
       <c r="G84" s="20" t="s">
         <v>8</v>
@@ -4467,7 +4461,7 @@
         <v>2035</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D85" s="20" t="s">
         <v>22</v>
@@ -4476,16 +4470,16 @@
         <v>143</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>8</v>
       </c>
       <c r="H85" s="20" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="J85" s="20" t="s">
         <v>26</v>
@@ -4511,7 +4505,7 @@
         <v>142</v>
       </c>
       <c r="F86" s="23" t="s">
-        <v>142</v>
+        <v>366</v>
       </c>
       <c r="G86" s="23"/>
       <c r="H86" s="23" t="s">
@@ -4542,7 +4536,7 @@
         <v>142</v>
       </c>
       <c r="F87" s="23" t="s">
-        <v>142</v>
+        <v>366</v>
       </c>
       <c r="G87" s="23"/>
       <c r="H87" s="23" t="s">
@@ -4674,7 +4668,7 @@
         <v>142</v>
       </c>
       <c r="F91" s="23" t="s">
-        <v>332</v>
+        <v>142</v>
       </c>
       <c r="G91" s="23" t="s">
         <v>8</v>
@@ -4700,7 +4694,7 @@
         <v>2035</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="D92" s="23" t="s">
         <v>22</v>
@@ -4709,16 +4703,16 @@
         <v>142</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G92" s="23" t="s">
         <v>8</v>
       </c>
       <c r="H92" s="23" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="J92" s="23" t="s">
         <v>26</v>
@@ -4744,7 +4738,7 @@
         <v>176</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>177</v>
+        <v>368</v>
       </c>
       <c r="G93" s="7"/>
       <c r="H93" s="7" t="s">
@@ -4876,7 +4870,7 @@
         <v>176</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>333</v>
+        <v>177</v>
       </c>
       <c r="G97" s="7" t="s">
         <v>8</v>
@@ -4902,7 +4896,7 @@
         <v>2035</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>22</v>
@@ -4911,16 +4905,16 @@
         <v>176</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G98" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="J98" s="7" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Added 2015_TM152_NGF_06 (not current)
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEAB1B4-DE42-4825-B136-0DA76E373137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4A1688-56E7-4FA5-8F1F-75A45D39CA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="23760" windowHeight="14130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="7065" windowWidth="21570" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$123</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="373">
   <si>
     <t>No Project</t>
   </si>
@@ -1146,6 +1146,15 @@
   </si>
   <si>
     <t>Pathway 4 - No New Pricing (more VZ, less trn)</t>
+  </si>
+  <si>
+    <t>2015_TM152_NGF_06</t>
+  </si>
+  <si>
+    <t>2015 base year (exp PNR fix)</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1204222536302922/f</t>
   </si>
 </sst>
 </file>
@@ -1694,11 +1703,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K122"/>
+  <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1937,34 +1946,37 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2035</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="J8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>27</v>
+    <row r="8" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="15">
+        <v>2015</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1975,59 +1987,58 @@
         <v>2035</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="19" t="s">
+      <c r="J10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2039,7 +2050,7 @@
         <v>2035</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>22</v>
@@ -2047,15 +2058,13 @@
       <c r="E11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>85</v>
-      </c>
+      <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>26</v>
@@ -2072,7 +2081,7 @@
         <v>2035</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>22</v>
@@ -2080,13 +2089,15 @@
       <c r="E12" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="20"/>
+      <c r="F12" s="20" t="s">
+        <v>85</v>
+      </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="J12" s="20" t="s">
         <v>26</v>
@@ -2103,7 +2114,7 @@
         <v>2035</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>22</v>
@@ -2111,9 +2122,7 @@
       <c r="E13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>118</v>
-      </c>
+      <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20" t="s">
         <v>108</v>
@@ -2136,7 +2145,7 @@
         <v>2035</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>22</v>
@@ -2145,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20" t="s">
@@ -2169,7 +2178,7 @@
         <v>2035</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>22</v>
@@ -2178,14 +2187,14 @@
         <v>0</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20" t="s">
         <v>108</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="J15" s="20" t="s">
         <v>26</v>
@@ -2202,7 +2211,7 @@
         <v>2035</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>22</v>
@@ -2211,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>250</v>
+        <v>122</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20" t="s">
@@ -2235,7 +2244,7 @@
         <v>2035</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>241</v>
+        <v>113</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>22</v>
@@ -2244,14 +2253,14 @@
         <v>0</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20" t="s">
-        <v>239</v>
+        <v>108</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>240</v>
+        <v>114</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>26</v>
@@ -2268,7 +2277,7 @@
         <v>2035</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>22</v>
@@ -2277,14 +2286,14 @@
         <v>0</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>326</v>
+        <v>112</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20" t="s">
         <v>239</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>281</v>
+        <v>240</v>
       </c>
       <c r="J18" s="20" t="s">
         <v>26</v>
@@ -2301,7 +2310,7 @@
         <v>2035</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>22</v>
@@ -2310,50 +2319,54 @@
         <v>0</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>8</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="G19" s="20"/>
       <c r="H19" s="20" t="s">
         <v>239</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="J19" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="6">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="6" t="s">
+      <c r="J20" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="19" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2365,7 +2378,7 @@
         <v>2035</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>22</v>
@@ -2376,7 +2389,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="7" t="s">
@@ -2394,7 +2407,7 @@
         <v>2035</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>22</v>
@@ -2405,7 +2418,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="7" t="s">
@@ -2423,7 +2436,7 @@
         <v>2035</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>22</v>
@@ -2434,7 +2447,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="7" t="s">
@@ -2452,7 +2465,7 @@
         <v>2035</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>22</v>
@@ -2463,7 +2476,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="7" t="s">
@@ -2481,7 +2494,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>22</v>
@@ -2510,7 +2523,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>22</v>
@@ -2539,7 +2552,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>22</v>
@@ -2550,11 +2563,9 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>195</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="I27" s="4"/>
       <c r="J27" s="7" t="s">
         <v>26</v>
       </c>
@@ -2570,7 +2581,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>22</v>
@@ -2578,15 +2589,13 @@
       <c r="E28" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>251</v>
-      </c>
+      <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>26</v>
@@ -2603,7 +2612,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>22</v>
@@ -2612,16 +2621,14 @@
         <v>141</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="G29" s="7"/>
       <c r="H29" s="7" t="s">
         <v>226</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>26</v>
@@ -2638,7 +2645,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>22</v>
@@ -2647,7 +2654,7 @@
         <v>141</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>8</v>
@@ -2656,7 +2663,7 @@
         <v>226</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>26</v>
@@ -2673,7 +2680,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>22</v>
@@ -2682,14 +2689,16 @@
         <v>141</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="G31" s="7"/>
+        <v>268</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="H31" s="7" t="s">
         <v>226</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="J31" s="7" t="s">
         <v>26</v>
@@ -2706,7 +2715,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>314</v>
+        <v>284</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>22</v>
@@ -2715,16 +2724,14 @@
         <v>141</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="G32" s="7"/>
       <c r="H32" s="7" t="s">
         <v>226</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>315</v>
+        <v>286</v>
       </c>
       <c r="J32" s="7" t="s">
         <v>26</v>
@@ -2741,7 +2748,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>22</v>
@@ -2750,52 +2757,56 @@
         <v>141</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>354</v>
+        <v>141</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H33" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I34" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="J33" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="J34" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K34" s="22" t="s">
+      <c r="J34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K34" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2807,7 +2818,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>22</v>
@@ -2821,7 +2832,7 @@
         <v>111</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J35" s="23" t="s">
         <v>26</v>
@@ -2838,7 +2849,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>22</v>
@@ -2869,7 +2880,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>22</v>
@@ -2877,15 +2888,13 @@
       <c r="E37" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="F37" s="23" t="s">
-        <v>130</v>
-      </c>
+      <c r="F37" s="23"/>
       <c r="G37" s="23"/>
       <c r="H37" s="23" t="s">
         <v>111</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J37" s="23" t="s">
         <v>26</v>
@@ -2902,7 +2911,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="D38" s="23" t="s">
         <v>22</v>
@@ -2911,13 +2920,15 @@
         <v>137</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>178</v>
+        <v>130</v>
       </c>
       <c r="G38" s="23"/>
       <c r="H38" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="I38" s="3"/>
+      <c r="I38" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="J38" s="23" t="s">
         <v>26</v>
       </c>
@@ -2933,7 +2944,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D39" s="23" t="s">
         <v>22</v>
@@ -2946,11 +2957,9 @@
       </c>
       <c r="G39" s="23"/>
       <c r="H39" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>197</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I39" s="3"/>
       <c r="J39" s="23" t="s">
         <v>26</v>
       </c>
@@ -2966,7 +2975,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="D40" s="23" t="s">
         <v>22</v>
@@ -2975,14 +2984,14 @@
         <v>137</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>253</v>
+        <v>178</v>
       </c>
       <c r="G40" s="23"/>
       <c r="H40" s="23" t="s">
         <v>198</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="J40" s="23" t="s">
         <v>26</v>
@@ -2999,7 +3008,7 @@
         <v>2035</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>22</v>
@@ -3008,16 +3017,14 @@
         <v>137</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>254</v>
-      </c>
-      <c r="G41" s="23" t="s">
-        <v>8</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="G41" s="23"/>
       <c r="H41" s="23" t="s">
         <v>198</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="J41" s="23" t="s">
         <v>26</v>
@@ -3034,7 +3041,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="D42" s="23" t="s">
         <v>22</v>
@@ -3043,7 +3050,7 @@
         <v>137</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="G42" s="23" t="s">
         <v>8</v>
@@ -3052,7 +3059,7 @@
         <v>198</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="J42" s="23" t="s">
         <v>26</v>
@@ -3069,7 +3076,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>131</v>
+        <v>270</v>
       </c>
       <c r="D43" s="23" t="s">
         <v>22</v>
@@ -3078,13 +3085,17 @@
         <v>137</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="G43" s="23"/>
+        <v>271</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>8</v>
+      </c>
       <c r="H43" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="I43" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="J43" s="23" t="s">
         <v>26</v>
       </c>
@@ -3100,7 +3111,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>22</v>
@@ -3109,7 +3120,7 @@
         <v>137</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G44" s="23"/>
       <c r="H44" s="23" t="s">
@@ -3131,7 +3142,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>22</v>
@@ -3140,7 +3151,7 @@
         <v>137</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G45" s="23"/>
       <c r="H45" s="23" t="s">
@@ -3162,7 +3173,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>22</v>
@@ -3171,7 +3182,7 @@
         <v>137</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>202</v>
+        <v>163</v>
       </c>
       <c r="G46" s="23"/>
       <c r="H46" s="23" t="s">
@@ -3193,7 +3204,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="D47" s="23" t="s">
         <v>22</v>
@@ -3202,15 +3213,13 @@
         <v>137</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G47" s="23"/>
       <c r="H47" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>192</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I47" s="3"/>
       <c r="J47" s="23" t="s">
         <v>26</v>
       </c>
@@ -3226,7 +3235,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>287</v>
+        <v>191</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>22</v>
@@ -3235,14 +3244,14 @@
         <v>137</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>288</v>
+        <v>203</v>
       </c>
       <c r="G48" s="23"/>
       <c r="H48" s="23" t="s">
         <v>189</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>289</v>
+        <v>192</v>
       </c>
       <c r="J48" s="23" t="s">
         <v>26</v>
@@ -3259,7 +3268,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>135</v>
+        <v>287</v>
       </c>
       <c r="D49" s="23" t="s">
         <v>22</v>
@@ -3268,13 +3277,15 @@
         <v>137</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>204</v>
+        <v>288</v>
       </c>
       <c r="G49" s="23"/>
       <c r="H49" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="I49" s="3"/>
+        <v>189</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>289</v>
+      </c>
       <c r="J49" s="23" t="s">
         <v>26</v>
       </c>
@@ -3290,7 +3301,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D50" s="23" t="s">
         <v>22</v>
@@ -3299,7 +3310,7 @@
         <v>137</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G50" s="23"/>
       <c r="H50" s="23" t="s">
@@ -3321,7 +3332,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>188</v>
+        <v>134</v>
       </c>
       <c r="D51" s="23" t="s">
         <v>22</v>
@@ -3330,15 +3341,13 @@
         <v>137</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G51" s="23"/>
       <c r="H51" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>190</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I51" s="3"/>
       <c r="J51" s="23" t="s">
         <v>26</v>
       </c>
@@ -3354,7 +3363,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>304</v>
+        <v>188</v>
       </c>
       <c r="D52" s="23" t="s">
         <v>22</v>
@@ -3363,16 +3372,14 @@
         <v>137</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="G52" s="23" t="s">
-        <v>8</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="G52" s="23"/>
       <c r="H52" s="23" t="s">
         <v>189</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>305</v>
+        <v>190</v>
       </c>
       <c r="J52" s="23" t="s">
         <v>26</v>
@@ -3389,7 +3396,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>22</v>
@@ -3398,54 +3405,56 @@
         <v>137</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>355</v>
+        <v>137</v>
       </c>
       <c r="G53" s="23" t="s">
         <v>8</v>
       </c>
       <c r="H53" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="J53" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K53" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>331</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="F54" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="G54" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="I54" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="J53" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K53" s="22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B54" s="12">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="I54" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K54" s="12" t="s">
+      <c r="J54" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K54" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3457,7 +3466,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>22</v>
@@ -3466,14 +3475,14 @@
         <v>218</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>265</v>
+        <v>218</v>
       </c>
       <c r="G55" s="13"/>
       <c r="H55" s="13" t="s">
         <v>219</v>
       </c>
       <c r="I55" s="37" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="J55" s="13" t="s">
         <v>26</v>
@@ -3490,7 +3499,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>22</v>
@@ -3499,14 +3508,14 @@
         <v>218</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>322</v>
+        <v>265</v>
       </c>
       <c r="G56" s="13"/>
       <c r="H56" s="13" t="s">
         <v>219</v>
       </c>
       <c r="I56" s="37" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="J56" s="13" t="s">
         <v>26</v>
@@ -3523,7 +3532,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="D57" s="13" t="s">
         <v>22</v>
@@ -3532,14 +3541,14 @@
         <v>218</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G57" s="13"/>
       <c r="H57" s="13" t="s">
         <v>219</v>
       </c>
       <c r="I57" s="37" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="J57" s="13" t="s">
         <v>26</v>
@@ -3556,7 +3565,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>290</v>
+        <v>262</v>
       </c>
       <c r="D58" s="13" t="s">
         <v>22</v>
@@ -3565,14 +3574,14 @@
         <v>218</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>292</v>
+        <v>323</v>
       </c>
       <c r="G58" s="13"/>
       <c r="H58" s="13" t="s">
         <v>219</v>
       </c>
       <c r="I58" s="37" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="J58" s="13" t="s">
         <v>26</v>
@@ -3589,7 +3598,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D59" s="13" t="s">
         <v>22</v>
@@ -3598,14 +3607,14 @@
         <v>218</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G59" s="13"/>
       <c r="H59" s="13" t="s">
         <v>219</v>
       </c>
       <c r="I59" s="37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J59" s="13" t="s">
         <v>26</v>
@@ -3622,7 +3631,7 @@
         <v>2035</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="D60" s="13" t="s">
         <v>22</v>
@@ -3631,16 +3640,14 @@
         <v>218</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>8</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="G60" s="13"/>
       <c r="H60" s="13" t="s">
         <v>219</v>
       </c>
       <c r="I60" s="37" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="J60" s="13" t="s">
         <v>26</v>
@@ -3657,7 +3664,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="D61" s="13" t="s">
         <v>22</v>
@@ -3666,7 +3673,7 @@
         <v>218</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>8</v>
@@ -3675,7 +3682,7 @@
         <v>219</v>
       </c>
       <c r="I61" s="37" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="J61" s="13" t="s">
         <v>26</v>
@@ -3692,7 +3699,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="D62" s="13" t="s">
         <v>22</v>
@@ -3701,16 +3708,16 @@
         <v>218</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>8</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>336</v>
+        <v>219</v>
       </c>
       <c r="I62" s="37" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="J62" s="13" t="s">
         <v>26</v>
@@ -3727,7 +3734,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>22</v>
@@ -3736,7 +3743,7 @@
         <v>218</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>8</v>
@@ -3745,43 +3752,47 @@
         <v>336</v>
       </c>
       <c r="I63" s="37" t="s">
+        <v>337</v>
+      </c>
+      <c r="J63" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K63" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" s="12">
+        <v>2035</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="I64" s="37" t="s">
         <v>338</v>
       </c>
-      <c r="J63" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K63" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B64" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C64" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="D64" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E64" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="F64" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="G64" s="26"/>
-      <c r="H64" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="I64" s="27"/>
-      <c r="J64" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="K64" s="25" t="s">
+      <c r="J64" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K64" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3793,7 +3804,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>221</v>
+        <v>139</v>
       </c>
       <c r="D65" s="26" t="s">
         <v>22</v>
@@ -3802,15 +3813,13 @@
         <v>138</v>
       </c>
       <c r="F65" s="26" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G65" s="26"/>
       <c r="H65" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="I65" s="38" t="s">
-        <v>223</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="I65" s="27"/>
       <c r="J65" s="26" t="s">
         <v>26</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D66" s="26" t="s">
         <v>22</v>
@@ -3835,14 +3844,14 @@
         <v>138</v>
       </c>
       <c r="F66" s="26" t="s">
-        <v>255</v>
+        <v>138</v>
       </c>
       <c r="G66" s="26"/>
       <c r="H66" s="26" t="s">
         <v>222</v>
       </c>
       <c r="I66" s="38" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="J66" s="26" t="s">
         <v>26</v>
@@ -3859,7 +3868,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="D67" s="26" t="s">
         <v>22</v>
@@ -3868,14 +3877,14 @@
         <v>138</v>
       </c>
       <c r="F67" s="26" t="s">
-        <v>324</v>
+        <v>255</v>
       </c>
       <c r="G67" s="26"/>
       <c r="H67" s="26" t="s">
         <v>222</v>
       </c>
       <c r="I67" s="38" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="J67" s="26" t="s">
         <v>26</v>
@@ -3892,7 +3901,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="D68" s="26" t="s">
         <v>22</v>
@@ -3901,14 +3910,14 @@
         <v>138</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G68" s="26"/>
       <c r="H68" s="26" t="s">
         <v>222</v>
       </c>
       <c r="I68" s="38" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="J68" s="26" t="s">
         <v>26</v>
@@ -3925,7 +3934,7 @@
         <v>2035</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="D69" s="26" t="s">
         <v>22</v>
@@ -3934,14 +3943,14 @@
         <v>138</v>
       </c>
       <c r="F69" s="26" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="G69" s="26"/>
       <c r="H69" s="26" t="s">
         <v>222</v>
       </c>
       <c r="I69" s="38" t="s">
-        <v>300</v>
+        <v>266</v>
       </c>
       <c r="J69" s="26" t="s">
         <v>26</v>
@@ -3958,7 +3967,7 @@
         <v>2035</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D70" s="26" t="s">
         <v>22</v>
@@ -3967,14 +3976,14 @@
         <v>138</v>
       </c>
       <c r="F70" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G70" s="26"/>
       <c r="H70" s="26" t="s">
         <v>222</v>
       </c>
       <c r="I70" s="38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J70" s="26" t="s">
         <v>26</v>
@@ -3991,7 +4000,7 @@
         <v>2035</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="D71" s="26" t="s">
         <v>22</v>
@@ -4000,16 +4009,14 @@
         <v>138</v>
       </c>
       <c r="F71" s="26" t="s">
-        <v>360</v>
-      </c>
-      <c r="G71" s="26" t="s">
-        <v>8</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="G71" s="26"/>
       <c r="H71" s="26" t="s">
         <v>222</v>
       </c>
       <c r="I71" s="38" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="J71" s="26" t="s">
         <v>26</v>
@@ -4026,7 +4033,7 @@
         <v>2035</v>
       </c>
       <c r="C72" s="26" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D72" s="26" t="s">
         <v>22</v>
@@ -4035,7 +4042,7 @@
         <v>138</v>
       </c>
       <c r="F72" s="26" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G72" s="26" t="s">
         <v>8</v>
@@ -4044,7 +4051,7 @@
         <v>222</v>
       </c>
       <c r="I72" s="38" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="J72" s="26" t="s">
         <v>26</v>
@@ -4061,7 +4068,7 @@
         <v>2035</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="D73" s="26" t="s">
         <v>22</v>
@@ -4070,16 +4077,16 @@
         <v>138</v>
       </c>
       <c r="F73" s="26" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G73" s="26" t="s">
         <v>8</v>
       </c>
       <c r="H73" s="26" t="s">
-        <v>341</v>
+        <v>222</v>
       </c>
       <c r="I73" s="38" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="J73" s="26" t="s">
         <v>26</v>
@@ -4096,7 +4103,7 @@
         <v>2035</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D74" s="26" t="s">
         <v>22</v>
@@ -4105,7 +4112,7 @@
         <v>138</v>
       </c>
       <c r="F74" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G74" s="26" t="s">
         <v>8</v>
@@ -4114,45 +4121,47 @@
         <v>341</v>
       </c>
       <c r="I74" s="38" t="s">
+        <v>342</v>
+      </c>
+      <c r="J74" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="K74" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" s="25">
+        <v>2035</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="D75" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F75" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="G75" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H75" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="I75" s="38" t="s">
         <v>343</v>
       </c>
-      <c r="J74" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="K74" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B75" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C75" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E75" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="G75" s="20"/>
-      <c r="H75" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J75" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K75" s="19" t="s">
+      <c r="J75" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="K75" s="25" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4164,7 +4173,7 @@
         <v>2035</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D76" s="20" t="s">
         <v>22</v>
@@ -4173,7 +4182,7 @@
         <v>143</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G76" s="20"/>
       <c r="H76" s="20" t="s">
@@ -4197,7 +4206,7 @@
         <v>2035</v>
       </c>
       <c r="C77" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>22</v>
@@ -4206,7 +4215,7 @@
         <v>143</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G77" s="20"/>
       <c r="H77" s="20" t="s">
@@ -4230,7 +4239,7 @@
         <v>2035</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>22</v>
@@ -4239,7 +4248,7 @@
         <v>143</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G78" s="20"/>
       <c r="H78" s="20" t="s">
@@ -4263,7 +4272,7 @@
         <v>2035</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>22</v>
@@ -4272,13 +4281,15 @@
         <v>143</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>364</v>
+        <v>171</v>
       </c>
       <c r="G79" s="20"/>
       <c r="H79" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="I79" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="J79" s="20" t="s">
         <v>26</v>
       </c>
@@ -4294,7 +4305,7 @@
         <v>2035</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="D80" s="20" t="s">
         <v>22</v>
@@ -4307,11 +4318,9 @@
       </c>
       <c r="G80" s="20"/>
       <c r="H80" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>187</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="I80" s="2"/>
       <c r="J80" s="20" t="s">
         <v>26</v>
       </c>
@@ -4327,7 +4336,7 @@
         <v>2035</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="D81" s="20" t="s">
         <v>22</v>
@@ -4336,14 +4345,14 @@
         <v>143</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>256</v>
+        <v>364</v>
       </c>
       <c r="G81" s="20"/>
       <c r="H81" s="20" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J81" s="20" t="s">
         <v>26</v>
@@ -4360,7 +4369,7 @@
         <v>2035</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="D82" s="20" t="s">
         <v>22</v>
@@ -4369,14 +4378,14 @@
         <v>143</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G82" s="20"/>
       <c r="H82" s="20" t="s">
         <v>200</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="J82" s="20" t="s">
         <v>26</v>
@@ -4393,7 +4402,7 @@
         <v>2035</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>283</v>
+        <v>236</v>
       </c>
       <c r="D83" s="20" t="s">
         <v>22</v>
@@ -4402,14 +4411,14 @@
         <v>143</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="G83" s="20"/>
       <c r="H83" s="20" t="s">
         <v>200</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="J83" s="20" t="s">
         <v>26</v>
@@ -4426,7 +4435,7 @@
         <v>2035</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="D84" s="20" t="s">
         <v>22</v>
@@ -4435,16 +4444,14 @@
         <v>143</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="G84" s="20" t="s">
-        <v>8</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="G84" s="20"/>
       <c r="H84" s="20" t="s">
         <v>200</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="J84" s="20" t="s">
         <v>26</v>
@@ -4461,7 +4468,7 @@
         <v>2035</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="D85" s="20" t="s">
         <v>22</v>
@@ -4470,52 +4477,56 @@
         <v>143</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>365</v>
+        <v>143</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>8</v>
       </c>
       <c r="H85" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="J85" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K85" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F86" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="G86" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H86" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I86" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="J85" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K85" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B86" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C86" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="D86" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="F86" s="23" t="s">
-        <v>366</v>
-      </c>
-      <c r="G86" s="23"/>
-      <c r="H86" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="I86" s="3"/>
-      <c r="J86" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K86" s="22" t="s">
+      <c r="J86" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K86" s="19" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4527,7 +4538,7 @@
         <v>2035</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="D87" s="23" t="s">
         <v>22</v>
@@ -4540,11 +4551,9 @@
       </c>
       <c r="G87" s="23"/>
       <c r="H87" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>184</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="I87" s="3"/>
       <c r="J87" s="23" t="s">
         <v>26</v>
       </c>
@@ -4560,7 +4569,7 @@
         <v>2035</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="D88" s="23" t="s">
         <v>22</v>
@@ -4569,14 +4578,14 @@
         <v>142</v>
       </c>
       <c r="F88" s="23" t="s">
-        <v>258</v>
+        <v>366</v>
       </c>
       <c r="G88" s="23"/>
       <c r="H88" s="23" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="J88" s="23" t="s">
         <v>26</v>
@@ -4593,7 +4602,7 @@
         <v>2035</v>
       </c>
       <c r="C89" s="23" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="D89" s="23" t="s">
         <v>22</v>
@@ -4602,14 +4611,14 @@
         <v>142</v>
       </c>
       <c r="F89" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G89" s="23"/>
       <c r="H89" s="23" t="s">
         <v>212</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="J89" s="23" t="s">
         <v>26</v>
@@ -4626,7 +4635,7 @@
         <v>2035</v>
       </c>
       <c r="C90" s="23" t="s">
-        <v>282</v>
+        <v>235</v>
       </c>
       <c r="D90" s="23" t="s">
         <v>22</v>
@@ -4635,14 +4644,14 @@
         <v>142</v>
       </c>
       <c r="F90" s="23" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="G90" s="23"/>
       <c r="H90" s="23" t="s">
         <v>212</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>279</v>
+        <v>237</v>
       </c>
       <c r="J90" s="23" t="s">
         <v>26</v>
@@ -4659,7 +4668,7 @@
         <v>2035</v>
       </c>
       <c r="C91" s="23" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="D91" s="23" t="s">
         <v>22</v>
@@ -4668,16 +4677,14 @@
         <v>142</v>
       </c>
       <c r="F91" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="G91" s="23" t="s">
-        <v>8</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="G91" s="23"/>
       <c r="H91" s="23" t="s">
         <v>212</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="J91" s="23" t="s">
         <v>26</v>
@@ -4694,7 +4701,7 @@
         <v>2035</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>347</v>
+        <v>306</v>
       </c>
       <c r="D92" s="23" t="s">
         <v>22</v>
@@ -4703,54 +4710,56 @@
         <v>142</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>367</v>
+        <v>142</v>
       </c>
       <c r="G92" s="23" t="s">
         <v>8</v>
       </c>
       <c r="H92" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="J92" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K92" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B93" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C93" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="D93" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F93" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="G93" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H93" s="23" t="s">
         <v>348</v>
       </c>
-      <c r="I92" s="3" t="s">
+      <c r="I93" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="J92" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K92" s="22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B93" s="6">
-        <v>2035</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="F93" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="I93" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J93" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K93" s="6" t="s">
+      <c r="J93" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K93" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4762,7 +4771,7 @@
         <v>2035</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>22</v>
@@ -4771,14 +4780,14 @@
         <v>176</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>260</v>
+        <v>368</v>
       </c>
       <c r="G94" s="7"/>
       <c r="H94" s="7" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="J94" s="7" t="s">
         <v>26</v>
@@ -4795,7 +4804,7 @@
         <v>2035</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>22</v>
@@ -4804,14 +4813,14 @@
         <v>176</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G95" s="7"/>
       <c r="H95" s="7" t="s">
         <v>215</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="J95" s="7" t="s">
         <v>26</v>
@@ -4828,7 +4837,7 @@
         <v>2035</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>273</v>
+        <v>231</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>22</v>
@@ -4837,14 +4846,14 @@
         <v>176</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="G96" s="7"/>
       <c r="H96" s="7" t="s">
         <v>215</v>
       </c>
       <c r="I96" s="4" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="J96" s="7" t="s">
         <v>26</v>
@@ -4861,7 +4870,7 @@
         <v>2035</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>22</v>
@@ -4870,16 +4879,14 @@
         <v>176</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G97" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="G97" s="7"/>
       <c r="H97" s="7" t="s">
         <v>215</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
       <c r="J97" s="7" t="s">
         <v>26</v>
@@ -4896,7 +4903,7 @@
         <v>2035</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>22</v>
@@ -4905,52 +4912,56 @@
         <v>176</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>369</v>
+        <v>177</v>
       </c>
       <c r="G98" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H98" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B99" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="I98" s="4" t="s">
+      <c r="I99" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="J98" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K98" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B99" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C99" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D99" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E99" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F99" s="30"/>
-      <c r="G99" s="30"/>
-      <c r="H99" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J99" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="K99" s="29" t="s">
+      <c r="J99" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K99" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4962,7 +4973,7 @@
         <v>2035</v>
       </c>
       <c r="C100" s="30" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D100" s="30" t="s">
         <v>22</v>
@@ -4970,15 +4981,13 @@
       <c r="E100" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F100" s="30" t="s">
-        <v>75</v>
-      </c>
+      <c r="F100" s="30"/>
       <c r="G100" s="30"/>
       <c r="H100" s="30" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="J100" s="30" t="s">
         <v>26</v>
@@ -4995,7 +5004,7 @@
         <v>2035</v>
       </c>
       <c r="C101" s="30" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D101" s="30" t="s">
         <v>22</v>
@@ -5003,13 +5012,15 @@
       <c r="E101" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F101" s="30"/>
+      <c r="F101" s="30" t="s">
+        <v>75</v>
+      </c>
       <c r="G101" s="30"/>
       <c r="H101" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I101" s="30" t="s">
-        <v>52</v>
+        <v>65</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="J101" s="30" t="s">
         <v>26</v>
@@ -5026,7 +5037,7 @@
         <v>2035</v>
       </c>
       <c r="C102" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D102" s="30" t="s">
         <v>22</v>
@@ -5037,7 +5048,7 @@
       <c r="F102" s="30"/>
       <c r="G102" s="30"/>
       <c r="H102" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I102" s="30" t="s">
         <v>52</v>
@@ -5057,7 +5068,7 @@
         <v>2035</v>
       </c>
       <c r="C103" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D103" s="30" t="s">
         <v>22</v>
@@ -5068,7 +5079,7 @@
       <c r="F103" s="30"/>
       <c r="G103" s="30"/>
       <c r="H103" s="30" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I103" s="30" t="s">
         <v>52</v>
@@ -5088,7 +5099,7 @@
         <v>2035</v>
       </c>
       <c r="C104" s="30" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D104" s="30" t="s">
         <v>22</v>
@@ -5096,53 +5107,51 @@
       <c r="E104" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F104" s="30" t="s">
-        <v>87</v>
-      </c>
+      <c r="F104" s="30"/>
       <c r="G104" s="30"/>
       <c r="H104" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="I104" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="J104" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="K104" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B105" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C105" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D105" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E105" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F105" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G105" s="30"/>
+      <c r="H105" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="I104" s="1" t="s">
+      <c r="I105" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J104" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="K104" s="29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A105" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B105" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C105" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D105" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E105" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="F105" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="G105" s="16"/>
-      <c r="H105" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="I105" t="s">
-        <v>28</v>
-      </c>
-      <c r="J105" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="K105" s="32" t="s">
+      <c r="J105" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="K105" s="29" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5154,7 +5163,7 @@
         <v>2035</v>
       </c>
       <c r="C106" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D106" s="31" t="s">
         <v>22</v>
@@ -5163,14 +5172,14 @@
         <v>29</v>
       </c>
       <c r="F106" s="33" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G106" s="16"/>
       <c r="H106" s="16" t="s">
         <v>36</v>
       </c>
       <c r="I106" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J106" s="31" t="s">
         <v>26</v>
@@ -5187,7 +5196,7 @@
         <v>2035</v>
       </c>
       <c r="C107" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D107" s="31" t="s">
         <v>22</v>
@@ -5196,14 +5205,14 @@
         <v>29</v>
       </c>
       <c r="F107" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G107" s="16"/>
       <c r="H107" s="16" t="s">
         <v>36</v>
       </c>
       <c r="I107" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J107" s="31" t="s">
         <v>26</v>
@@ -5220,7 +5229,7 @@
         <v>2035</v>
       </c>
       <c r="C108" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D108" s="31" t="s">
         <v>22</v>
@@ -5229,14 +5238,14 @@
         <v>29</v>
       </c>
       <c r="F108" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G108" s="16"/>
       <c r="H108" s="16" t="s">
         <v>36</v>
       </c>
       <c r="I108" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J108" s="31" t="s">
         <v>26</v>
@@ -5253,7 +5262,7 @@
         <v>2035</v>
       </c>
       <c r="C109" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D109" s="31" t="s">
         <v>22</v>
@@ -5262,14 +5271,14 @@
         <v>29</v>
       </c>
       <c r="F109" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G109" s="16"/>
       <c r="H109" s="16" t="s">
         <v>36</v>
       </c>
       <c r="I109" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J109" s="31" t="s">
         <v>26</v>
@@ -5286,7 +5295,7 @@
         <v>2035</v>
       </c>
       <c r="C110" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D110" s="31" t="s">
         <v>22</v>
@@ -5294,13 +5303,15 @@
       <c r="E110" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F110" s="33"/>
+      <c r="F110" s="33" t="s">
+        <v>81</v>
+      </c>
       <c r="G110" s="16"/>
       <c r="H110" s="16" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="I110" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="J110" s="31" t="s">
         <v>26</v>
@@ -5317,7 +5328,7 @@
         <v>2035</v>
       </c>
       <c r="C111" s="16" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="D111" s="31" t="s">
         <v>22</v>
@@ -5325,14 +5336,12 @@
       <c r="E111" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F111" s="33" t="s">
-        <v>84</v>
-      </c>
+      <c r="F111" s="33"/>
       <c r="G111" s="16"/>
       <c r="H111" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="I111" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="I111" t="s">
         <v>49</v>
       </c>
       <c r="J111" s="31" t="s">
@@ -5350,7 +5359,7 @@
         <v>2035</v>
       </c>
       <c r="C112" s="16" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="D112" s="31" t="s">
         <v>22</v>
@@ -5359,14 +5368,14 @@
         <v>29</v>
       </c>
       <c r="F112" s="33" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G112" s="16"/>
       <c r="H112" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="I112" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="I112" s="34" t="s">
+        <v>49</v>
       </c>
       <c r="J112" s="31" t="s">
         <v>26</v>
@@ -5383,7 +5392,7 @@
         <v>2035</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D113" s="31" t="s">
         <v>22</v>
@@ -5392,14 +5401,14 @@
         <v>29</v>
       </c>
       <c r="F113" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G113" s="16"/>
       <c r="H113" s="16" t="s">
         <v>36</v>
       </c>
       <c r="I113" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J113" s="31" t="s">
         <v>26</v>
@@ -5416,7 +5425,7 @@
         <v>2035</v>
       </c>
       <c r="C114" s="16" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D114" s="31" t="s">
         <v>22</v>
@@ -5424,10 +5433,12 @@
       <c r="E114" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F114" s="33"/>
+      <c r="F114" s="33" t="s">
+        <v>83</v>
+      </c>
       <c r="G114" s="16"/>
       <c r="H114" s="16" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="I114" t="s">
         <v>51</v>
@@ -5447,7 +5458,7 @@
         <v>2035</v>
       </c>
       <c r="C115" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D115" s="31" t="s">
         <v>22</v>
@@ -5478,7 +5489,7 @@
         <v>2035</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D116" s="31" t="s">
         <v>22</v>
@@ -5509,7 +5520,7 @@
         <v>2035</v>
       </c>
       <c r="C117" s="16" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D117" s="31" t="s">
         <v>22</v>
@@ -5517,15 +5528,13 @@
       <c r="E117" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F117" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F117" s="33"/>
       <c r="G117" s="16"/>
       <c r="H117" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I117" s="35" t="s">
-        <v>98</v>
+      <c r="I117" t="s">
+        <v>51</v>
       </c>
       <c r="J117" s="31" t="s">
         <v>26</v>
@@ -5542,7 +5551,7 @@
         <v>2035</v>
       </c>
       <c r="C118" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D118" s="31" t="s">
         <v>22</v>
@@ -5551,12 +5560,15 @@
         <v>29</v>
       </c>
       <c r="F118" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G118" s="16"/>
       <c r="H118" s="16" t="s">
         <v>67</v>
       </c>
+      <c r="I118" s="35" t="s">
+        <v>98</v>
+      </c>
       <c r="J118" s="31" t="s">
         <v>26</v>
       </c>
@@ -5572,7 +5584,7 @@
         <v>2035</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D119" s="31" t="s">
         <v>22</v>
@@ -5581,7 +5593,7 @@
         <v>29</v>
       </c>
       <c r="F119" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G119" s="16"/>
       <c r="H119" s="16" t="s">
@@ -5602,7 +5614,7 @@
         <v>2035</v>
       </c>
       <c r="C120" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D120" s="31" t="s">
         <v>22</v>
@@ -5611,7 +5623,7 @@
         <v>29</v>
       </c>
       <c r="F120" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G120" s="16"/>
       <c r="H120" s="16" t="s">
@@ -5624,36 +5636,33 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B121" s="6">
-        <v>2035</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E121" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F121" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G121" s="7"/>
-      <c r="H121" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I121" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J121" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K121" s="6" t="s">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B121" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C121" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D121" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E121" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F121" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J121" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="K121" s="32" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5665,7 +5674,7 @@
         <v>2035</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D122" s="7" t="s">
         <v>22</v>
@@ -5674,61 +5683,94 @@
         <v>100</v>
       </c>
       <c r="F122" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G122" s="7"/>
       <c r="H122" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I122" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J122" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K122" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B123" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G123" s="7"/>
+      <c r="H123" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I122" s="4" t="s">
+      <c r="I123" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J122" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K122" s="6" t="s">
+      <c r="J123" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K123" s="6" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K122" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K123" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I99" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
-    <hyperlink ref="I10" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
-    <hyperlink ref="I104" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
-    <hyperlink ref="I111" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
-    <hyperlink ref="I117" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
+    <hyperlink ref="I100" r:id="rId1" xr:uid="{1592469A-6192-4612-A267-6BA2A8A5332E}"/>
+    <hyperlink ref="I11" r:id="rId2" xr:uid="{80FF85B6-B74F-4630-8C50-DD7A861E052E}"/>
+    <hyperlink ref="I105" r:id="rId3" xr:uid="{30D26D8C-2A74-4237-8F78-E44E033C219F}"/>
+    <hyperlink ref="I112" r:id="rId4" xr:uid="{026875A0-06DC-485C-AF97-C17FD3560539}"/>
+    <hyperlink ref="I118" r:id="rId5" xr:uid="{4F17BDA8-8FC4-4405-8A40-E962F4688BAC}"/>
     <hyperlink ref="I7" r:id="rId6" xr:uid="{9E0A47EE-7266-4903-A851-FCDEA1D076D4}"/>
-    <hyperlink ref="I15" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
-    <hyperlink ref="I16" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
-    <hyperlink ref="I14" r:id="rId9" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{07D1B2DA-E517-4DD9-B4E8-AE0933FD4973}"/>
-    <hyperlink ref="I13" r:id="rId10" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{4A8E9582-524B-46F3-8A76-0C1F5220D214}"/>
-    <hyperlink ref="I12" r:id="rId11" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{E622471D-8EED-401F-9FFF-3C4854166AD2}"/>
-    <hyperlink ref="I34" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
-    <hyperlink ref="I35" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
-    <hyperlink ref="I36" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
-    <hyperlink ref="I37" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
-    <hyperlink ref="I93" r:id="rId16" xr:uid="{C5D42A4A-7D1E-4E61-A6D8-57E8258064CF}"/>
-    <hyperlink ref="I27" r:id="rId17" display="https://app.asana.com/0/1201809392759895/1204199508775563/f" xr:uid="{AD5B4BF6-019A-41E5-B4FF-144AB869AC79}"/>
-    <hyperlink ref="I39" r:id="rId18" display="https://app.asana.com/0/1201809392759895/1204199508775567/f" xr:uid="{4D75E071-693C-4E6B-9BC3-F13FF7899650}"/>
-    <hyperlink ref="I81" r:id="rId19" display="https://app.asana.com/0/1201809392759895/1204199508775554/f" xr:uid="{93FEBC25-3D8F-4C29-A30C-17379D746E6A}"/>
-    <hyperlink ref="I9" r:id="rId20" display="https://app.asana.com/0/0/1204199508775527/f" xr:uid="{F74BF0A2-72BF-4CE6-B53E-B781F9178384}"/>
-    <hyperlink ref="I88" r:id="rId21" display="https://app.asana.com/0/1201809392759895/1204199508775559/f" xr:uid="{22B796F7-F10B-406F-9671-D0DD2372085C}"/>
-    <hyperlink ref="I94" r:id="rId22" display="https://app.asana.com/0/1201809392759895/1204199508775550/f" xr:uid="{7477F2BA-CE56-4250-ACD2-6910E3E300C3}"/>
-    <hyperlink ref="I54" r:id="rId23" display="https://app.asana.com/0/1201809392759895/1203498380299819/f" xr:uid="{D93F0873-C671-4938-A6C2-30B74CB13B5B}"/>
-    <hyperlink ref="I65" r:id="rId24" display="https://app.asana.com/0/1201809392759895/1204220790822201/f" xr:uid="{1F3B0FA4-6BBC-474D-88B3-E82D1113FB80}"/>
-    <hyperlink ref="I28" r:id="rId25" display="https://app.asana.com/0/1201809392759895/1204295579502963/f" xr:uid="{7875DFD5-B0A2-459C-ABF9-F11D4ADD4F71}"/>
-    <hyperlink ref="I40" r:id="rId26" display="https://app.asana.com/0/1201809392759895/1204295579502969/f" xr:uid="{B63AFD9E-EB13-4B90-9FAB-319386521DF8}"/>
-    <hyperlink ref="I66" r:id="rId27" display="https://app.asana.com/0/1201809392759895/1204295579502978/f" xr:uid="{D43A960D-5A0B-4CBA-902D-69F4EB319BB3}"/>
-    <hyperlink ref="I95" r:id="rId28" display="https://app.asana.com/0/1201809392759895/1204286896724186/f" xr:uid="{E7EC1047-9DA4-4F9C-9B0E-D17FAE0F1E7C}"/>
-    <hyperlink ref="I55" r:id="rId29" display="https://app.asana.com/0/1201809392759895/1204295579502973/f" xr:uid="{F1F5C8FB-27AF-4015-BE70-7BAE285B89BD}"/>
-    <hyperlink ref="I89" r:id="rId30" display="https://app.asana.com/0/1201809392759895/1204295579502982/f" xr:uid="{9733EDE0-72F9-4C80-9C31-A649304EDFB2}"/>
-    <hyperlink ref="I82" r:id="rId31" display="https://app.asana.com/0/1201809392759895/1204295579502980/f" xr:uid="{96530962-B1F6-43FD-8386-80D23BCD0DC5}"/>
-    <hyperlink ref="I17" r:id="rId32" display="https://app.asana.com/0/1201809392759895/1204295579503110/f" xr:uid="{D535BCFB-415F-4CB0-9E44-1802BFB9227E}"/>
-    <hyperlink ref="I56" r:id="rId33" display="https://app.asana.com/0/1201809392759895/1204311438003508" xr:uid="{2C5CE002-FBD3-497B-96C2-D3AE6CF1127A}"/>
-    <hyperlink ref="I29" r:id="rId34" display="https://app.asana.com/0/1201809392759895/1204311438003500/f" xr:uid="{CCE9A3E3-3E67-4CD0-9AFB-C48B52AC84C0}"/>
-    <hyperlink ref="I41" r:id="rId35" display="https://app.asana.com/0/1201809392759895/1204311438003504/f" xr:uid="{1BF2101D-1E81-4B8C-973E-389A06EF5483}"/>
+    <hyperlink ref="I16" r:id="rId7" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{C316BADE-CE8A-410D-806D-41702DD2671E}"/>
+    <hyperlink ref="I17" r:id="rId8" display="https://app.asana.com/0/1203644633064654/1203877656488838/f" xr:uid="{CA1A1C19-C74D-4152-80C2-56A5ED7CA320}"/>
+    <hyperlink ref="I15" r:id="rId9" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{07D1B2DA-E517-4DD9-B4E8-AE0933FD4973}"/>
+    <hyperlink ref="I14" r:id="rId10" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{4A8E9582-524B-46F3-8A76-0C1F5220D214}"/>
+    <hyperlink ref="I13" r:id="rId11" display="https://app.asana.com/0/1201809392759895/1203877656488835/f" xr:uid="{E622471D-8EED-401F-9FFF-3C4854166AD2}"/>
+    <hyperlink ref="I35" r:id="rId12" display="https://app.asana.com/0/1201809392759895/1203877656488839/f" xr:uid="{0CFB59A4-5D4F-4072-A2BF-CFCF972DDB64}"/>
+    <hyperlink ref="I36" r:id="rId13" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{E29828B3-C096-4F2B-9C5F-ECAF8C622B0B}"/>
+    <hyperlink ref="I37" r:id="rId14" display="https://app.asana.com/0/1201809392759895/1203877656488840/f" xr:uid="{4ED3F112-A06E-4134-8BF7-D3E5E410C48B}"/>
+    <hyperlink ref="I38" r:id="rId15" display="https://app.asana.com/0/0/1203877656488841/f" xr:uid="{AB8B1EB1-BBCD-47E6-8630-0F9A3674F595}"/>
+    <hyperlink ref="I94" r:id="rId16" xr:uid="{C5D42A4A-7D1E-4E61-A6D8-57E8258064CF}"/>
+    <hyperlink ref="I28" r:id="rId17" display="https://app.asana.com/0/1201809392759895/1204199508775563/f" xr:uid="{AD5B4BF6-019A-41E5-B4FF-144AB869AC79}"/>
+    <hyperlink ref="I40" r:id="rId18" display="https://app.asana.com/0/1201809392759895/1204199508775567/f" xr:uid="{4D75E071-693C-4E6B-9BC3-F13FF7899650}"/>
+    <hyperlink ref="I82" r:id="rId19" display="https://app.asana.com/0/1201809392759895/1204199508775554/f" xr:uid="{93FEBC25-3D8F-4C29-A30C-17379D746E6A}"/>
+    <hyperlink ref="I10" r:id="rId20" display="https://app.asana.com/0/0/1204199508775527/f" xr:uid="{F74BF0A2-72BF-4CE6-B53E-B781F9178384}"/>
+    <hyperlink ref="I89" r:id="rId21" display="https://app.asana.com/0/1201809392759895/1204199508775559/f" xr:uid="{22B796F7-F10B-406F-9671-D0DD2372085C}"/>
+    <hyperlink ref="I95" r:id="rId22" display="https://app.asana.com/0/1201809392759895/1204199508775550/f" xr:uid="{7477F2BA-CE56-4250-ACD2-6910E3E300C3}"/>
+    <hyperlink ref="I55" r:id="rId23" display="https://app.asana.com/0/1201809392759895/1203498380299819/f" xr:uid="{D93F0873-C671-4938-A6C2-30B74CB13B5B}"/>
+    <hyperlink ref="I66" r:id="rId24" display="https://app.asana.com/0/1201809392759895/1204220790822201/f" xr:uid="{1F3B0FA4-6BBC-474D-88B3-E82D1113FB80}"/>
+    <hyperlink ref="I29" r:id="rId25" display="https://app.asana.com/0/1201809392759895/1204295579502963/f" xr:uid="{7875DFD5-B0A2-459C-ABF9-F11D4ADD4F71}"/>
+    <hyperlink ref="I41" r:id="rId26" display="https://app.asana.com/0/1201809392759895/1204295579502969/f" xr:uid="{B63AFD9E-EB13-4B90-9FAB-319386521DF8}"/>
+    <hyperlink ref="I67" r:id="rId27" display="https://app.asana.com/0/1201809392759895/1204295579502978/f" xr:uid="{D43A960D-5A0B-4CBA-902D-69F4EB319BB3}"/>
+    <hyperlink ref="I96" r:id="rId28" display="https://app.asana.com/0/1201809392759895/1204286896724186/f" xr:uid="{E7EC1047-9DA4-4F9C-9B0E-D17FAE0F1E7C}"/>
+    <hyperlink ref="I56" r:id="rId29" display="https://app.asana.com/0/1201809392759895/1204295579502973/f" xr:uid="{F1F5C8FB-27AF-4015-BE70-7BAE285B89BD}"/>
+    <hyperlink ref="I90" r:id="rId30" display="https://app.asana.com/0/1201809392759895/1204295579502982/f" xr:uid="{9733EDE0-72F9-4C80-9C31-A649304EDFB2}"/>
+    <hyperlink ref="I83" r:id="rId31" display="https://app.asana.com/0/1201809392759895/1204295579502980/f" xr:uid="{96530962-B1F6-43FD-8386-80D23BCD0DC5}"/>
+    <hyperlink ref="I18" r:id="rId32" display="https://app.asana.com/0/1201809392759895/1204295579503110/f" xr:uid="{D535BCFB-415F-4CB0-9E44-1802BFB9227E}"/>
+    <hyperlink ref="I57" r:id="rId33" display="https://app.asana.com/0/1201809392759895/1204311438003508" xr:uid="{2C5CE002-FBD3-497B-96C2-D3AE6CF1127A}"/>
+    <hyperlink ref="I30" r:id="rId34" display="https://app.asana.com/0/1201809392759895/1204311438003500/f" xr:uid="{CCE9A3E3-3E67-4CD0-9AFB-C48B52AC84C0}"/>
+    <hyperlink ref="I42" r:id="rId35" display="https://app.asana.com/0/1201809392759895/1204311438003504/f" xr:uid="{1BF2101D-1E81-4B8C-973E-389A06EF5483}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId36"/>

</xml_diff>

<commit_message>
Only keep NP02 runs
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4A1688-56E7-4FA5-8F1F-75A45D39CA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AD3E8D-740F-46AF-B18A-631AAE280E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="7065" windowWidth="21570" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="373">
   <si>
     <t>No Project</t>
   </si>
@@ -1706,23 +1706,23 @@
   <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" customWidth="1"/>
+    <col min="6" max="6" width="38.296875" customWidth="1"/>
+    <col min="8" max="8" width="47.3984375" customWidth="1"/>
+    <col min="10" max="10" width="43.69921875" customWidth="1"/>
     <col min="11" max="11" width="15" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>39</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>39</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>39</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>39</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>39</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>39</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>39</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>39</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>39</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>39</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>39</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>39</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>39</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>39</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>39</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>39</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>39</v>
       </c>
@@ -2656,9 +2656,7 @@
       <c r="F30" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="G30" s="7"/>
       <c r="H30" s="7" t="s">
         <v>226</v>
       </c>
@@ -2672,7 +2670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>39</v>
       </c>
@@ -2691,9 +2689,7 @@
       <c r="F31" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
         <v>226</v>
       </c>
@@ -2707,7 +2703,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>39</v>
       </c>
@@ -2740,7 +2736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
@@ -2759,9 +2755,7 @@
       <c r="F33" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
         <v>226</v>
       </c>
@@ -2775,7 +2769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>39</v>
       </c>
@@ -2810,7 +2804,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>39</v>
       </c>
@@ -2841,7 +2835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>39</v>
       </c>
@@ -2872,7 +2866,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>39</v>
       </c>
@@ -2903,7 +2897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>39</v>
       </c>
@@ -2936,7 +2930,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
         <v>39</v>
       </c>
@@ -2967,7 +2961,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>39</v>
       </c>
@@ -3000,7 +2994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
         <v>39</v>
       </c>
@@ -3033,7 +3027,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="21" t="s">
         <v>39</v>
       </c>
@@ -3052,9 +3046,7 @@
       <c r="F42" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="G42" s="23" t="s">
-        <v>8</v>
-      </c>
+      <c r="G42" s="23"/>
       <c r="H42" s="23" t="s">
         <v>198</v>
       </c>
@@ -3068,7 +3060,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
         <v>39</v>
       </c>
@@ -3087,9 +3079,7 @@
       <c r="F43" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="G43" s="23" t="s">
-        <v>8</v>
-      </c>
+      <c r="G43" s="23"/>
       <c r="H43" s="23" t="s">
         <v>198</v>
       </c>
@@ -3103,7 +3093,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="21" t="s">
         <v>39</v>
       </c>
@@ -3134,7 +3124,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>39</v>
       </c>
@@ -3165,7 +3155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
         <v>39</v>
       </c>
@@ -3196,7 +3186,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>39</v>
       </c>
@@ -3227,7 +3217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="21" t="s">
         <v>39</v>
       </c>
@@ -3260,7 +3250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
         <v>39</v>
       </c>
@@ -3293,7 +3283,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
         <v>39</v>
       </c>
@@ -3324,7 +3314,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
         <v>39</v>
       </c>
@@ -3355,7 +3345,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
         <v>39</v>
       </c>
@@ -3388,7 +3378,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
         <v>39</v>
       </c>
@@ -3407,9 +3397,7 @@
       <c r="F53" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="G53" s="23" t="s">
-        <v>8</v>
-      </c>
+      <c r="G53" s="23"/>
       <c r="H53" s="23" t="s">
         <v>189</v>
       </c>
@@ -3423,7 +3411,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21" t="s">
         <v>39</v>
       </c>
@@ -3458,7 +3446,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>39</v>
       </c>
@@ -3491,7 +3479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>39</v>
       </c>
@@ -3524,7 +3512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>39</v>
       </c>
@@ -3557,7 +3545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>39</v>
       </c>
@@ -3590,7 +3578,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>39</v>
       </c>
@@ -3623,7 +3611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>39</v>
       </c>
@@ -3656,7 +3644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>39</v>
       </c>
@@ -3675,9 +3663,7 @@
       <c r="F61" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="G61" s="13" t="s">
-        <v>8</v>
-      </c>
+      <c r="G61" s="13"/>
       <c r="H61" s="13" t="s">
         <v>219</v>
       </c>
@@ -3691,7 +3677,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>39</v>
       </c>
@@ -3710,9 +3696,7 @@
       <c r="F62" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="G62" s="13" t="s">
-        <v>8</v>
-      </c>
+      <c r="G62" s="13"/>
       <c r="H62" s="13" t="s">
         <v>219</v>
       </c>
@@ -3726,7 +3710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>39</v>
       </c>
@@ -3761,7 +3745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
         <v>39</v>
       </c>
@@ -3796,7 +3780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="24" t="s">
         <v>39</v>
       </c>
@@ -3827,7 +3811,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
         <v>39</v>
       </c>
@@ -3860,7 +3844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="24" t="s">
         <v>39</v>
       </c>
@@ -3893,7 +3877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="24" t="s">
         <v>39</v>
       </c>
@@ -3926,7 +3910,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="24" t="s">
         <v>39</v>
       </c>
@@ -3959,7 +3943,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="24" t="s">
         <v>39</v>
       </c>
@@ -3992,7 +3976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="24" t="s">
         <v>39</v>
       </c>
@@ -4025,7 +4009,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
         <v>39</v>
       </c>
@@ -4044,9 +4028,7 @@
       <c r="F72" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="G72" s="26" t="s">
-        <v>8</v>
-      </c>
+      <c r="G72" s="26"/>
       <c r="H72" s="26" t="s">
         <v>222</v>
       </c>
@@ -4060,7 +4042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="24" t="s">
         <v>39</v>
       </c>
@@ -4079,9 +4061,7 @@
       <c r="F73" s="26" t="s">
         <v>361</v>
       </c>
-      <c r="G73" s="26" t="s">
-        <v>8</v>
-      </c>
+      <c r="G73" s="26"/>
       <c r="H73" s="26" t="s">
         <v>222</v>
       </c>
@@ -4095,7 +4075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="24" t="s">
         <v>39</v>
       </c>
@@ -4130,7 +4110,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="24" t="s">
         <v>39</v>
       </c>
@@ -4165,7 +4145,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="18" t="s">
         <v>39</v>
       </c>
@@ -4198,7 +4178,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="18" t="s">
         <v>39</v>
       </c>
@@ -4231,7 +4211,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18" t="s">
         <v>39</v>
       </c>
@@ -4264,7 +4244,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18" t="s">
         <v>39</v>
       </c>
@@ -4297,7 +4277,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18" t="s">
         <v>39</v>
       </c>
@@ -4328,7 +4308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="18" t="s">
         <v>39</v>
       </c>
@@ -4361,7 +4341,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="18" t="s">
         <v>39</v>
       </c>
@@ -4394,7 +4374,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="18" t="s">
         <v>39</v>
       </c>
@@ -4427,7 +4407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="18" t="s">
         <v>39</v>
       </c>
@@ -4460,7 +4440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="18" t="s">
         <v>39</v>
       </c>
@@ -4479,9 +4459,7 @@
       <c r="F85" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="G85" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="G85" s="20"/>
       <c r="H85" s="20" t="s">
         <v>200</v>
       </c>
@@ -4495,7 +4473,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="18" t="s">
         <v>39</v>
       </c>
@@ -4530,7 +4508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="21" t="s">
         <v>39</v>
       </c>
@@ -4561,7 +4539,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="21" t="s">
         <v>39</v>
       </c>
@@ -4594,7 +4572,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="21" t="s">
         <v>39</v>
       </c>
@@ -4627,7 +4605,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="21" t="s">
         <v>39</v>
       </c>
@@ -4660,7 +4638,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="21" t="s">
         <v>39</v>
       </c>
@@ -4693,7 +4671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="21" t="s">
         <v>39</v>
       </c>
@@ -4712,9 +4690,7 @@
       <c r="F92" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="G92" s="23" t="s">
-        <v>8</v>
-      </c>
+      <c r="G92" s="23"/>
       <c r="H92" s="23" t="s">
         <v>212</v>
       </c>
@@ -4728,7 +4704,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="21" t="s">
         <v>39</v>
       </c>
@@ -4763,7 +4739,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>39</v>
       </c>
@@ -4796,7 +4772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>39</v>
       </c>
@@ -4829,7 +4805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>39</v>
       </c>
@@ -4862,7 +4838,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>39</v>
       </c>
@@ -4895,7 +4871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>39</v>
       </c>
@@ -4914,9 +4890,7 @@
       <c r="F98" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G98" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="G98" s="7"/>
       <c r="H98" s="7" t="s">
         <v>215</v>
       </c>
@@ -4930,7 +4904,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>39</v>
       </c>
@@ -4965,7 +4939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="28" t="s">
         <v>39</v>
       </c>
@@ -4996,7 +4970,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="28" t="s">
         <v>39</v>
       </c>
@@ -5029,7 +5003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="28" t="s">
         <v>39</v>
       </c>
@@ -5060,7 +5034,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="28" t="s">
         <v>39</v>
       </c>
@@ -5091,7 +5065,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="28" t="s">
         <v>39</v>
       </c>
@@ -5122,7 +5096,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="28" t="s">
         <v>39</v>
       </c>
@@ -5155,7 +5129,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="31" t="s">
         <v>39</v>
       </c>
@@ -5188,7 +5162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="31" t="s">
         <v>39</v>
       </c>
@@ -5221,7 +5195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="31" t="s">
         <v>39</v>
       </c>
@@ -5254,7 +5228,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="31" t="s">
         <v>39</v>
       </c>
@@ -5287,7 +5261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="31" t="s">
         <v>39</v>
       </c>
@@ -5320,7 +5294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="31" t="s">
         <v>39</v>
       </c>
@@ -5351,7 +5325,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="31" t="s">
         <v>39</v>
       </c>
@@ -5384,7 +5358,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="31" t="s">
         <v>39</v>
       </c>
@@ -5417,7 +5391,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="31" t="s">
         <v>39</v>
       </c>
@@ -5450,7 +5424,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="31" t="s">
         <v>39</v>
       </c>
@@ -5481,7 +5455,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="31" t="s">
         <v>39</v>
       </c>
@@ -5512,7 +5486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="31" t="s">
         <v>39</v>
       </c>
@@ -5543,7 +5517,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="31" t="s">
         <v>39</v>
       </c>
@@ -5576,7 +5550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="31" t="s">
         <v>39</v>
       </c>
@@ -5606,7 +5580,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="31" t="s">
         <v>39</v>
       </c>
@@ -5636,7 +5610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="31" t="s">
         <v>39</v>
       </c>
@@ -5666,7 +5640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="122" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>39</v>
       </c>
@@ -5699,7 +5673,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Make short names clear because of pathway renumbering
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns.xlsx
+++ b/utilities/NextGenFwys/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AD3E8D-740F-46AF-B18A-631AAE280E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3250AF90-ED9B-4BE7-808D-EBD8C86338C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="2265" windowWidth="28185" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="372">
   <si>
     <t>No Project</t>
   </si>
@@ -1100,54 +1100,27 @@
     <t>directory</t>
   </si>
   <si>
-    <t>Pathway 1a (more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 1b (more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
     <t>Pathway 2a with 20pct art toll</t>
   </si>
   <si>
     <t>Pathway 2a with 10pct art toll</t>
   </si>
   <si>
-    <t>Pathway 2a with 20pct art toll (more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 2a with 10pct art toll (more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
     <t>Pathway 2b with 20pct art toll</t>
   </si>
   <si>
     <t>Pathway 2b with 10pct art toll</t>
   </si>
   <si>
-    <t>Pathway 2b with 20pct art toll (more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
-    <t>Pathway 2b with 10pct art toll (more VZ, less trn, lower toll)</t>
-  </si>
-  <si>
     <t>Pathway 3a (NP07)</t>
   </si>
   <si>
-    <t>Pathway 3a (more VZ, less trn)</t>
-  </si>
-  <si>
     <t>Pathway 3b (NP07)</t>
   </si>
   <si>
-    <t>Pathway 3b (more VZ, less trn)</t>
-  </si>
-  <si>
     <t>Pathway 4 - No New Pricing (NP07)</t>
   </si>
   <si>
-    <t>Pathway 4 - No New Pricing (more VZ, less trn)</t>
-  </si>
-  <si>
     <t>2015_TM152_NGF_06</t>
   </si>
   <si>
@@ -1155,6 +1128,30 @@
   </si>
   <si>
     <t>https://app.asana.com/0/0/1204222536302922/f</t>
+  </si>
+  <si>
+    <t>Pathway 1a - All Lane Tolling + Transit Double Down</t>
+  </si>
+  <si>
+    <t>Pathway 1b - All Lane Tolling + Affordable</t>
+  </si>
+  <si>
+    <t>Pathway 2a  All Lane &amp; 10% Arterial Tolling + Transit Double Down</t>
+  </si>
+  <si>
+    <t>Pathway 2a - All Lane &amp; 20% Arterial Tolling + Transit Double Down</t>
+  </si>
+  <si>
+    <t>Pathway 2b - All Lane &amp; 20% Arterial Tolling + Affordable</t>
+  </si>
+  <si>
+    <t>Pathway 2b - All Lane &amp; 10% Arterial Tolling + Affordable</t>
+  </si>
+  <si>
+    <t>Pathway 3a - Cordon Tolling + Transit Double Down</t>
+  </si>
+  <si>
+    <t>Pathway 3b - Cordon Tolling + Affordable</t>
   </si>
 </sst>
 </file>
@@ -1706,23 +1703,23 @@
   <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="13.09765625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="38.296875" customWidth="1"/>
-    <col min="8" max="8" width="47.3984375" customWidth="1"/>
-    <col min="10" max="10" width="43.69921875" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" customWidth="1"/>
     <col min="11" max="11" width="15" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -1757,7 +1754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -1785,7 +1782,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>39</v>
       </c>
@@ -1816,7 +1813,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>39</v>
       </c>
@@ -1847,7 +1844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>39</v>
       </c>
@@ -1878,7 +1875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
@@ -1911,7 +1908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
@@ -1946,7 +1943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>39</v>
       </c>
@@ -1954,7 +1951,7 @@
         <v>2015</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>22</v>
@@ -1963,14 +1960,14 @@
         <v>93</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="s">
         <v>55</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>13</v>
@@ -1979,7 +1976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -2009,7 +2006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
@@ -2042,7 +2039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>39</v>
       </c>
@@ -2073,7 +2070,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>39</v>
       </c>
@@ -2106,7 +2103,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>39</v>
       </c>
@@ -2137,7 +2134,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>39</v>
       </c>
@@ -2170,7 +2167,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>39</v>
       </c>
@@ -2203,7 +2200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>39</v>
       </c>
@@ -2236,7 +2233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>39</v>
       </c>
@@ -2269,7 +2266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>39</v>
       </c>
@@ -2302,7 +2299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>39</v>
       </c>
@@ -2335,7 +2332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>39</v>
       </c>
@@ -2370,7 +2367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
@@ -2399,7 +2396,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
@@ -2428,7 +2425,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>39</v>
       </c>
@@ -2457,7 +2454,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
@@ -2486,7 +2483,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
@@ -2515,7 +2512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
@@ -2544,7 +2541,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>39</v>
       </c>
@@ -2573,7 +2570,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>39</v>
       </c>
@@ -2604,7 +2601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>39</v>
       </c>
@@ -2637,7 +2634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>39</v>
       </c>
@@ -2670,7 +2667,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>39</v>
       </c>
@@ -2703,7 +2700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>39</v>
       </c>
@@ -2736,7 +2733,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
@@ -2769,7 +2766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>39</v>
       </c>
@@ -2786,7 +2783,7 @@
         <v>141</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>8</v>
@@ -2804,7 +2801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>39</v>
       </c>
@@ -2835,7 +2832,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>39</v>
       </c>
@@ -2866,7 +2863,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>39</v>
       </c>
@@ -2897,7 +2894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>39</v>
       </c>
@@ -2930,7 +2927,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>39</v>
       </c>
@@ -2961,7 +2958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
         <v>39</v>
       </c>
@@ -2994,7 +2991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
         <v>39</v>
       </c>
@@ -3027,7 +3024,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
         <v>39</v>
       </c>
@@ -3060,7 +3057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>39</v>
       </c>
@@ -3093,7 +3090,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
         <v>39</v>
       </c>
@@ -3124,7 +3121,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
         <v>39</v>
       </c>
@@ -3155,7 +3152,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
         <v>39</v>
       </c>
@@ -3186,7 +3183,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>39</v>
       </c>
@@ -3217,7 +3214,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
         <v>39</v>
       </c>
@@ -3250,7 +3247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>39</v>
       </c>
@@ -3283,7 +3280,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
         <v>39</v>
       </c>
@@ -3314,7 +3311,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
         <v>39</v>
       </c>
@@ -3345,7 +3342,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
         <v>39</v>
       </c>
@@ -3378,7 +3375,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
         <v>39</v>
       </c>
@@ -3411,7 +3408,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
         <v>39</v>
       </c>
@@ -3428,7 +3425,7 @@
         <v>137</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="G54" s="23" t="s">
         <v>8</v>
@@ -3446,7 +3443,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>39</v>
       </c>
@@ -3479,7 +3476,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>39</v>
       </c>
@@ -3512,7 +3509,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>39</v>
       </c>
@@ -3545,7 +3542,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>39</v>
       </c>
@@ -3578,7 +3575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>39</v>
       </c>
@@ -3611,7 +3608,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>39</v>
       </c>
@@ -3644,7 +3641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>39</v>
       </c>
@@ -3661,7 +3658,7 @@
         <v>218</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G61" s="13"/>
       <c r="H61" s="13" t="s">
@@ -3677,7 +3674,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>39</v>
       </c>
@@ -3694,7 +3691,7 @@
         <v>218</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G62" s="13"/>
       <c r="H62" s="13" t="s">
@@ -3710,7 +3707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
         <v>39</v>
       </c>
@@ -3727,7 +3724,7 @@
         <v>218</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>8</v>
@@ -3745,7 +3742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>39</v>
       </c>
@@ -3762,7 +3759,7 @@
         <v>218</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>8</v>
@@ -3780,7 +3777,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="24" t="s">
         <v>39</v>
       </c>
@@ -3811,7 +3808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="24" t="s">
         <v>39</v>
       </c>
@@ -3844,7 +3841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="24" t="s">
         <v>39</v>
       </c>
@@ -3877,7 +3874,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="24" t="s">
         <v>39</v>
       </c>
@@ -3910,7 +3907,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="24" t="s">
         <v>39</v>
       </c>
@@ -3943,7 +3940,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="24" t="s">
         <v>39</v>
       </c>
@@ -3976,7 +3973,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="24" t="s">
         <v>39</v>
       </c>
@@ -4009,7 +4006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
         <v>39</v>
       </c>
@@ -4026,7 +4023,7 @@
         <v>138</v>
       </c>
       <c r="F72" s="26" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G72" s="26"/>
       <c r="H72" s="26" t="s">
@@ -4042,7 +4039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
         <v>39</v>
       </c>
@@ -4059,7 +4056,7 @@
         <v>138</v>
       </c>
       <c r="F73" s="26" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G73" s="26"/>
       <c r="H73" s="26" t="s">
@@ -4075,7 +4072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
         <v>39</v>
       </c>
@@ -4092,7 +4089,7 @@
         <v>138</v>
       </c>
       <c r="F74" s="26" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="G74" s="26" t="s">
         <v>8</v>
@@ -4110,7 +4107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="24" t="s">
         <v>39</v>
       </c>
@@ -4127,7 +4124,7 @@
         <v>138</v>
       </c>
       <c r="F75" s="26" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="G75" s="26" t="s">
         <v>8</v>
@@ -4145,7 +4142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
         <v>39</v>
       </c>
@@ -4178,7 +4175,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
         <v>39</v>
       </c>
@@ -4211,7 +4208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="18" t="s">
         <v>39</v>
       </c>
@@ -4244,7 +4241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="18" t="s">
         <v>39</v>
       </c>
@@ -4277,7 +4274,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="18" t="s">
         <v>39</v>
       </c>
@@ -4294,7 +4291,7 @@
         <v>143</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G80" s="20"/>
       <c r="H80" s="20" t="s">
@@ -4308,7 +4305,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="18" t="s">
         <v>39</v>
       </c>
@@ -4325,7 +4322,7 @@
         <v>143</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G81" s="20"/>
       <c r="H81" s="20" t="s">
@@ -4341,7 +4338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="18" t="s">
         <v>39</v>
       </c>
@@ -4374,7 +4371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="18" t="s">
         <v>39</v>
       </c>
@@ -4407,7 +4404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="18" t="s">
         <v>39</v>
       </c>
@@ -4440,7 +4437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
         <v>39</v>
       </c>
@@ -4473,7 +4470,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="18" t="s">
         <v>39</v>
       </c>
@@ -4490,7 +4487,7 @@
         <v>143</v>
       </c>
       <c r="F86" s="20" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="G86" s="20" t="s">
         <v>8</v>
@@ -4508,7 +4505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
         <v>39</v>
       </c>
@@ -4525,7 +4522,7 @@
         <v>142</v>
       </c>
       <c r="F87" s="23" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="G87" s="23"/>
       <c r="H87" s="23" t="s">
@@ -4539,7 +4536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="21" t="s">
         <v>39</v>
       </c>
@@ -4556,7 +4553,7 @@
         <v>142</v>
       </c>
       <c r="F88" s="23" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="G88" s="23"/>
       <c r="H88" s="23" t="s">
@@ -4572,7 +4569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="21" t="s">
         <v>39</v>
       </c>
@@ -4605,7 +4602,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="21" t="s">
         <v>39</v>
       </c>
@@ -4638,7 +4635,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="21" t="s">
         <v>39</v>
       </c>
@@ -4671,7 +4668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="21" t="s">
         <v>39</v>
       </c>
@@ -4704,7 +4701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="21" t="s">
         <v>39</v>
       </c>
@@ -4721,7 +4718,7 @@
         <v>142</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="G93" s="23" t="s">
         <v>8</v>
@@ -4739,7 +4736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>39</v>
       </c>
@@ -4756,7 +4753,7 @@
         <v>176</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="G94" s="7"/>
       <c r="H94" s="7" t="s">
@@ -4772,7 +4769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>39</v>
       </c>
@@ -4805,7 +4802,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>39</v>
       </c>
@@ -4838,7 +4835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>39</v>
       </c>
@@ -4871,7 +4868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>39</v>
       </c>
@@ -4904,7 +4901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>39</v>
       </c>
@@ -4921,7 +4918,7 @@
         <v>176</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>369</v>
+        <v>177</v>
       </c>
       <c r="G99" s="7" t="s">
         <v>8</v>
@@ -4939,7 +4936,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="28" t="s">
         <v>39</v>
       </c>
@@ -4970,7 +4967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="28" t="s">
         <v>39</v>
       </c>
@@ -5003,7 +5000,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="28" t="s">
         <v>39</v>
       </c>
@@ -5034,7 +5031,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="28" t="s">
         <v>39</v>
       </c>
@@ -5065,7 +5062,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="28" t="s">
         <v>39</v>
       </c>
@@ -5096,7 +5093,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="28" t="s">
         <v>39</v>
       </c>
@@ -5129,7 +5126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="31" t="s">
         <v>39</v>
       </c>
@@ -5162,7 +5159,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="31" t="s">
         <v>39</v>
       </c>
@@ -5195,7 +5192,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="31" t="s">
         <v>39</v>
       </c>
@@ -5228,7 +5225,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="31" t="s">
         <v>39</v>
       </c>
@@ -5261,7 +5258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="31" t="s">
         <v>39</v>
       </c>
@@ -5294,7 +5291,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="31" t="s">
         <v>39</v>
       </c>
@@ -5325,7 +5322,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="31" t="s">
         <v>39</v>
       </c>
@@ -5358,7 +5355,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="31" t="s">
         <v>39</v>
       </c>
@@ -5391,7 +5388,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="31" t="s">
         <v>39</v>
       </c>
@@ -5424,7 +5421,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="31" t="s">
         <v>39</v>
       </c>
@@ -5455,7 +5452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="31" t="s">
         <v>39</v>
       </c>
@@ -5486,7 +5483,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="31" t="s">
         <v>39</v>
       </c>
@@ -5517,7 +5514,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="31" t="s">
         <v>39</v>
       </c>
@@ -5550,7 +5547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="31" t="s">
         <v>39</v>
       </c>
@@ -5580,7 +5577,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="31" t="s">
         <v>39</v>
       </c>
@@ -5610,7 +5607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="31" t="s">
         <v>39</v>
       </c>
@@ -5640,7 +5637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="122" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>39</v>
       </c>
@@ -5673,7 +5670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>39</v>
       </c>

</xml_diff>